<commit_message>
Actualizando cronograma del Proyecto
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carloss\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carloss\Desktop\Cursos 2020\GESTION DE CONFIGURACION Y MANTENIMIENTO-G1\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="117">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>Realizar acta de conformidad</t>
+  </si>
+  <si>
+    <t>Unocc Sihuinta, Roberto Carlos</t>
   </si>
 </sst>
 </file>
@@ -748,6 +751,9 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -759,9 +765,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1334,7 +1337,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -1344,12 +1347,116 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
                 <a:srgbClr val="FFC000"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="20"/>
+            <c:idx val="25"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="26"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1359,7 +1466,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="21"/>
+            <c:idx val="29"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1369,7 +1476,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="22"/>
+            <c:idx val="30"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1379,17 +1486,46 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="23"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="24"/>
+            <c:idx val="31"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="32"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="33"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="34"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1399,7 +1535,46 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="25"/>
+            <c:idx val="35"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="36"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="37"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="38"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1409,7 +1584,33 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="26"/>
+            <c:idx val="39"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="40"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="41"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1419,7 +1620,33 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="27"/>
+            <c:idx val="42"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="43"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="44"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1429,7 +1656,59 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="28"/>
+            <c:idx val="45"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="46"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="47"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="48"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="49"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1439,177 +1718,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="29"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="30"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="31"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="32"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="33"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="34"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="35"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="36"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="37"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="38"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="39"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="40"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="41"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="42"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="43"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="44"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="45"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="46"/>
+            <c:idx val="50"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1839,7 +1948,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>7</c:v>
@@ -1854,13 +1963,13 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>7</c:v>
@@ -1933,11 +2042,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-708009392"/>
-        <c:axId val="-709652656"/>
+        <c:axId val="1743524864"/>
+        <c:axId val="1939330944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-708009392"/>
+        <c:axId val="1743524864"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1947,7 +2056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-709652656"/>
+        <c:crossAx val="1939330944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1955,7 +2064,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-709652656"/>
+        <c:axId val="1939330944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44078"/>
@@ -1968,10 +2077,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-708009392"/>
+        <c:crossAx val="1743524864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
+        <c:majorUnit val="15"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -2345,8 +2454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="C36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2363,43 +2472,43 @@
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
     </row>
     <row r="3" spans="1:9" ht="18.75">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="52"/>
+      <c r="C3" s="53"/>
     </row>
     <row r="4" spans="1:9" ht="18.75">
       <c r="A4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="53"/>
     </row>
     <row r="5" spans="1:9" ht="18.75">
       <c r="A5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="53"/>
+      <c r="C5" s="54"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="14"/>
@@ -2769,9 +2878,7 @@
       <c r="A27" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="22" t="s">
-        <v>76</v>
-      </c>
+      <c r="B27" s="22"/>
       <c r="C27" s="23">
         <v>44024</v>
       </c>
@@ -2787,14 +2894,14 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
     </row>
     <row r="29" spans="1:6" s="39" customFormat="1" ht="30.75" customHeight="1">
       <c r="A29" s="38" t="s">
@@ -2826,11 +2933,11 @@
         <v>44029</v>
       </c>
       <c r="D30" s="41">
-        <v>44043</v>
+        <v>44050</v>
       </c>
       <c r="E30" s="40">
         <f t="shared" ref="E30" si="8">D30-C30</f>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F30" s="42" t="s">
         <v>10</v>
@@ -2841,7 +2948,7 @@
         <v>50</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="C31" s="41">
         <v>44029</v>
@@ -2861,8 +2968,8 @@
       <c r="A32" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="22" t="s">
-        <v>76</v>
+      <c r="B32" s="40" t="s">
+        <v>116</v>
       </c>
       <c r="C32" s="23">
         <v>44029</v>
@@ -2882,8 +2989,8 @@
       <c r="A33" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="22" t="s">
-        <v>75</v>
+      <c r="B33" s="40" t="s">
+        <v>116</v>
       </c>
       <c r="C33" s="23">
         <v>44036</v>
@@ -2939,11 +3046,11 @@
         <v>44029</v>
       </c>
       <c r="D36" s="41">
-        <v>44043</v>
+        <v>44050</v>
       </c>
       <c r="E36" s="40">
         <f>D36-C36</f>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F36" s="42" t="s">
         <v>10</v>
@@ -2980,26 +3087,26 @@
       <c r="C38" s="23">
         <v>44032</v>
       </c>
-      <c r="D38" s="23">
-        <v>44043</v>
+      <c r="D38" s="41">
+        <v>44050</v>
       </c>
       <c r="E38" s="22">
         <f>D38-C38</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F38" s="27" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A39" s="50" t="s">
+      <c r="A39" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
     </row>
     <row r="40" spans="1:6" ht="44.25" customHeight="1">
       <c r="A40" s="16" t="s">
@@ -3111,7 +3218,7 @@
       <c r="B45" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="54">
+      <c r="C45" s="50">
         <v>44058</v>
       </c>
       <c r="D45" s="41">
@@ -3399,14 +3506,14 @@
       </c>
     </row>
     <row r="59" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A59" s="50" t="s">
+      <c r="A59" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="51"/>
     </row>
     <row r="64" spans="1:17" s="44" customFormat="1" ht="15.75" customHeight="1">
       <c r="D64" s="45"/>

</xml_diff>

<commit_message>
Actualizando los Requisitos funcionales 001 y 002
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -1381,7 +1381,17 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="22"/>
+            <c:idx val="23"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1394,7 +1404,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="23"/>
+            <c:idx val="25"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1407,17 +1417,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="24"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="25"/>
+            <c:idx val="26"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1430,7 +1430,37 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="26"/>
+            <c:idx val="27"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="29"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="30"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1443,7 +1473,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="27"/>
+            <c:idx val="31"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1456,37 +1486,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="28"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="29"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="30"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="31"/>
+            <c:idx val="32"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1499,7 +1499,17 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="32"/>
+            <c:idx val="33"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="34"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1512,7 +1522,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="33"/>
+            <c:idx val="35"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1525,17 +1535,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="34"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="35"/>
+            <c:idx val="36"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1548,7 +1548,17 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="36"/>
+            <c:idx val="37"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="38"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1561,7 +1571,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="37"/>
+            <c:idx val="39"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1574,7 +1584,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="38"/>
+            <c:idx val="40"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1584,7 +1594,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="39"/>
+            <c:idx val="41"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1597,7 +1607,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="40"/>
+            <c:idx val="42"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1610,7 +1620,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="41"/>
+            <c:idx val="43"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1620,7 +1630,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="42"/>
+            <c:idx val="44"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1633,7 +1643,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="43"/>
+            <c:idx val="45"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1646,17 +1656,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="44"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="45"/>
+            <c:idx val="46"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1669,7 +1669,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="46"/>
+            <c:idx val="47"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1682,7 +1682,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="47"/>
+            <c:idx val="48"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1695,7 +1695,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="48"/>
+            <c:idx val="49"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1708,7 +1708,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="49"/>
+            <c:idx val="50"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1718,7 +1718,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="50"/>
+            <c:idx val="51"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -2042,11 +2042,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1743524864"/>
-        <c:axId val="1939330944"/>
+        <c:axId val="369586000"/>
+        <c:axId val="369592528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1743524864"/>
+        <c:axId val="369586000"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2056,7 +2056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1939330944"/>
+        <c:crossAx val="369592528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2064,7 +2064,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1939330944"/>
+        <c:axId val="369592528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44078"/>
@@ -2077,7 +2077,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1743524864"/>
+        <c:crossAx val="369586000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
@@ -2454,8 +2454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Actualizando el cronograma del Proyecto
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -795,10 +795,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -834,7 +834,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1131,13 +1133,13 @@
                   <c:v>44066</c:v>
                 </c:pt>
                 <c:pt idx="42">
+                  <c:v>44066</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>44067</c:v>
                 </c:pt>
-                <c:pt idx="43">
-                  <c:v>44069</c:v>
-                </c:pt>
                 <c:pt idx="44">
-                  <c:v>44069</c:v>
+                  <c:v>44067</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>44070</c:v>
@@ -1160,572 +1162,265 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="23"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="26"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="27"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="28"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="29"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="30"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="31"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="32"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="33"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="34"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="35"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="36"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="37"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="38"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="39"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="40"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="41"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="42"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="43"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="44"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="45"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="46"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="47"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="48"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="49"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="50"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="51"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="52"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2011,19 +1706,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>1</c:v>
@@ -2042,21 +1737,54 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="369586000"/>
-        <c:axId val="369592528"/>
+        <c:axId val="-1741585184"/>
+        <c:axId val="-1741584096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="369586000"/>
+        <c:axId val="-1741585184"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="369592528"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1741584096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2064,7 +1792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="369592528"/>
+        <c:axId val="-1741584096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44078"/>
@@ -2072,27 +1800,644 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="369586000"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1741585184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2454,8 +2799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2611,8 +2956,8 @@
       <c r="A14" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>78</v>
+      <c r="B14" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="C14" s="23">
         <v>44002</v>
@@ -2651,8 +2996,8 @@
       <c r="A16" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>78</v>
+      <c r="B16" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="C16" s="23">
         <v>44008</v>
@@ -2756,8 +3101,8 @@
       <c r="A21" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>78</v>
+      <c r="B21" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="C21" s="23">
         <v>44018</v>
@@ -2927,7 +3272,7 @@
         <v>101</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="C30" s="41">
         <v>44029</v>
@@ -3040,7 +3385,7 @@
         <v>102</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C36" s="41">
         <v>44029</v>
@@ -3060,8 +3405,8 @@
       <c r="A37" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="22" t="s">
-        <v>43</v>
+      <c r="B37" s="40" t="s">
+        <v>76</v>
       </c>
       <c r="C37" s="23">
         <v>44029</v>
@@ -3390,11 +3735,11 @@
         <v>44066</v>
       </c>
       <c r="D53" s="41">
-        <v>44069</v>
+        <v>44067</v>
       </c>
       <c r="E53" s="22">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F53" s="26" t="s">
         <v>10</v>
@@ -3429,14 +3774,14 @@
         <v>77</v>
       </c>
       <c r="C55" s="41">
+        <v>44066</v>
+      </c>
+      <c r="D55" s="41">
         <v>44067</v>
-      </c>
-      <c r="D55" s="41">
-        <v>44069</v>
       </c>
       <c r="E55" s="40">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" s="42" t="s">
         <v>10</v>
@@ -3450,14 +3795,14 @@
         <v>43</v>
       </c>
       <c r="C56" s="41">
-        <v>44069</v>
+        <v>44067</v>
       </c>
       <c r="D56" s="41">
         <v>44071</v>
       </c>
       <c r="E56" s="22">
         <f>D56-C56</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F56" s="26" t="s">
         <v>10</v>
@@ -3471,14 +3816,14 @@
         <v>43</v>
       </c>
       <c r="C57" s="41">
-        <v>44069</v>
+        <v>44067</v>
       </c>
       <c r="D57" s="41">
         <v>44070</v>
       </c>
       <c r="E57" s="40">
         <f t="shared" ref="E57" si="16">D57-C57</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F57" s="42" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Añadiendo porcentaje de avance al Cronograma
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alumno\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alumno\Documents\GitHub\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -447,7 +447,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +481,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,7 +542,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -657,6 +663,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1168,11 +1175,6 @@
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:dPt>
-            <c:idx val="31"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-          </c:dPt>
-          <c:dPt>
             <c:idx val="32"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
@@ -1309,6 +1311,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="59"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="60"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -1627,11 +1634,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1300278640"/>
-        <c:axId val="-1300285168"/>
+        <c:axId val="856315504"/>
+        <c:axId val="856311152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1300278640"/>
+        <c:axId val="856315504"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1674,7 +1681,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300285168"/>
+        <c:crossAx val="856311152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1682,7 +1689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1300285168"/>
+        <c:axId val="856311152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44078"/>
@@ -1735,7 +1742,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1300278640"/>
+        <c:crossAx val="856315504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
@@ -2689,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2825,6 +2832,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="46">
+        <f>AVERAGE(G13:G14)</f>
         <v>1</v>
       </c>
     </row>
@@ -2895,7 +2903,8 @@
         <v>8</v>
       </c>
       <c r="G15" s="46">
-        <v>0.8</v>
+        <f>AVERAGE(G16:G22)</f>
+        <v>0.7857142857142857</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="29.25" customHeight="1">
@@ -3085,6 +3094,7 @@
         <v>9</v>
       </c>
       <c r="G23" s="46">
+        <f>AVERAGE(G24:G27)</f>
         <v>0</v>
       </c>
     </row>
@@ -3210,6 +3220,7 @@
         <v>9</v>
       </c>
       <c r="G29" s="46">
+        <f>AVERAGE(G30,G36)</f>
         <v>0</v>
       </c>
     </row>
@@ -3234,6 +3245,7 @@
         <v>9</v>
       </c>
       <c r="G30" s="47">
+        <f>AVERAGE(G31:G35)</f>
         <v>0</v>
       </c>
     </row>
@@ -3365,6 +3377,7 @@
         <v>9</v>
       </c>
       <c r="G36" s="47">
+        <f>AVERAGE(G37:G38,G40:G41)</f>
         <v>0</v>
       </c>
     </row>
@@ -3494,6 +3507,7 @@
         <v>9</v>
       </c>
       <c r="G42" s="46">
+        <f>AVERAGE(G46,G50,G53)</f>
         <v>0</v>
       </c>
     </row>
@@ -3590,6 +3604,7 @@
         <v>9</v>
       </c>
       <c r="G46" s="47">
+        <f>AVERAGE(G47:G49)</f>
         <v>0</v>
       </c>
     </row>
@@ -3686,6 +3701,7 @@
         <v>9</v>
       </c>
       <c r="G50" s="47">
+        <f>AVERAGE(G51:G52)</f>
         <v>0</v>
       </c>
     </row>
@@ -3757,7 +3773,8 @@
       <c r="F53" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G53" s="45">
+      <c r="G53" s="47">
+        <f>AVERAGE(G54:G55)</f>
         <v>0</v>
       </c>
     </row>
@@ -3781,7 +3798,7 @@
       <c r="F54" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="G54" s="47">
+      <c r="G54" s="52">
         <v>0</v>
       </c>
     </row>
@@ -3830,6 +3847,7 @@
         <v>9</v>
       </c>
       <c r="G56" s="46">
+        <f>AVERAGE(G57:G58)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizando fecha del cronograma
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="89">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -250,9 +250,6 @@
     <t>Diseño de la base de datos.</t>
   </si>
   <si>
-    <t>Diseño de la arquitectura del sistema.</t>
-  </si>
-  <si>
     <t>Planificación</t>
   </si>
   <si>
@@ -320,6 +317,9 @@
   </si>
   <si>
     <t>Porcentaje de Avance</t>
+  </si>
+  <si>
+    <t>Documento de la arquitectura del sistema.</t>
   </si>
 </sst>
 </file>
@@ -783,7 +783,7 @@
                   <c:v>Estimación de costos</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Diseño de la arquitectura del sistema.</c:v>
+                  <c:v>Documento de la arquitectura del sistema.</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Planificar la gestión de calidad</c:v>
@@ -946,13 +946,13 @@
                   <c:v>44022</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44022</c:v>
+                  <c:v>44021</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44022</c:v>
+                  <c:v>44021</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44023</c:v>
+                  <c:v>44021</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>44024</c:v>
@@ -1175,11 +1175,6 @@
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:dPt>
-            <c:idx val="33"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-          </c:dPt>
-          <c:dPt>
             <c:idx val="34"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
@@ -1316,6 +1311,11 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="61"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="62"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -1362,7 +1362,7 @@
                   <c:v>Estimación de costos</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Diseño de la arquitectura del sistema.</c:v>
+                  <c:v>Documento de la arquitectura del sistema.</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Planificar la gestión de calidad</c:v>
@@ -1525,13 +1525,13 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>5</c:v>
@@ -1634,11 +1634,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="735931008"/>
-        <c:axId val="919027984"/>
+        <c:axId val="-642952912"/>
+        <c:axId val="-460415744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="735931008"/>
+        <c:axId val="-642952912"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1681,7 +1681,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="919027984"/>
+        <c:crossAx val="-460415744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1689,7 +1689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="919027984"/>
+        <c:axId val="-460415744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44078"/>
@@ -1742,7 +1742,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="735931008"/>
+        <c:crossAx val="-642952912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
@@ -2696,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2781,7 +2781,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="5">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -2810,7 +2810,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.75" customHeight="1">
@@ -2886,7 +2886,7 @@
     </row>
     <row r="15" spans="1:9" ht="26.25" customHeight="1">
       <c r="A15" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="19">
@@ -2957,7 +2957,7 @@
     </row>
     <row r="18" spans="1:7" ht="28.5" customHeight="1">
       <c r="A18" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>55</v>
@@ -2981,7 +2981,7 @@
     </row>
     <row r="19" spans="1:7" ht="24" customHeight="1">
       <c r="A19" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>55</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="21" spans="1:7" ht="25.5" customHeight="1">
       <c r="A21" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="33" t="s">
         <v>23</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="22" spans="1:7" ht="25.5" customHeight="1">
       <c r="A22" s="27" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>57</v>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="23" spans="1:7" s="32" customFormat="1" ht="25.5" customHeight="1">
       <c r="A23" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>58</v>
@@ -3104,44 +3104,46 @@
         <v>63</v>
       </c>
       <c r="B24" s="18"/>
-      <c r="C24" s="19">
-        <v>44022</v>
+      <c r="C24" s="34">
+        <v>44021</v>
       </c>
       <c r="D24" s="19">
         <v>44029</v>
       </c>
       <c r="E24" s="18">
         <f t="shared" ref="E24" si="5">D24-C24</f>
-        <v>7</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="G24" s="46">
         <f>AVERAGE(G25:G27)</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="22.5" customHeight="1">
       <c r="A25" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19">
-        <v>44022</v>
+      <c r="B25" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="34">
+        <v>44021</v>
       </c>
       <c r="D25" s="19">
-        <v>44025</v>
+        <v>44024</v>
       </c>
       <c r="E25" s="18">
         <f t="shared" ref="E25" si="6">D25-C25</f>
         <v>3</v>
       </c>
-      <c r="F25" s="22" t="s">
-        <v>9</v>
+      <c r="F25" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="G25" s="45">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30.75" customHeight="1">
@@ -3151,28 +3153,30 @@
       <c r="B26" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="19">
-        <v>44023</v>
-      </c>
-      <c r="D26" s="19">
-        <v>44027</v>
+      <c r="C26" s="34">
+        <v>44021</v>
+      </c>
+      <c r="D26" s="34">
+        <v>44022</v>
       </c>
       <c r="E26" s="18">
         <f>D26-C26</f>
-        <v>4</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>10</v>
       </c>
       <c r="G26" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30.75" customHeight="1">
       <c r="A27" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="33" t="s">
+        <v>57</v>
+      </c>
       <c r="C27" s="19">
         <v>44024</v>
       </c>
@@ -3203,7 +3207,7 @@
     </row>
     <row r="29" spans="1:7" s="32" customFormat="1" ht="30.75" customHeight="1">
       <c r="A29" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="34">
@@ -3226,10 +3230,10 @@
     </row>
     <row r="30" spans="1:7" s="32" customFormat="1" ht="27" customHeight="1">
       <c r="A30" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="34">
         <v>44029</v>
@@ -3254,7 +3258,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="34">
         <v>44029</v>
@@ -3278,7 +3282,7 @@
         <v>33</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="19">
         <v>44029</v>
@@ -3302,7 +3306,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" s="19">
         <v>44036</v>
@@ -3358,7 +3362,7 @@
     </row>
     <row r="36" spans="1:7" s="32" customFormat="1" ht="33.75" customHeight="1">
       <c r="A36" s="41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="33" t="s">
         <v>56</v>
@@ -3513,7 +3517,7 @@
     </row>
     <row r="43" spans="1:7" s="32" customFormat="1" ht="25.5" customHeight="1">
       <c r="A43" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B43" s="33" t="s">
         <v>55</v>
@@ -3537,7 +3541,7 @@
     </row>
     <row r="44" spans="1:7" s="32" customFormat="1" ht="24.75" customHeight="1">
       <c r="A44" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="33" t="s">
         <v>55</v>
@@ -3561,7 +3565,7 @@
     </row>
     <row r="45" spans="1:7" s="32" customFormat="1" ht="20.25" customHeight="1">
       <c r="A45" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45" s="33" t="s">
         <v>55</v>
@@ -3585,7 +3589,7 @@
     </row>
     <row r="46" spans="1:7" s="32" customFormat="1" ht="24.75" customHeight="1">
       <c r="A46" s="42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B46" s="33" t="s">
         <v>55</v>
@@ -3610,7 +3614,7 @@
     </row>
     <row r="47" spans="1:7" s="32" customFormat="1" ht="21.75" customHeight="1">
       <c r="A47" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B47" s="33" t="s">
         <v>55</v>
@@ -3634,7 +3638,7 @@
     </row>
     <row r="48" spans="1:7" s="32" customFormat="1" ht="18.75" customHeight="1">
       <c r="A48" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="33" t="s">
         <v>55</v>
@@ -3658,7 +3662,7 @@
     </row>
     <row r="49" spans="1:17" s="32" customFormat="1" ht="21.75" customHeight="1">
       <c r="A49" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B49" s="33" t="s">
         <v>55</v>
@@ -3707,7 +3711,7 @@
     </row>
     <row r="51" spans="1:17" s="32" customFormat="1" ht="18.75" customHeight="1">
       <c r="A51" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" s="33" t="s">
         <v>58</v>
@@ -3731,7 +3735,7 @@
     </row>
     <row r="52" spans="1:17" s="32" customFormat="1" ht="20.25" customHeight="1">
       <c r="A52" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B52" s="33" t="s">
         <v>58</v>
@@ -3755,7 +3759,7 @@
     </row>
     <row r="53" spans="1:17" ht="22.5" customHeight="1">
       <c r="A53" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>57</v>
@@ -3780,7 +3784,7 @@
     </row>
     <row r="54" spans="1:17" s="32" customFormat="1" ht="25.5" customHeight="1">
       <c r="A54" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B54" s="33" t="s">
         <v>57</v>
@@ -3853,7 +3857,7 @@
     </row>
     <row r="57" spans="1:17" s="32" customFormat="1" ht="25.5" customHeight="1">
       <c r="A57" s="36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B57" s="33" t="s">
         <v>23</v>
@@ -3877,7 +3881,7 @@
     </row>
     <row r="58" spans="1:17" ht="25.5" customHeight="1">
       <c r="A58" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B58" s="33" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Actualizacion Cronograma - Front
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -326,7 +326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;S/&quot;\ #,##0.00;[Red]&quot;S/&quot;\ \-#,##0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -411,14 +411,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -532,7 +524,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -577,11 +569,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -614,7 +603,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1272,7 +1261,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="36"/>
+            <c:idx val="37"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1282,7 +1271,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="37"/>
+            <c:idx val="38"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1292,7 +1281,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="38"/>
+            <c:idx val="39"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1302,7 +1291,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="39"/>
+            <c:idx val="40"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1312,7 +1301,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="40"/>
+            <c:idx val="41"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1322,7 +1311,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="41"/>
+            <c:idx val="42"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1332,7 +1321,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="42"/>
+            <c:idx val="43"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1342,7 +1331,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="43"/>
+            <c:idx val="44"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1352,7 +1341,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="44"/>
+            <c:idx val="45"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1362,7 +1351,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="45"/>
+            <c:idx val="46"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1372,7 +1361,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="46"/>
+            <c:idx val="47"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1382,7 +1371,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="47"/>
+            <c:idx val="48"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1392,7 +1381,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="48"/>
+            <c:idx val="49"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1402,7 +1391,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="49"/>
+            <c:idx val="50"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1412,7 +1401,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="50"/>
+            <c:idx val="51"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1422,7 +1411,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="51"/>
+            <c:idx val="52"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1432,7 +1421,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="52"/>
+            <c:idx val="53"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1442,7 +1431,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="53"/>
+            <c:idx val="54"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1452,7 +1441,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="54"/>
+            <c:idx val="55"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1462,7 +1451,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="55"/>
+            <c:idx val="56"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1472,7 +1461,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="56"/>
+            <c:idx val="57"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1482,7 +1471,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="57"/>
+            <c:idx val="58"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1492,7 +1481,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="58"/>
+            <c:idx val="59"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1502,7 +1491,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="59"/>
+            <c:idx val="60"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1512,7 +1501,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="60"/>
+            <c:idx val="61"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1522,7 +1511,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="61"/>
+            <c:idx val="62"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1532,7 +1521,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="62"/>
+            <c:idx val="63"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1542,7 +1531,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="63"/>
+            <c:idx val="64"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -1552,7 +1541,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="64"/>
+            <c:idx val="65"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:extLst>
@@ -2943,8 +2932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2962,43 +2951,43 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
     </row>
     <row r="3" spans="1:9" ht="18.75">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="50"/>
+      <c r="C3" s="49"/>
     </row>
     <row r="4" spans="1:9" ht="18.75">
       <c r="A4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="50"/>
+      <c r="C4" s="49"/>
     </row>
     <row r="5" spans="1:9" ht="18.75">
       <c r="A5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="51"/>
+      <c r="C5" s="50"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="10"/>
@@ -3056,12 +3045,12 @@
       <c r="F11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="42" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="18"/>
@@ -3078,13 +3067,13 @@
       <c r="F12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="45">
+      <c r="G12" s="44">
         <f>AVERAGE(G13:G14)</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="23.25" customHeight="1">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>60</v>
       </c>
       <c r="B13" s="18" t="s">
@@ -3103,15 +3092,15 @@
       <c r="F13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="19">
@@ -3127,12 +3116,12 @@
       <c r="F14" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="44">
+      <c r="G14" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="18"/>
@@ -3149,22 +3138,22 @@
       <c r="F15" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="45">
+      <c r="G15" s="44">
         <f>AVERAGE(G16:G23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="19">
         <v>44008</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="32">
         <v>44013</v>
       </c>
       <c r="E16" s="18">
@@ -3174,12 +3163,12 @@
       <c r="F16" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="44">
+      <c r="G16" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="27" customHeight="1">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="18" t="s">
@@ -3188,7 +3177,7 @@
       <c r="C17" s="19">
         <v>44008</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="32">
         <v>44013</v>
       </c>
       <c r="E17" s="18">
@@ -3198,12 +3187,12 @@
       <c r="F17" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="44">
+      <c r="G17" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="25" t="s">
         <v>65</v>
       </c>
       <c r="B18" s="18" t="s">
@@ -3212,7 +3201,7 @@
       <c r="C18" s="19">
         <v>44010</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="32">
         <v>44013</v>
       </c>
       <c r="E18" s="18">
@@ -3222,12 +3211,12 @@
       <c r="F18" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="44">
+      <c r="G18" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="24" customHeight="1">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="25" t="s">
         <v>66</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3236,7 +3225,7 @@
       <c r="C19" s="19">
         <v>44012</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="32">
         <v>44013</v>
       </c>
       <c r="E19" s="18">
@@ -3246,21 +3235,21 @@
       <c r="F19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="44">
+      <c r="G19" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="22.5" customHeight="1">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="32">
         <v>44010</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="32">
         <v>44013</v>
       </c>
       <c r="E20" s="18">
@@ -3270,15 +3259,15 @@
       <c r="F20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="44">
+      <c r="G20" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="19">
@@ -3294,21 +3283,21 @@
       <c r="F21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="44">
+      <c r="G21" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="25" t="s">
         <v>86</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="33">
+      <c r="C22" s="32">
         <v>44019</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="32">
         <v>44022</v>
       </c>
       <c r="E22" s="18">
@@ -3318,12 +3307,12 @@
       <c r="F22" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="44">
+      <c r="G22" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="31" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A23" s="28" t="s">
+    <row r="23" spans="1:7" s="30" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A23" s="27" t="s">
         <v>87</v>
       </c>
       <c r="B23" s="18" t="s">
@@ -3342,16 +3331,16 @@
       <c r="F23" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="44">
+      <c r="G23" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="22.5" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="18"/>
-      <c r="C24" s="33">
+      <c r="C24" s="32">
         <v>44021</v>
       </c>
       <c r="D24" s="19">
@@ -3364,19 +3353,19 @@
       <c r="F24" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="45">
+      <c r="G24" s="44">
         <f>AVERAGE(G25:G27)</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="22.5" customHeight="1">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C25" s="32">
         <v>44021</v>
       </c>
       <c r="D25" s="19">
@@ -3389,21 +3378,21 @@
       <c r="F25" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="44">
+      <c r="G25" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30.75" customHeight="1">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="25" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C26" s="32">
         <v>44021</v>
       </c>
-      <c r="D26" s="33">
+      <c r="D26" s="32">
         <v>44022</v>
       </c>
       <c r="E26" s="18">
@@ -3413,15 +3402,15 @@
       <c r="F26" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="44">
+      <c r="G26" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30.75" customHeight="1">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="31" t="s">
         <v>56</v>
       </c>
       <c r="C27" s="19">
@@ -3437,98 +3426,98 @@
       <c r="F27" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="44">
+      <c r="G27" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30.75" customHeight="1">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="44"/>
-    </row>
-    <row r="29" spans="1:7" s="31" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A29" s="30" t="s">
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="43"/>
+    </row>
+    <row r="29" spans="1:7" s="30" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A29" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="33">
+      <c r="B29" s="31"/>
+      <c r="C29" s="32">
         <v>44029</v>
       </c>
-      <c r="D29" s="33">
+      <c r="D29" s="32">
         <v>44050</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="31">
         <f t="shared" ref="E29" si="7">D29-C29</f>
         <v>21</v>
       </c>
-      <c r="F29" s="34" t="s">
+      <c r="F29" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="45">
+      <c r="G29" s="44">
         <f>AVERAGE(G30,G36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="31" customFormat="1" ht="27" customHeight="1">
-      <c r="A30" s="39" t="s">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="30" customFormat="1" ht="27" customHeight="1">
+      <c r="A30" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="33">
+      <c r="C30" s="32">
         <v>44029</v>
       </c>
-      <c r="D30" s="33">
+      <c r="D30" s="32">
         <v>44050</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="31">
         <f t="shared" ref="E30" si="8">D30-C30</f>
         <v>21</v>
       </c>
-      <c r="F30" s="34" t="s">
+      <c r="F30" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="46">
+      <c r="G30" s="45">
         <f>AVERAGE(G31:G35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="33">
+      <c r="C31" s="32">
         <v>44029</v>
       </c>
-      <c r="D31" s="33">
+      <c r="D31" s="32">
         <v>44036</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="31">
         <f t="shared" ref="E31" si="9">D31-C31</f>
         <v>7</v>
       </c>
-      <c r="F31" s="34" t="s">
+      <c r="F31" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="44">
+      <c r="G31" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="31" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A32" s="29" t="s">
+    <row r="32" spans="1:7" s="30" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A32" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="31" t="s">
         <v>84</v>
       </c>
       <c r="C32" s="19">
@@ -3544,15 +3533,15 @@
       <c r="F32" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="44">
+      <c r="G32" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="31" customFormat="1" ht="33" customHeight="1">
-      <c r="A33" s="26" t="s">
+    <row r="33" spans="1:7" s="30" customFormat="1" ht="33" customHeight="1">
+      <c r="A33" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="31" t="s">
         <v>84</v>
       </c>
       <c r="C33" s="19">
@@ -3568,81 +3557,81 @@
       <c r="F33" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="44">
+      <c r="G33" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="31" customFormat="1" ht="2.25" hidden="1" customHeight="1">
-      <c r="A34" s="26"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="44">
+    <row r="34" spans="1:7" s="30" customFormat="1" ht="2.25" hidden="1" customHeight="1">
+      <c r="A34" s="25"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="31" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A35" s="26" t="s">
+    <row r="35" spans="1:7" s="30" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A35" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="33">
+      <c r="C35" s="32">
         <v>44039</v>
       </c>
-      <c r="D35" s="33">
+      <c r="D35" s="32">
         <v>44050</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="31">
         <f>D35-C35</f>
         <v>11</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="F35" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="44">
+      <c r="G35" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="31" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A36" s="40" t="s">
+    <row r="36" spans="1:7" s="30" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A36" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="33">
+      <c r="C36" s="32">
         <v>44029</v>
       </c>
-      <c r="D36" s="33">
+      <c r="D36" s="32">
         <v>44050</v>
       </c>
-      <c r="E36" s="32">
+      <c r="E36" s="31">
         <f>D36-C36</f>
         <v>21</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="F36" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="46">
+      <c r="G36" s="45">
         <f>AVERAGE(G37:G38,G40:G41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="31" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A37" s="26" t="s">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="30" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A37" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="31" t="s">
         <v>55</v>
       </c>
       <c r="C37" s="19">
         <v>44029</v>
       </c>
-      <c r="D37" s="33">
+      <c r="D37" s="32">
         <v>44050</v>
       </c>
       <c r="E37" s="18">
@@ -3652,12 +3641,12 @@
       <c r="F37" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="44">
+      <c r="G37" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="31" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A38" s="29" t="s">
+    <row r="38" spans="1:7" s="30" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A38" s="28" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="18" t="s">
@@ -3666,52 +3655,52 @@
       <c r="C38" s="19">
         <v>44032</v>
       </c>
-      <c r="D38" s="33">
+      <c r="D38" s="32">
         <v>44050</v>
       </c>
       <c r="E38" s="18">
         <f>D38-C38</f>
         <v>18</v>
       </c>
-      <c r="F38" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="44">
-        <v>0</v>
+      <c r="F38" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="43">
+        <v>0.4</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="22.5" customHeight="1">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="44"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="43"/>
     </row>
     <row r="40" spans="1:7" ht="44.25" customHeight="1">
       <c r="A40" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="33">
+      <c r="C40" s="32">
         <v>44043</v>
       </c>
-      <c r="D40" s="33">
+      <c r="D40" s="32">
         <v>44050</v>
       </c>
-      <c r="E40" s="32">
+      <c r="E40" s="31">
         <f t="shared" ref="E40:E41" si="10">D40-C40</f>
         <v>7</v>
       </c>
-      <c r="F40" s="34" t="s">
+      <c r="F40" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="44">
+      <c r="G40" s="43">
         <v>0</v>
       </c>
     </row>
@@ -3719,35 +3708,35 @@
       <c r="A41" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="33">
+      <c r="C41" s="32">
         <v>44050</v>
       </c>
-      <c r="D41" s="33">
+      <c r="D41" s="32">
         <v>44057</v>
       </c>
-      <c r="E41" s="32">
+      <c r="E41" s="31">
         <f t="shared" si="10"/>
         <v>7</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="F41" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="44">
+      <c r="G41" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="24" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="18"/>
       <c r="C42" s="19">
         <v>44057</v>
       </c>
-      <c r="D42" s="33">
+      <c r="D42" s="32">
         <v>44060</v>
       </c>
       <c r="E42" s="18">
@@ -3757,188 +3746,188 @@
       <c r="F42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="45">
+      <c r="G42" s="44">
         <f>AVERAGE(G46,G50,G53)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="31" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A43" s="26" t="s">
+    <row r="43" spans="1:7" s="30" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A43" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="33">
+      <c r="C43" s="32">
         <v>44057</v>
       </c>
-      <c r="D43" s="33">
+      <c r="D43" s="32">
         <v>44058</v>
       </c>
-      <c r="E43" s="32">
+      <c r="E43" s="31">
         <f t="shared" ref="E43:E49" si="12">D43-C43</f>
         <v>1</v>
       </c>
-      <c r="F43" s="34" t="s">
+      <c r="F43" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="44">
+      <c r="G43" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="31" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A44" s="26" t="s">
+    <row r="44" spans="1:7" s="30" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A44" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="33">
+      <c r="C44" s="32">
         <v>44057</v>
       </c>
-      <c r="D44" s="33">
+      <c r="D44" s="32">
         <v>44058</v>
       </c>
-      <c r="E44" s="32">
+      <c r="E44" s="31">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="F44" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G44" s="44">
+      <c r="G44" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="31" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A45" s="26" t="s">
+    <row r="45" spans="1:7" s="30" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A45" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="42">
+      <c r="C45" s="41">
         <v>44058</v>
       </c>
-      <c r="D45" s="33">
+      <c r="D45" s="32">
         <v>44060</v>
       </c>
-      <c r="E45" s="32">
+      <c r="E45" s="31">
         <f t="shared" si="12"/>
         <v>2</v>
       </c>
-      <c r="F45" s="34" t="s">
+      <c r="F45" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G45" s="44">
+      <c r="G45" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="31" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A46" s="41" t="s">
+    <row r="46" spans="1:7" s="30" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A46" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="33">
+      <c r="C46" s="32">
         <v>44060</v>
       </c>
-      <c r="D46" s="33">
+      <c r="D46" s="32">
         <v>44064</v>
       </c>
-      <c r="E46" s="32">
+      <c r="E46" s="31">
         <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="F46" s="34" t="s">
+      <c r="F46" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G46" s="46">
+      <c r="G46" s="45">
         <f>AVERAGE(G47:G49)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="31" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" s="26" t="s">
+    <row r="47" spans="1:7" s="30" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A47" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="33">
+      <c r="C47" s="32">
         <v>44060</v>
       </c>
-      <c r="D47" s="33">
+      <c r="D47" s="32">
         <v>44061</v>
       </c>
-      <c r="E47" s="32">
+      <c r="E47" s="31">
         <f t="shared" ref="E47:E48" si="13">D47-C47</f>
         <v>1</v>
       </c>
-      <c r="F47" s="34" t="s">
+      <c r="F47" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G47" s="44">
+      <c r="G47" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="31" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A48" s="26" t="s">
+    <row r="48" spans="1:7" s="30" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A48" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="32" t="s">
+      <c r="B48" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="33">
+      <c r="C48" s="32">
         <v>44060</v>
       </c>
-      <c r="D48" s="33">
+      <c r="D48" s="32">
         <v>44062</v>
       </c>
-      <c r="E48" s="32">
+      <c r="E48" s="31">
         <f t="shared" si="13"/>
         <v>2</v>
       </c>
-      <c r="F48" s="34" t="s">
+      <c r="F48" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="44">
+      <c r="G48" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="31" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A49" s="26" t="s">
+    <row r="49" spans="1:17" s="30" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A49" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="33">
+      <c r="C49" s="32">
         <v>44060</v>
       </c>
-      <c r="D49" s="33">
+      <c r="D49" s="32">
         <v>44064</v>
       </c>
-      <c r="E49" s="32">
+      <c r="E49" s="31">
         <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="F49" s="34" t="s">
+      <c r="F49" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G49" s="44">
+      <c r="G49" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="24" customHeight="1">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="40" t="s">
         <v>38</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="33">
+      <c r="C50" s="32">
         <v>44064</v>
       </c>
       <c r="D50" s="19">
@@ -3951,70 +3940,70 @@
       <c r="F50" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G50" s="46">
+      <c r="G50" s="45">
         <f>AVERAGE(G51:G52)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="31" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A51" s="26" t="s">
+    <row r="51" spans="1:17" s="30" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A51" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B51" s="32" t="s">
+      <c r="B51" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="33">
+      <c r="C51" s="32">
         <v>44064</v>
       </c>
-      <c r="D51" s="33">
+      <c r="D51" s="32">
         <v>44065</v>
       </c>
-      <c r="E51" s="32">
+      <c r="E51" s="31">
         <f t="shared" ref="E51:E52" si="14">D51-C51</f>
         <v>1</v>
       </c>
-      <c r="F51" s="34" t="s">
+      <c r="F51" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G51" s="44">
+      <c r="G51" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="31" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A52" s="26" t="s">
+    <row r="52" spans="1:17" s="30" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A52" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="32" t="s">
+      <c r="B52" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="33">
+      <c r="C52" s="32">
         <v>44065</v>
       </c>
-      <c r="D52" s="33">
+      <c r="D52" s="32">
         <v>44066</v>
       </c>
-      <c r="E52" s="32">
+      <c r="E52" s="31">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="F52" s="34" t="s">
+      <c r="F52" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G52" s="44">
+      <c r="G52" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="22.5" customHeight="1">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="40" t="s">
         <v>80</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="33">
+      <c r="C53" s="32">
         <v>44066</v>
       </c>
-      <c r="D53" s="33">
+      <c r="D53" s="32">
         <v>44067</v>
       </c>
       <c r="E53" s="18">
@@ -4024,70 +4013,70 @@
       <c r="F53" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G53" s="46">
+      <c r="G53" s="45">
         <f>AVERAGE(G54:G55)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="31" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A54" s="27" t="s">
+    <row r="54" spans="1:17" s="30" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A54" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B54" s="32" t="s">
+      <c r="B54" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="33">
+      <c r="C54" s="32">
         <v>44066</v>
       </c>
-      <c r="D54" s="33">
+      <c r="D54" s="32">
         <v>44067</v>
       </c>
-      <c r="E54" s="32">
+      <c r="E54" s="31">
         <f t="shared" ref="E54:E55" si="15">D54-C54</f>
         <v>1</v>
       </c>
-      <c r="F54" s="34" t="s">
+      <c r="F54" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G54" s="47">
+      <c r="G54" s="46">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" s="31" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A55" s="27" t="s">
+    <row r="55" spans="1:17" s="30" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A55" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B55" s="32" t="s">
+      <c r="B55" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="33">
+      <c r="C55" s="32">
         <v>44066</v>
       </c>
-      <c r="D55" s="33">
+      <c r="D55" s="32">
         <v>44067</v>
       </c>
-      <c r="E55" s="32">
+      <c r="E55" s="31">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="F55" s="34" t="s">
+      <c r="F55" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G55" s="44">
+      <c r="G55" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A56" s="38" t="s">
+      <c r="A56" s="37" t="s">
         <v>40</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="33">
+      <c r="C56" s="32">
         <v>44067</v>
       </c>
-      <c r="D56" s="33">
+      <c r="D56" s="32">
         <v>44071</v>
       </c>
       <c r="E56" s="18">
@@ -4097,40 +4086,40 @@
       <c r="F56" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G56" s="45">
+      <c r="G56" s="44">
         <f>AVERAGE(G57:G58)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="31" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A57" s="35" t="s">
+    <row r="57" spans="1:17" s="30" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A57" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="B57" s="32" t="s">
+      <c r="B57" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C57" s="33">
+      <c r="C57" s="32">
         <v>44067</v>
       </c>
-      <c r="D57" s="33">
+      <c r="D57" s="32">
         <v>44070</v>
       </c>
-      <c r="E57" s="32">
+      <c r="E57" s="31">
         <f t="shared" ref="E57" si="16">D57-C57</f>
         <v>3</v>
       </c>
-      <c r="F57" s="34" t="s">
+      <c r="F57" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G57" s="44">
+      <c r="G57" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C58" s="19">
@@ -4146,46 +4135,46 @@
       <c r="F58" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G58" s="44">
+      <c r="G58" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="25.5" customHeight="1">
-      <c r="A59" s="48" t="s">
+      <c r="A59" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B59" s="48"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="44"/>
-    </row>
-    <row r="64" spans="1:17" s="36" customFormat="1" ht="15.75" customHeight="1">
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
-      <c r="I64" s="37" t="s">
+      <c r="B59" s="47"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="43"/>
+    </row>
+    <row r="64" spans="1:17" s="35" customFormat="1" ht="15.75" customHeight="1">
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="36"/>
+      <c r="I64" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="N64" s="37"/>
-      <c r="O64" s="37"/>
-      <c r="P64" s="37"/>
-      <c r="Q64" s="37"/>
-    </row>
-    <row r="65" spans="2:17" s="36" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B65" s="37"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
-      <c r="H65" s="37"/>
-      <c r="M65" s="37"/>
-      <c r="N65" s="37"/>
-      <c r="O65" s="37"/>
-      <c r="P65" s="37"/>
-      <c r="Q65" s="37"/>
+      <c r="N64" s="36"/>
+      <c r="O64" s="36"/>
+      <c r="P64" s="36"/>
+      <c r="Q64" s="36"/>
+    </row>
+    <row r="65" spans="2:17" s="35" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
+      <c r="H65" s="36"/>
+      <c r="M65" s="36"/>
+      <c r="N65" s="36"/>
+      <c r="O65" s="36"/>
+      <c r="P65" s="36"/>
+      <c r="Q65" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4430,20 +4419,20 @@
       <c r="A13" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24">
+      <c r="B13" s="22"/>
+      <c r="C13" s="23">
         <f>SUM(C4:C12)</f>
         <v>25297.5</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="23">
         <f t="shared" ref="D13:E13" si="0">SUM(D4:D12)</f>
         <v>25297.5</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="23">
         <f t="shared" si="0"/>
         <v>25297.5</v>
       </c>
-      <c r="F13" s="23"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="43.15" customHeight="1"/>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de avance general de proyecto
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alumno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antony\Desktop\Repositorio\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A7809A-977B-403C-8C10-B27A177E6C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de proyecto y Gantt" sheetId="1" r:id="rId1"/>
@@ -20,9 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -662,9 +661,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;S/&quot;\ #,##0.00;[Red]&quot;S/&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;S/&quot;\ #,##0.00;[Red]&quot;S/&quot;\ \-#,##0.00"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -1122,14 +1121,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1332,6 +1331,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1341,6 +1361,102 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1352,123 +1468,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1477,7 +1476,7 @@
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6"/>
+    <cellStyle name="Hyperlink" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1494,7 +1493,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1921,7 +1920,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BC27-42F0-95D7-3BD26C201260}"/>
             </c:ext>
@@ -1955,7 +1954,7 @@
             <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -1965,7 +1964,7 @@
             <c:idx val="1"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -1975,7 +1974,7 @@
             <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -1985,7 +1984,7 @@
             <c:idx val="3"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -1995,7 +1994,7 @@
             <c:idx val="4"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2005,7 +2004,7 @@
             <c:idx val="5"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2015,7 +2014,7 @@
             <c:idx val="6"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2025,7 +2024,7 @@
             <c:idx val="7"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000008-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2035,7 +2034,7 @@
             <c:idx val="8"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2045,7 +2044,7 @@
             <c:idx val="9"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000A-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2055,7 +2054,7 @@
             <c:idx val="10"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2065,7 +2064,7 @@
             <c:idx val="11"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000C-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2075,7 +2074,7 @@
             <c:idx val="12"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000D-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2085,7 +2084,7 @@
             <c:idx val="13"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000E-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2095,7 +2094,7 @@
             <c:idx val="14"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000F-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2105,7 +2104,7 @@
             <c:idx val="15"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000010-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2115,7 +2114,7 @@
             <c:idx val="17"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000011-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2125,7 +2124,7 @@
             <c:idx val="18"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000012-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2135,7 +2134,7 @@
             <c:idx val="19"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000013-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2145,7 +2144,7 @@
             <c:idx val="20"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000014-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2155,7 +2154,7 @@
             <c:idx val="21"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000015-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2165,7 +2164,7 @@
             <c:idx val="52"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000017-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2175,7 +2174,7 @@
             <c:idx val="53"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000018-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2185,7 +2184,7 @@
             <c:idx val="54"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000019-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2195,7 +2194,7 @@
             <c:idx val="55"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001A-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2205,7 +2204,7 @@
             <c:idx val="56"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001B-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2215,7 +2214,7 @@
             <c:idx val="57"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001C-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2225,7 +2224,7 @@
             <c:idx val="58"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001D-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2235,7 +2234,7 @@
             <c:idx val="59"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001E-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2245,7 +2244,7 @@
             <c:idx val="60"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001F-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2255,7 +2254,7 @@
             <c:idx val="61"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000020-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2265,7 +2264,7 @@
             <c:idx val="62"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000021-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2275,7 +2274,7 @@
             <c:idx val="63"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000022-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2285,7 +2284,7 @@
             <c:idx val="64"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000023-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2295,7 +2294,7 @@
             <c:idx val="65"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000024-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2305,7 +2304,7 @@
             <c:idx val="66"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000025-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2315,7 +2314,7 @@
             <c:idx val="67"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000026-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2325,7 +2324,7 @@
             <c:idx val="68"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000027-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2335,7 +2334,7 @@
             <c:idx val="69"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000028-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2345,7 +2344,7 @@
             <c:idx val="70"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000029-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2355,7 +2354,7 @@
             <c:idx val="71"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002A-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2365,7 +2364,7 @@
             <c:idx val="72"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002B-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2375,7 +2374,7 @@
             <c:idx val="73"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002C-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2385,7 +2384,7 @@
             <c:idx val="74"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002D-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2395,7 +2394,7 @@
             <c:idx val="75"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002E-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2405,7 +2404,7 @@
             <c:idx val="76"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002F-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2415,7 +2414,7 @@
             <c:idx val="77"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000030-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2425,7 +2424,7 @@
             <c:idx val="78"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000031-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2435,7 +2434,7 @@
             <c:idx val="79"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000032-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2445,6 +2444,11 @@
             <c:idx val="80"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-A56B-4092-AD44-F6187A193878}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2819,7 +2823,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000033-BC27-42F0-95D7-3BD26C201260}"/>
             </c:ext>
@@ -3558,7 +3562,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3900,11 +3904,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3927,21 +3931,21 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="137"/>
-      <c r="N2" s="137"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
@@ -3955,15 +3959,15 @@
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="138" t="s">
+      <c r="B3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -3983,15 +3987,15 @@
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -4011,15 +4015,15 @@
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -4120,7 +4124,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="5">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4269,7 +4273,7 @@
       <c r="C13" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="105"/>
+      <c r="D13" s="130"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26" t="s">
         <v>26</v>
@@ -4305,16 +4309,16 @@
       <c r="V13" s="25"/>
     </row>
     <row r="14" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A14" s="114" t="s">
+      <c r="A14" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="116" t="s">
+      <c r="C14" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="106"/>
+      <c r="D14" s="131"/>
       <c r="E14" s="90" t="s">
         <v>31</v>
       </c>
@@ -4342,10 +4346,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A15" s="115"/>
-      <c r="B15" s="112"/>
-      <c r="C15" s="117"/>
-      <c r="D15" s="106"/>
+      <c r="A15" s="123"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="125"/>
+      <c r="D15" s="131"/>
       <c r="E15" s="90" t="s">
         <v>31</v>
       </c>
@@ -4382,7 +4386,7 @@
       <c r="C16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="106"/>
+      <c r="D16" s="131"/>
       <c r="E16" s="43" t="s">
         <v>34</v>
       </c>
@@ -4418,7 +4422,7 @@
       <c r="C17" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="107"/>
+      <c r="D17" s="132"/>
       <c r="E17" s="44" t="s">
         <v>36</v>
       </c>
@@ -4449,12 +4453,12 @@
       <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="98"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="100"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="139"/>
       <c r="H18" s="27">
         <v>44008</v>
       </c>
@@ -4484,16 +4488,16 @@
       <c r="V18" s="25"/>
     </row>
     <row r="19" spans="1:22" s="25" customFormat="1" ht="36" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="123" t="s">
+      <c r="C19" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="94" t="s">
+      <c r="D19" s="101" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="89" t="s">
@@ -4522,10 +4526,10 @@
       </c>
     </row>
     <row r="20" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="102"/>
-      <c r="B20" s="95"/>
-      <c r="C20" s="124"/>
-      <c r="D20" s="95"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="102"/>
       <c r="E20" s="61" t="s">
         <v>44</v>
       </c>
@@ -4552,10 +4556,10 @@
       </c>
     </row>
     <row r="21" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A21" s="103"/>
-      <c r="B21" s="96"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="96"/>
+      <c r="A21" s="100"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="103"/>
       <c r="E21" s="49" t="s">
         <v>46</v>
       </c>
@@ -4631,16 +4635,16 @@
       <c r="V22" s="25"/>
     </row>
     <row r="23" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A23" s="101" t="s">
+      <c r="A23" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="116" t="s">
+      <c r="B23" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="94" t="s">
+      <c r="D23" s="101" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="61" t="s">
@@ -4670,10 +4674,10 @@
       </c>
     </row>
     <row r="24" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A24" s="102"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="116"/>
-      <c r="D24" s="95"/>
+      <c r="A24" s="99"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="102"/>
       <c r="E24" s="89" t="s">
         <v>56</v>
       </c>
@@ -4701,10 +4705,10 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="52.5" customHeight="1">
-      <c r="A25" s="102"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="116"/>
-      <c r="D25" s="95"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="102"/>
       <c r="E25" s="84" t="s">
         <v>36</v>
       </c>
@@ -4742,61 +4746,61 @@
       <c r="V25" s="25"/>
     </row>
     <row r="26" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A26" s="118" t="s">
+      <c r="A26" s="126" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="110" t="s">
+      <c r="B26" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="110" t="s">
+      <c r="C26" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="112" t="s">
+      <c r="D26" s="124" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="110" t="s">
+      <c r="F26" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="97" t="s">
+      <c r="G26" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="109">
+      <c r="H26" s="134">
         <v>44012</v>
       </c>
-      <c r="I26" s="109">
+      <c r="I26" s="134">
         <v>44013</v>
       </c>
-      <c r="J26" s="112">
+      <c r="J26" s="124">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K26" s="111" t="s">
+      <c r="K26" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="104">
+      <c r="L26" s="129">
         <v>1</v>
       </c>
       <c r="M26" s="67"/>
       <c r="N26" s="48"/>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
-      <c r="A27" s="119"/>
-      <c r="B27" s="110"/>
-      <c r="C27" s="110"/>
-      <c r="D27" s="113"/>
+      <c r="A27" s="127"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="128"/>
       <c r="E27" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="110"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="113"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="104"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="136"/>
+      <c r="H27" s="134"/>
+      <c r="I27" s="134"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="135"/>
+      <c r="L27" s="129"/>
       <c r="M27" s="67"/>
       <c r="N27" s="48"/>
       <c r="O27" s="25"/>
@@ -4809,16 +4813,16 @@
       <c r="V27" s="25"/>
     </row>
     <row r="28" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="101" t="s">
+      <c r="A28" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="110" t="s">
+      <c r="B28" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="110" t="s">
+      <c r="C28" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="110" t="s">
+      <c r="D28" s="111" t="s">
         <v>66</v>
       </c>
       <c r="E28" s="90" t="s">
@@ -4827,51 +4831,51 @@
       <c r="F28" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="97" t="s">
+      <c r="G28" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="H28" s="108">
+      <c r="H28" s="133">
         <v>44010</v>
       </c>
-      <c r="I28" s="109">
+      <c r="I28" s="134">
         <v>44013</v>
       </c>
-      <c r="J28" s="110">
+      <c r="J28" s="111">
         <f>I28-H28</f>
         <v>3</v>
       </c>
-      <c r="K28" s="111" t="s">
+      <c r="K28" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="104">
+      <c r="L28" s="129">
         <v>1</v>
       </c>
       <c r="N28" s="48"/>
     </row>
     <row r="29" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="102"/>
-      <c r="B29" s="110"/>
-      <c r="C29" s="110"/>
-      <c r="D29" s="110"/>
+      <c r="A29" s="99"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="111"/>
+      <c r="D29" s="111"/>
       <c r="E29" s="92" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="97"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="109"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="111"/>
-      <c r="L29" s="104"/>
+      <c r="G29" s="136"/>
+      <c r="H29" s="133"/>
+      <c r="I29" s="134"/>
+      <c r="J29" s="111"/>
+      <c r="K29" s="135"/>
+      <c r="L29" s="129"/>
       <c r="N29" s="48"/>
     </row>
     <row r="30" spans="1:22" ht="30" customHeight="1">
-      <c r="A30" s="103"/>
-      <c r="B30" s="110"/>
-      <c r="C30" s="110"/>
-      <c r="D30" s="110"/>
+      <c r="A30" s="100"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="111"/>
+      <c r="D30" s="111"/>
       <c r="E30" s="26" t="s">
         <v>70</v>
       </c>
@@ -4881,11 +4885,11 @@
       <c r="G30" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="108"/>
-      <c r="I30" s="109"/>
-      <c r="J30" s="110"/>
-      <c r="K30" s="111"/>
-      <c r="L30" s="104"/>
+      <c r="H30" s="133"/>
+      <c r="I30" s="134"/>
+      <c r="J30" s="111"/>
+      <c r="K30" s="135"/>
+      <c r="L30" s="129"/>
       <c r="M30" s="25"/>
       <c r="N30" s="48"/>
       <c r="O30" s="25"/>
@@ -4898,16 +4902,16 @@
       <c r="V30" s="25"/>
     </row>
     <row r="31" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A31" s="101" t="s">
+      <c r="A31" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="123" t="s">
+      <c r="C31" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="94" t="s">
+      <c r="D31" s="101" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="56" t="s">
@@ -4937,10 +4941,10 @@
       </c>
     </row>
     <row r="32" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A32" s="102"/>
-      <c r="B32" s="95"/>
-      <c r="C32" s="124"/>
-      <c r="D32" s="95"/>
+      <c r="A32" s="99"/>
+      <c r="B32" s="102"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="102"/>
       <c r="E32" s="44" t="s">
         <v>78</v>
       </c>
@@ -4967,10 +4971,10 @@
       </c>
     </row>
     <row r="33" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A33" s="102"/>
-      <c r="B33" s="95"/>
-      <c r="C33" s="124"/>
-      <c r="D33" s="95"/>
+      <c r="A33" s="99"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="105"/>
+      <c r="D33" s="102"/>
       <c r="E33" s="44" t="s">
         <v>80</v>
       </c>
@@ -4998,10 +5002,10 @@
       </c>
     </row>
     <row r="34" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A34" s="102"/>
-      <c r="B34" s="95"/>
-      <c r="C34" s="124"/>
-      <c r="D34" s="95"/>
+      <c r="A34" s="99"/>
+      <c r="B34" s="102"/>
+      <c r="C34" s="105"/>
+      <c r="D34" s="102"/>
       <c r="E34" s="44" t="s">
         <v>82</v>
       </c>
@@ -5029,10 +5033,10 @@
       </c>
     </row>
     <row r="35" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A35" s="102"/>
-      <c r="B35" s="95"/>
-      <c r="C35" s="124"/>
-      <c r="D35" s="95"/>
+      <c r="A35" s="99"/>
+      <c r="B35" s="102"/>
+      <c r="C35" s="105"/>
+      <c r="D35" s="102"/>
       <c r="E35" s="44" t="s">
         <v>84</v>
       </c>
@@ -5060,10 +5064,10 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="33" customHeight="1">
-      <c r="A36" s="103"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="96"/>
+      <c r="A36" s="100"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="103"/>
       <c r="E36" s="44" t="s">
         <v>86</v>
       </c>
@@ -5142,12 +5146,12 @@
       <c r="A38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="98"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="99"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="100"/>
+      <c r="B38" s="137"/>
+      <c r="C38" s="138"/>
+      <c r="D38" s="138"/>
+      <c r="E38" s="138"/>
+      <c r="F38" s="138"/>
+      <c r="G38" s="139"/>
       <c r="H38" s="27">
         <v>43837</v>
       </c>
@@ -5176,14 +5180,14 @@
       <c r="V38" s="25"/>
     </row>
     <row r="39" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A39" s="94" t="s">
+      <c r="A39" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="94" t="s">
+      <c r="B39" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="94"/>
-      <c r="D39" s="94" t="s">
+      <c r="C39" s="101"/>
+      <c r="D39" s="101" t="s">
         <v>96</v>
       </c>
       <c r="E39" s="63" t="s">
@@ -5213,10 +5217,10 @@
       <c r="N39" s="48"/>
     </row>
     <row r="40" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A40" s="95"/>
-      <c r="B40" s="95"/>
-      <c r="C40" s="95"/>
-      <c r="D40" s="95"/>
+      <c r="A40" s="102"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="102"/>
+      <c r="D40" s="102"/>
       <c r="E40" s="49" t="s">
         <v>100</v>
       </c>
@@ -5244,10 +5248,10 @@
       <c r="N40" s="48"/>
     </row>
     <row r="41" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A41" s="95"/>
-      <c r="B41" s="95"/>
-      <c r="C41" s="95"/>
-      <c r="D41" s="95"/>
+      <c r="A41" s="102"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="102"/>
+      <c r="D41" s="102"/>
       <c r="E41" s="49" t="s">
         <v>102</v>
       </c>
@@ -5275,10 +5279,10 @@
       <c r="N41" s="48"/>
     </row>
     <row r="42" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A42" s="95"/>
-      <c r="B42" s="95"/>
-      <c r="C42" s="95"/>
-      <c r="D42" s="95"/>
+      <c r="A42" s="102"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="102"/>
+      <c r="D42" s="102"/>
       <c r="E42" s="63" t="s">
         <v>104</v>
       </c>
@@ -5306,10 +5310,10 @@
       <c r="N42" s="48"/>
     </row>
     <row r="43" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A43" s="96"/>
-      <c r="B43" s="96"/>
-      <c r="C43" s="96"/>
-      <c r="D43" s="96"/>
+      <c r="A43" s="103"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="103"/>
       <c r="E43" s="43" t="s">
         <v>106</v>
       </c>
@@ -5386,16 +5390,16 @@
       <c r="V44" s="25"/>
     </row>
     <row r="45" spans="1:22" s="25" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A45" s="101" t="s">
+      <c r="A45" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="94" t="s">
+      <c r="B45" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="123" t="s">
+      <c r="C45" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="101" t="s">
+      <c r="D45" s="98" t="s">
         <v>27</v>
       </c>
       <c r="E45" s="43" t="s">
@@ -5425,10 +5429,10 @@
       <c r="N45" s="48"/>
     </row>
     <row r="46" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A46" s="103"/>
-      <c r="B46" s="96"/>
-      <c r="C46" s="125"/>
-      <c r="D46" s="103"/>
+      <c r="A46" s="100"/>
+      <c r="B46" s="103"/>
+      <c r="C46" s="106"/>
+      <c r="D46" s="100"/>
       <c r="E46" s="90" t="s">
         <v>117</v>
       </c>
@@ -5466,19 +5470,19 @@
       <c r="V46" s="25"/>
     </row>
     <row r="47" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A47" s="131" t="s">
+      <c r="A47" s="97" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="131"/>
-      <c r="C47" s="131"/>
-      <c r="D47" s="131"/>
-      <c r="E47" s="131"/>
-      <c r="F47" s="131"/>
-      <c r="G47" s="131"/>
-      <c r="H47" s="131"/>
-      <c r="I47" s="131"/>
-      <c r="J47" s="131"/>
-      <c r="K47" s="131"/>
+      <c r="B47" s="97"/>
+      <c r="C47" s="97"/>
+      <c r="D47" s="97"/>
+      <c r="E47" s="97"/>
+      <c r="F47" s="97"/>
+      <c r="G47" s="97"/>
+      <c r="H47" s="97"/>
+      <c r="I47" s="97"/>
+      <c r="J47" s="97"/>
+      <c r="K47" s="97"/>
       <c r="L47" s="38"/>
       <c r="M47" s="25"/>
       <c r="N47" s="25"/>
@@ -5548,16 +5552,16 @@
       </c>
     </row>
     <row r="50" spans="1:22" ht="38.25" customHeight="1">
-      <c r="A50" s="126" t="s">
+      <c r="A50" s="120" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="110" t="s">
+      <c r="B50" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="123" t="s">
+      <c r="C50" s="104" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="128"/>
+      <c r="D50" s="108"/>
       <c r="E50" s="44" t="s">
         <v>124</v>
       </c>
@@ -5595,10 +5599,10 @@
       <c r="V50" s="25"/>
     </row>
     <row r="51" spans="1:22" s="25" customFormat="1" ht="45" customHeight="1">
-      <c r="A51" s="126"/>
-      <c r="B51" s="110"/>
-      <c r="C51" s="125"/>
-      <c r="D51" s="129"/>
+      <c r="A51" s="120"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="106"/>
+      <c r="D51" s="109"/>
       <c r="E51" s="49" t="s">
         <v>126</v>
       </c>
@@ -5626,16 +5630,16 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A52" s="130" t="s">
+      <c r="A52" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="110" t="s">
+      <c r="B52" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="116" t="s">
+      <c r="C52" s="107" t="s">
         <v>123</v>
       </c>
-      <c r="D52" s="110"/>
+      <c r="D52" s="111"/>
       <c r="E52" s="88" t="s">
         <v>129</v>
       </c>
@@ -5663,10 +5667,10 @@
       </c>
     </row>
     <row r="53" spans="1:22" s="25" customFormat="1" ht="57" customHeight="1">
-      <c r="A53" s="130"/>
-      <c r="B53" s="110"/>
-      <c r="C53" s="116"/>
-      <c r="D53" s="110"/>
+      <c r="A53" s="110"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="107"/>
+      <c r="D53" s="111"/>
       <c r="E53" s="88" t="s">
         <v>130</v>
       </c>
@@ -5694,16 +5698,16 @@
       </c>
     </row>
     <row r="54" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A54" s="126" t="s">
+      <c r="A54" s="120" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="127" t="s">
+      <c r="B54" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="116" t="s">
+      <c r="C54" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="127"/>
+      <c r="D54" s="121"/>
       <c r="E54" s="88" t="s">
         <v>134</v>
       </c>
@@ -5731,10 +5735,10 @@
       </c>
     </row>
     <row r="55" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A55" s="126"/>
-      <c r="B55" s="127"/>
-      <c r="C55" s="116"/>
-      <c r="D55" s="127"/>
+      <c r="A55" s="120"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="107"/>
+      <c r="D55" s="121"/>
       <c r="E55" s="90" t="s">
         <v>136</v>
       </c>
@@ -5826,16 +5830,16 @@
       </c>
     </row>
     <row r="58" spans="1:22" s="25" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A58" s="120" t="s">
+      <c r="A58" s="117" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="94" t="s">
+      <c r="B58" s="101" t="s">
         <v>141</v>
       </c>
-      <c r="C58" s="123" t="s">
+      <c r="C58" s="104" t="s">
         <v>143</v>
       </c>
-      <c r="D58" s="94"/>
+      <c r="D58" s="101"/>
       <c r="E58" s="49" t="s">
         <v>144</v>
       </c>
@@ -5863,10 +5867,10 @@
       </c>
     </row>
     <row r="59" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A59" s="121"/>
-      <c r="B59" s="95"/>
-      <c r="C59" s="124"/>
-      <c r="D59" s="95"/>
+      <c r="A59" s="118"/>
+      <c r="B59" s="102"/>
+      <c r="C59" s="105"/>
+      <c r="D59" s="102"/>
       <c r="E59" s="84" t="s">
         <v>146</v>
       </c>
@@ -5893,10 +5897,10 @@
       </c>
     </row>
     <row r="60" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A60" s="122"/>
-      <c r="B60" s="96"/>
-      <c r="C60" s="125"/>
-      <c r="D60" s="96"/>
+      <c r="A60" s="119"/>
+      <c r="B60" s="103"/>
+      <c r="C60" s="106"/>
+      <c r="D60" s="103"/>
       <c r="E60" s="84" t="s">
         <v>148</v>
       </c>
@@ -5921,16 +5925,16 @@
       </c>
     </row>
     <row r="61" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A61" s="130" t="s">
+      <c r="A61" s="110" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="94" t="s">
+      <c r="B61" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="123" t="s">
+      <c r="C61" s="104" t="s">
         <v>150</v>
       </c>
-      <c r="D61" s="128"/>
+      <c r="D61" s="108"/>
       <c r="E61" s="61" t="s">
         <v>151</v>
       </c>
@@ -5958,10 +5962,10 @@
       </c>
     </row>
     <row r="62" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A62" s="130"/>
-      <c r="B62" s="95"/>
-      <c r="C62" s="124"/>
-      <c r="D62" s="135"/>
+      <c r="A62" s="110"/>
+      <c r="B62" s="102"/>
+      <c r="C62" s="105"/>
+      <c r="D62" s="115"/>
       <c r="E62" s="61" t="s">
         <v>154</v>
       </c>
@@ -5989,10 +5993,10 @@
       </c>
     </row>
     <row r="63" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A63" s="130"/>
-      <c r="B63" s="133"/>
-      <c r="C63" s="134"/>
-      <c r="D63" s="136"/>
+      <c r="A63" s="110"/>
+      <c r="B63" s="113"/>
+      <c r="C63" s="114"/>
+      <c r="D63" s="116"/>
       <c r="E63" s="61" t="s">
         <v>156</v>
       </c>
@@ -6020,19 +6024,19 @@
       </c>
     </row>
     <row r="64" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A64" s="132" t="s">
+      <c r="A64" s="112" t="s">
         <v>159</v>
       </c>
-      <c r="B64" s="132"/>
-      <c r="C64" s="132"/>
-      <c r="D64" s="132"/>
-      <c r="E64" s="132"/>
-      <c r="F64" s="132"/>
-      <c r="G64" s="132"/>
-      <c r="H64" s="132"/>
-      <c r="I64" s="132"/>
-      <c r="J64" s="132"/>
-      <c r="K64" s="132"/>
+      <c r="B64" s="112"/>
+      <c r="C64" s="112"/>
+      <c r="D64" s="112"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="112"/>
+      <c r="G64" s="112"/>
+      <c r="H64" s="112"/>
+      <c r="I64" s="112"/>
+      <c r="J64" s="112"/>
+      <c r="K64" s="112"/>
       <c r="L64" s="57"/>
       <c r="M64" s="25"/>
       <c r="N64" s="25"/>
@@ -6670,19 +6674,19 @@
       <c r="V83" s="25"/>
     </row>
     <row r="84" spans="1:22" ht="25.5" customHeight="1">
-      <c r="A84" s="131" t="s">
+      <c r="A84" s="97" t="s">
         <v>179</v>
       </c>
-      <c r="B84" s="131"/>
-      <c r="C84" s="131"/>
-      <c r="D84" s="131"/>
-      <c r="E84" s="131"/>
-      <c r="F84" s="131"/>
-      <c r="G84" s="131"/>
-      <c r="H84" s="131"/>
-      <c r="I84" s="131"/>
-      <c r="J84" s="131"/>
-      <c r="K84" s="131"/>
+      <c r="B84" s="97"/>
+      <c r="C84" s="97"/>
+      <c r="D84" s="97"/>
+      <c r="E84" s="97"/>
+      <c r="F84" s="97"/>
+      <c r="G84" s="97"/>
+      <c r="H84" s="97"/>
+      <c r="I84" s="97"/>
+      <c r="J84" s="97"/>
+      <c r="K84" s="97"/>
       <c r="L84" s="38"/>
       <c r="M84" s="25"/>
       <c r="N84" s="25"/>
@@ -6861,6 +6865,64 @@
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A84:K84"/>
+    <mergeCell ref="A64:K64"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
@@ -6877,99 +6939,41 @@
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="C31:C36"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A84:K84"/>
-    <mergeCell ref="A64:K64"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G20" r:id="rId1"/>
-    <hyperlink ref="G21" r:id="rId2"/>
-    <hyperlink ref="G34" r:id="rId3"/>
-    <hyperlink ref="G23" r:id="rId4"/>
-    <hyperlink ref="G63" r:id="rId5"/>
-    <hyperlink ref="G12" r:id="rId6"/>
-    <hyperlink ref="G24" r:id="rId7"/>
-    <hyperlink ref="G39" r:id="rId8"/>
-    <hyperlink ref="G30" r:id="rId9"/>
-    <hyperlink ref="G33" r:id="rId10"/>
-    <hyperlink ref="G43" r:id="rId11"/>
-    <hyperlink ref="G25" r:id="rId12"/>
-    <hyperlink ref="G41" r:id="rId13"/>
-    <hyperlink ref="G44" r:id="rId14"/>
-    <hyperlink ref="G32" r:id="rId15"/>
-    <hyperlink ref="G40" r:id="rId16"/>
-    <hyperlink ref="G26:G27" r:id="rId17" display="https://github.com/antonyMontalvo/FaceSolutions/commit/8f0ec13380b96dbff2cf0f44e517515e6d8e935b"/>
-    <hyperlink ref="G58" r:id="rId18"/>
-    <hyperlink ref="G51" r:id="rId19"/>
-    <hyperlink ref="G36" r:id="rId20"/>
-    <hyperlink ref="G28:G29" r:id="rId21" display="https://github.com/antonyMontalvo/FaceSolutions/commit/b7f87017c045c76f3ed7353bf35a7680607f9adf"/>
-    <hyperlink ref="G42" r:id="rId22"/>
-    <hyperlink ref="G37" r:id="rId23"/>
-    <hyperlink ref="G50" r:id="rId24"/>
-    <hyperlink ref="G31" r:id="rId25"/>
-    <hyperlink ref="G55" r:id="rId26"/>
-    <hyperlink ref="G61" r:id="rId27"/>
-    <hyperlink ref="G19" r:id="rId28"/>
-    <hyperlink ref="G35" r:id="rId29"/>
-    <hyperlink ref="G54" r:id="rId30"/>
-    <hyperlink ref="G53" r:id="rId31"/>
-    <hyperlink ref="G62" r:id="rId32"/>
-    <hyperlink ref="G59" r:id="rId33"/>
+    <hyperlink ref="G20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G23" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G63" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G12" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G24" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G39" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G30" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G33" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G43" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G25" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G41" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G44" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G32" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G40" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G26:G27" r:id="rId17" display="https://github.com/antonyMontalvo/FaceSolutions/commit/8f0ec13380b96dbff2cf0f44e517515e6d8e935b" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G58" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G51" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G36" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G28:G29" r:id="rId21" display="https://github.com/antonyMontalvo/FaceSolutions/commit/b7f87017c045c76f3ed7353bf35a7680607f9adf" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G42" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G37" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G50" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G31" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G55" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G61" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G19" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G35" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G54" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G53" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G62" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G59" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId34"/>
@@ -6978,7 +6982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Actualización de porcentaje global de avance de proyecto
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -1,29 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alumno\Desktop\Nueva carpeta (5)\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antony\Desktop\Repo\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB46D06-53DD-4AF9-B9B5-444DF031061A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de proyecto y Gantt" sheetId="1" r:id="rId1"/>
     <sheet name="Línea base de costo" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -684,9 +677,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;S/&quot;\ #,##0.00;[Red]&quot;S/&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;S/&quot;\ #,##0.00;[Red]&quot;S/&quot;\ \-#,##0.00"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -1144,14 +1137,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1369,6 +1362,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1377,159 +1523,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1538,7 +1531,7 @@
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6"/>
+    <cellStyle name="Hyperlink" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1555,7 +1548,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2003,7 +1996,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BC27-42F0-95D7-3BD26C201260}"/>
             </c:ext>
@@ -2037,7 +2030,7 @@
             <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2047,7 +2040,7 @@
             <c:idx val="1"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2057,7 +2050,7 @@
             <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2067,7 +2060,7 @@
             <c:idx val="3"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2077,7 +2070,7 @@
             <c:idx val="4"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2087,7 +2080,7 @@
             <c:idx val="5"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2097,7 +2090,7 @@
             <c:idx val="6"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2107,7 +2100,7 @@
             <c:idx val="7"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000008-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2117,7 +2110,7 @@
             <c:idx val="8"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2127,7 +2120,7 @@
             <c:idx val="9"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000A-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2137,7 +2130,7 @@
             <c:idx val="10"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2147,7 +2140,7 @@
             <c:idx val="11"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000C-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2157,7 +2150,7 @@
             <c:idx val="12"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000D-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2167,7 +2160,7 @@
             <c:idx val="13"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000E-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2177,7 +2170,7 @@
             <c:idx val="14"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000F-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2187,7 +2180,7 @@
             <c:idx val="15"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000010-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2197,7 +2190,7 @@
             <c:idx val="17"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000011-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2207,7 +2200,7 @@
             <c:idx val="18"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000012-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2217,7 +2210,7 @@
             <c:idx val="19"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000013-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2227,7 +2220,7 @@
             <c:idx val="20"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000014-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2237,7 +2230,7 @@
             <c:idx val="21"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000015-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2247,7 +2240,7 @@
             <c:idx val="52"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000018-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2257,7 +2250,7 @@
             <c:idx val="53"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000019-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2267,7 +2260,7 @@
             <c:idx val="54"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001A-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2277,7 +2270,7 @@
             <c:idx val="55"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001B-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2287,7 +2280,7 @@
             <c:idx val="56"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001C-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2297,7 +2290,7 @@
             <c:idx val="57"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001D-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2307,7 +2300,7 @@
             <c:idx val="58"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001E-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2317,7 +2310,7 @@
             <c:idx val="59"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001F-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2327,7 +2320,7 @@
             <c:idx val="60"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000020-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2337,7 +2330,7 @@
             <c:idx val="61"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000021-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2347,7 +2340,7 @@
             <c:idx val="62"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000022-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2357,7 +2350,7 @@
             <c:idx val="63"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000023-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2367,7 +2360,7 @@
             <c:idx val="64"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000024-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2377,7 +2370,7 @@
             <c:idx val="65"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000025-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2387,7 +2380,7 @@
             <c:idx val="66"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000026-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2397,7 +2390,7 @@
             <c:idx val="67"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000027-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2407,7 +2400,7 @@
             <c:idx val="68"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000028-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2417,7 +2410,7 @@
             <c:idx val="69"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000029-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2427,7 +2420,7 @@
             <c:idx val="70"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002A-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2437,7 +2430,7 @@
             <c:idx val="71"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002B-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2447,7 +2440,7 @@
             <c:idx val="72"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002C-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2457,7 +2450,7 @@
             <c:idx val="73"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002D-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2467,7 +2460,7 @@
             <c:idx val="74"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002E-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2477,7 +2470,7 @@
             <c:idx val="75"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000002F-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2487,7 +2480,7 @@
             <c:idx val="76"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000030-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2497,7 +2490,7 @@
             <c:idx val="77"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000031-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2507,7 +2500,7 @@
             <c:idx val="78"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000032-BC27-42F0-95D7-3BD26C201260}"/>
               </c:ext>
@@ -2517,7 +2510,7 @@
             <c:idx val="79"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000031-A56B-4092-AD44-F6187A193878}"/>
               </c:ext>
@@ -2527,6 +2520,11 @@
             <c:idx val="80"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-6AFF-4213-8C94-68D0D3B9F6B8}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2922,7 +2920,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000033-BC27-42F0-95D7-3BD26C201260}"/>
             </c:ext>
@@ -3661,7 +3659,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4003,11 +4001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4030,21 +4028,21 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="150"/>
+      <c r="L2" s="150"/>
+      <c r="M2" s="150"/>
+      <c r="N2" s="150"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
@@ -4058,15 +4056,15 @@
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -4086,15 +4084,15 @@
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="151" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -4114,15 +4112,15 @@
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="152" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
+      <c r="E5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="152"/>
+      <c r="H5" s="152"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -4223,7 +4221,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="5">
-        <v>0.46</v>
+        <v>0.6</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4372,7 +4370,7 @@
       <c r="C13" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="135"/>
+      <c r="D13" s="112"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26" t="s">
         <v>26</v>
@@ -4408,16 +4406,16 @@
       <c r="V13" s="25"/>
     </row>
     <row r="14" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A14" s="127" t="s">
+      <c r="A14" s="121" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="116" t="s">
+      <c r="B14" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="112" t="s">
+      <c r="C14" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="136"/>
+      <c r="D14" s="113"/>
       <c r="E14" s="90" t="s">
         <v>31</v>
       </c>
@@ -4445,10 +4443,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A15" s="128"/>
-      <c r="B15" s="129"/>
-      <c r="C15" s="130"/>
-      <c r="D15" s="136"/>
+      <c r="A15" s="122"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="113"/>
       <c r="E15" s="90" t="s">
         <v>31</v>
       </c>
@@ -4485,7 +4483,7 @@
       <c r="C16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="136"/>
+      <c r="D16" s="113"/>
       <c r="E16" s="43" t="s">
         <v>34</v>
       </c>
@@ -4521,7 +4519,7 @@
       <c r="C17" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="137"/>
+      <c r="D17" s="114"/>
       <c r="E17" s="44" t="s">
         <v>36</v>
       </c>
@@ -4552,12 +4550,12 @@
       <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="142"/>
-      <c r="C18" s="143"/>
-      <c r="D18" s="143"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="144"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="107"/>
       <c r="H18" s="27">
         <v>44008</v>
       </c>
@@ -4587,16 +4585,16 @@
       <c r="V18" s="25"/>
     </row>
     <row r="19" spans="1:22" s="25" customFormat="1" ht="36" customHeight="1">
-      <c r="A19" s="103" t="s">
+      <c r="A19" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="109" t="s">
+      <c r="C19" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="106" t="s">
+      <c r="D19" s="101" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="89" t="s">
@@ -4625,10 +4623,10 @@
       </c>
     </row>
     <row r="20" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="104"/>
-      <c r="B20" s="107"/>
-      <c r="C20" s="110"/>
-      <c r="D20" s="107"/>
+      <c r="A20" s="109"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="131"/>
+      <c r="D20" s="102"/>
       <c r="E20" s="61" t="s">
         <v>44</v>
       </c>
@@ -4655,10 +4653,10 @@
       </c>
     </row>
     <row r="21" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A21" s="105"/>
-      <c r="B21" s="108"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="108"/>
+      <c r="A21" s="110"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="132"/>
+      <c r="D21" s="103"/>
       <c r="E21" s="49" t="s">
         <v>46</v>
       </c>
@@ -4734,16 +4732,16 @@
       <c r="V22" s="25"/>
     </row>
     <row r="23" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A23" s="103" t="s">
+      <c r="A23" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="112" t="s">
+      <c r="B23" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="112" t="s">
+      <c r="C23" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="106" t="s">
+      <c r="D23" s="101" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="61" t="s">
@@ -4773,10 +4771,10 @@
       </c>
     </row>
     <row r="24" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A24" s="104"/>
-      <c r="B24" s="112"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="107"/>
+      <c r="A24" s="109"/>
+      <c r="B24" s="123"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="102"/>
       <c r="E24" s="89" t="s">
         <v>56</v>
       </c>
@@ -4804,10 +4802,10 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="52.5" customHeight="1">
-      <c r="A25" s="104"/>
-      <c r="B25" s="112"/>
-      <c r="C25" s="112"/>
-      <c r="D25" s="107"/>
+      <c r="A25" s="109"/>
+      <c r="B25" s="123"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="102"/>
       <c r="E25" s="84" t="s">
         <v>36</v>
       </c>
@@ -4845,61 +4843,61 @@
       <c r="V25" s="25"/>
     </row>
     <row r="26" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A26" s="131" t="s">
+      <c r="A26" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="116" t="s">
+      <c r="B26" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="116" t="s">
+      <c r="C26" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="129" t="s">
+      <c r="D26" s="119" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="116" t="s">
+      <c r="F26" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="141" t="s">
+      <c r="G26" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="139">
+      <c r="H26" s="116">
         <v>44012</v>
       </c>
-      <c r="I26" s="139">
+      <c r="I26" s="116">
         <v>44013</v>
       </c>
-      <c r="J26" s="129">
+      <c r="J26" s="119">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K26" s="140" t="s">
+      <c r="K26" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="134">
+      <c r="L26" s="111">
         <v>1</v>
       </c>
       <c r="M26" s="67"/>
       <c r="N26" s="48"/>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
-      <c r="A27" s="132"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="133"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="120"/>
       <c r="E27" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="116"/>
-      <c r="G27" s="141"/>
-      <c r="H27" s="139"/>
-      <c r="I27" s="139"/>
-      <c r="J27" s="133"/>
-      <c r="K27" s="140"/>
-      <c r="L27" s="134"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="116"/>
+      <c r="I27" s="116"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="111"/>
       <c r="M27" s="67"/>
       <c r="N27" s="48"/>
       <c r="O27" s="25"/>
@@ -4912,16 +4910,16 @@
       <c r="V27" s="25"/>
     </row>
     <row r="28" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="103" t="s">
+      <c r="A28" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="116" t="s">
+      <c r="B28" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="116" t="s">
+      <c r="C28" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="116" t="s">
+      <c r="D28" s="117" t="s">
         <v>66</v>
       </c>
       <c r="E28" s="90" t="s">
@@ -4930,51 +4928,51 @@
       <c r="F28" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="141" t="s">
+      <c r="G28" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="H28" s="138">
+      <c r="H28" s="115">
         <v>44010</v>
       </c>
-      <c r="I28" s="139">
+      <c r="I28" s="116">
         <v>44013</v>
       </c>
-      <c r="J28" s="116">
+      <c r="J28" s="117">
         <f>I28-H28</f>
         <v>3</v>
       </c>
-      <c r="K28" s="140" t="s">
+      <c r="K28" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="134">
+      <c r="L28" s="111">
         <v>1</v>
       </c>
       <c r="N28" s="48"/>
     </row>
     <row r="29" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="104"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="116"/>
-      <c r="D29" s="116"/>
+      <c r="A29" s="109"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="117"/>
+      <c r="D29" s="117"/>
       <c r="E29" s="92" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="141"/>
-      <c r="H29" s="138"/>
-      <c r="I29" s="139"/>
-      <c r="J29" s="116"/>
-      <c r="K29" s="140"/>
-      <c r="L29" s="134"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="115"/>
+      <c r="I29" s="116"/>
+      <c r="J29" s="117"/>
+      <c r="K29" s="118"/>
+      <c r="L29" s="111"/>
       <c r="N29" s="48"/>
     </row>
     <row r="30" spans="1:22" ht="30" customHeight="1">
-      <c r="A30" s="105"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
+      <c r="A30" s="110"/>
+      <c r="B30" s="117"/>
+      <c r="C30" s="117"/>
+      <c r="D30" s="117"/>
       <c r="E30" s="26" t="s">
         <v>70</v>
       </c>
@@ -4984,11 +4982,11 @@
       <c r="G30" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="138"/>
-      <c r="I30" s="139"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="140"/>
-      <c r="L30" s="134"/>
+      <c r="H30" s="115"/>
+      <c r="I30" s="116"/>
+      <c r="J30" s="117"/>
+      <c r="K30" s="118"/>
+      <c r="L30" s="111"/>
       <c r="M30" s="25"/>
       <c r="N30" s="48"/>
       <c r="O30" s="25"/>
@@ -5001,16 +4999,16 @@
       <c r="V30" s="25"/>
     </row>
     <row r="31" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="108" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="106" t="s">
+      <c r="B31" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="109" t="s">
+      <c r="C31" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="106" t="s">
+      <c r="D31" s="101" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="56" t="s">
@@ -5040,10 +5038,10 @@
       </c>
     </row>
     <row r="32" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A32" s="104"/>
-      <c r="B32" s="107"/>
-      <c r="C32" s="110"/>
-      <c r="D32" s="107"/>
+      <c r="A32" s="109"/>
+      <c r="B32" s="102"/>
+      <c r="C32" s="131"/>
+      <c r="D32" s="102"/>
       <c r="E32" s="44" t="s">
         <v>78</v>
       </c>
@@ -5070,10 +5068,10 @@
       </c>
     </row>
     <row r="33" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A33" s="104"/>
-      <c r="B33" s="107"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="107"/>
+      <c r="A33" s="109"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="131"/>
+      <c r="D33" s="102"/>
       <c r="E33" s="44" t="s">
         <v>80</v>
       </c>
@@ -5101,10 +5099,10 @@
       </c>
     </row>
     <row r="34" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A34" s="104"/>
-      <c r="B34" s="107"/>
-      <c r="C34" s="110"/>
-      <c r="D34" s="107"/>
+      <c r="A34" s="109"/>
+      <c r="B34" s="102"/>
+      <c r="C34" s="131"/>
+      <c r="D34" s="102"/>
       <c r="E34" s="44" t="s">
         <v>82</v>
       </c>
@@ -5132,10 +5130,10 @@
       </c>
     </row>
     <row r="35" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A35" s="104"/>
-      <c r="B35" s="107"/>
-      <c r="C35" s="110"/>
-      <c r="D35" s="107"/>
+      <c r="A35" s="109"/>
+      <c r="B35" s="102"/>
+      <c r="C35" s="131"/>
+      <c r="D35" s="102"/>
       <c r="E35" s="44" t="s">
         <v>84</v>
       </c>
@@ -5163,10 +5161,10 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="33" customHeight="1">
-      <c r="A36" s="105"/>
-      <c r="B36" s="108"/>
-      <c r="C36" s="111"/>
-      <c r="D36" s="108"/>
+      <c r="A36" s="110"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="132"/>
+      <c r="D36" s="103"/>
       <c r="E36" s="44" t="s">
         <v>86</v>
       </c>
@@ -5245,12 +5243,12 @@
       <c r="A38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="142"/>
-      <c r="C38" s="143"/>
-      <c r="D38" s="143"/>
-      <c r="E38" s="143"/>
-      <c r="F38" s="143"/>
-      <c r="G38" s="144"/>
+      <c r="B38" s="105"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="107"/>
       <c r="H38" s="27">
         <v>43837</v>
       </c>
@@ -5279,14 +5277,14 @@
       <c r="V38" s="25"/>
     </row>
     <row r="39" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A39" s="106" t="s">
+      <c r="A39" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="106" t="s">
+      <c r="B39" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="106"/>
-      <c r="D39" s="106" t="s">
+      <c r="C39" s="101"/>
+      <c r="D39" s="101" t="s">
         <v>96</v>
       </c>
       <c r="E39" s="63" t="s">
@@ -5316,10 +5314,10 @@
       <c r="N39" s="48"/>
     </row>
     <row r="40" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A40" s="107"/>
-      <c r="B40" s="107"/>
-      <c r="C40" s="107"/>
-      <c r="D40" s="107"/>
+      <c r="A40" s="102"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="102"/>
+      <c r="D40" s="102"/>
       <c r="E40" s="49" t="s">
         <v>100</v>
       </c>
@@ -5347,10 +5345,10 @@
       <c r="N40" s="48"/>
     </row>
     <row r="41" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A41" s="107"/>
-      <c r="B41" s="107"/>
-      <c r="C41" s="107"/>
-      <c r="D41" s="107"/>
+      <c r="A41" s="102"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="102"/>
+      <c r="D41" s="102"/>
       <c r="E41" s="49" t="s">
         <v>102</v>
       </c>
@@ -5378,10 +5376,10 @@
       <c r="N41" s="48"/>
     </row>
     <row r="42" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A42" s="107"/>
-      <c r="B42" s="107"/>
-      <c r="C42" s="107"/>
-      <c r="D42" s="107"/>
+      <c r="A42" s="102"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="102"/>
+      <c r="D42" s="102"/>
       <c r="E42" s="63" t="s">
         <v>104</v>
       </c>
@@ -5409,10 +5407,10 @@
       <c r="N42" s="48"/>
     </row>
     <row r="43" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A43" s="108"/>
-      <c r="B43" s="108"/>
-      <c r="C43" s="108"/>
-      <c r="D43" s="108"/>
+      <c r="A43" s="103"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="103"/>
       <c r="E43" s="43" t="s">
         <v>106</v>
       </c>
@@ -5489,16 +5487,16 @@
       <c r="V44" s="25"/>
     </row>
     <row r="45" spans="1:22" s="25" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A45" s="103" t="s">
+      <c r="A45" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="106" t="s">
+      <c r="B45" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="109" t="s">
+      <c r="C45" s="130" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="103" t="s">
+      <c r="D45" s="108" t="s">
         <v>27</v>
       </c>
       <c r="E45" s="43" t="s">
@@ -5528,10 +5526,10 @@
       <c r="N45" s="48"/>
     </row>
     <row r="46" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A46" s="105"/>
-      <c r="B46" s="108"/>
-      <c r="C46" s="111"/>
-      <c r="D46" s="105"/>
+      <c r="A46" s="110"/>
+      <c r="B46" s="103"/>
+      <c r="C46" s="132"/>
+      <c r="D46" s="110"/>
       <c r="E46" s="90" t="s">
         <v>117</v>
       </c>
@@ -5569,19 +5567,19 @@
       <c r="V46" s="25"/>
     </row>
     <row r="47" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A47" s="102" t="s">
+      <c r="A47" s="140" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="102"/>
-      <c r="C47" s="102"/>
-      <c r="D47" s="102"/>
-      <c r="E47" s="102"/>
-      <c r="F47" s="102"/>
-      <c r="G47" s="102"/>
-      <c r="H47" s="102"/>
-      <c r="I47" s="102"/>
-      <c r="J47" s="102"/>
-      <c r="K47" s="102"/>
+      <c r="B47" s="140"/>
+      <c r="C47" s="140"/>
+      <c r="D47" s="140"/>
+      <c r="E47" s="140"/>
+      <c r="F47" s="140"/>
+      <c r="G47" s="140"/>
+      <c r="H47" s="140"/>
+      <c r="I47" s="140"/>
+      <c r="J47" s="140"/>
+      <c r="K47" s="140"/>
       <c r="L47" s="38"/>
       <c r="M47" s="25"/>
       <c r="N47" s="25"/>
@@ -5651,16 +5649,16 @@
       </c>
     </row>
     <row r="50" spans="1:22" ht="38.25" customHeight="1">
-      <c r="A50" s="125" t="s">
+      <c r="A50" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="116" t="s">
+      <c r="B50" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="109" t="s">
+      <c r="C50" s="130" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="113"/>
+      <c r="D50" s="137"/>
       <c r="E50" s="44" t="s">
         <v>124</v>
       </c>
@@ -5698,10 +5696,10 @@
       <c r="V50" s="25"/>
     </row>
     <row r="51" spans="1:22" s="25" customFormat="1" ht="45" customHeight="1">
-      <c r="A51" s="125"/>
-      <c r="B51" s="116"/>
-      <c r="C51" s="111"/>
-      <c r="D51" s="114"/>
+      <c r="A51" s="133"/>
+      <c r="B51" s="117"/>
+      <c r="C51" s="132"/>
+      <c r="D51" s="138"/>
       <c r="E51" s="49" t="s">
         <v>126</v>
       </c>
@@ -5729,16 +5727,16 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A52" s="115" t="s">
+      <c r="A52" s="139" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="116" t="s">
+      <c r="B52" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="112" t="s">
+      <c r="C52" s="123" t="s">
         <v>123</v>
       </c>
-      <c r="D52" s="116"/>
+      <c r="D52" s="117"/>
       <c r="E52" s="88" t="s">
         <v>129</v>
       </c>
@@ -5766,10 +5764,10 @@
       </c>
     </row>
     <row r="53" spans="1:22" s="25" customFormat="1" ht="57" customHeight="1">
-      <c r="A53" s="115"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="112"/>
-      <c r="D53" s="116"/>
+      <c r="A53" s="139"/>
+      <c r="B53" s="117"/>
+      <c r="C53" s="123"/>
+      <c r="D53" s="117"/>
       <c r="E53" s="88" t="s">
         <v>130</v>
       </c>
@@ -5797,16 +5795,16 @@
       </c>
     </row>
     <row r="54" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A54" s="125" t="s">
+      <c r="A54" s="133" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="116" t="s">
+      <c r="B54" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="112" t="s">
+      <c r="C54" s="123" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="126"/>
+      <c r="D54" s="135"/>
       <c r="E54" s="88" t="s">
         <v>134</v>
       </c>
@@ -5834,10 +5832,10 @@
       </c>
     </row>
     <row r="55" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A55" s="125"/>
-      <c r="B55" s="116"/>
-      <c r="C55" s="112"/>
-      <c r="D55" s="126"/>
+      <c r="A55" s="133"/>
+      <c r="B55" s="117"/>
+      <c r="C55" s="123"/>
+      <c r="D55" s="135"/>
       <c r="E55" s="96" t="s">
         <v>136</v>
       </c>
@@ -5864,11 +5862,11 @@
       </c>
     </row>
     <row r="56" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A56" s="150"/>
-      <c r="B56" s="129"/>
-      <c r="C56" s="130"/>
-      <c r="D56" s="148"/>
-      <c r="E56" s="149" t="s">
+      <c r="A56" s="134"/>
+      <c r="B56" s="119"/>
+      <c r="C56" s="124"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="100" t="s">
         <v>201</v>
       </c>
       <c r="F56" s="95" t="s">
@@ -5892,11 +5890,11 @@
       </c>
     </row>
     <row r="57" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A57" s="150"/>
-      <c r="B57" s="129"/>
-      <c r="C57" s="130"/>
-      <c r="D57" s="148"/>
-      <c r="E57" s="149" t="s">
+      <c r="A57" s="134"/>
+      <c r="B57" s="119"/>
+      <c r="C57" s="124"/>
+      <c r="D57" s="136"/>
+      <c r="E57" s="100" t="s">
         <v>203</v>
       </c>
       <c r="F57" s="95" t="s">
@@ -5920,11 +5918,11 @@
       </c>
     </row>
     <row r="58" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A58" s="150"/>
-      <c r="B58" s="129"/>
-      <c r="C58" s="130"/>
-      <c r="D58" s="148"/>
-      <c r="E58" s="149" t="s">
+      <c r="A58" s="134"/>
+      <c r="B58" s="119"/>
+      <c r="C58" s="124"/>
+      <c r="D58" s="136"/>
+      <c r="E58" s="100" t="s">
         <v>204</v>
       </c>
       <c r="F58" s="96" t="s">
@@ -5951,20 +5949,20 @@
       <c r="A59" s="146" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="151" t="s">
+      <c r="B59" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="152" t="s">
+      <c r="C59" s="148" t="s">
         <v>133</v>
       </c>
-      <c r="D59" s="147"/>
+      <c r="D59" s="149"/>
       <c r="E59" s="96" t="s">
         <v>198</v>
       </c>
       <c r="F59" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="145"/>
+      <c r="G59" s="99"/>
       <c r="H59" s="50">
         <v>44043</v>
       </c>
@@ -5983,16 +5981,16 @@
     </row>
     <row r="60" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
       <c r="A60" s="146"/>
-      <c r="B60" s="151"/>
-      <c r="C60" s="152"/>
-      <c r="D60" s="147"/>
+      <c r="B60" s="147"/>
+      <c r="C60" s="148"/>
+      <c r="D60" s="149"/>
       <c r="E60" s="96" t="s">
         <v>199</v>
       </c>
       <c r="F60" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="145"/>
+      <c r="G60" s="99"/>
       <c r="H60" s="50">
         <v>44043</v>
       </c>
@@ -6011,9 +6009,9 @@
     </row>
     <row r="61" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
       <c r="A61" s="146"/>
-      <c r="B61" s="151"/>
-      <c r="C61" s="152"/>
-      <c r="D61" s="147"/>
+      <c r="B61" s="147"/>
+      <c r="C61" s="148"/>
+      <c r="D61" s="149"/>
       <c r="E61" s="96" t="s">
         <v>200</v>
       </c>
@@ -6069,16 +6067,16 @@
       </c>
     </row>
     <row r="63" spans="1:22" s="25" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A63" s="122" t="s">
+      <c r="A63" s="127" t="s">
         <v>142</v>
       </c>
-      <c r="B63" s="106" t="s">
+      <c r="B63" s="101" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="109" t="s">
+      <c r="C63" s="130" t="s">
         <v>143</v>
       </c>
-      <c r="D63" s="106"/>
+      <c r="D63" s="101"/>
       <c r="E63" s="49" t="s">
         <v>144</v>
       </c>
@@ -6106,10 +6104,10 @@
       </c>
     </row>
     <row r="64" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A64" s="123"/>
-      <c r="B64" s="107"/>
-      <c r="C64" s="110"/>
-      <c r="D64" s="107"/>
+      <c r="A64" s="128"/>
+      <c r="B64" s="102"/>
+      <c r="C64" s="131"/>
+      <c r="D64" s="102"/>
       <c r="E64" s="84" t="s">
         <v>146</v>
       </c>
@@ -6136,10 +6134,10 @@
       </c>
     </row>
     <row r="65" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A65" s="123"/>
-      <c r="B65" s="107"/>
-      <c r="C65" s="110"/>
-      <c r="D65" s="107"/>
+      <c r="A65" s="128"/>
+      <c r="B65" s="102"/>
+      <c r="C65" s="131"/>
+      <c r="D65" s="102"/>
       <c r="E65" s="94" t="s">
         <v>148</v>
       </c>
@@ -6164,10 +6162,10 @@
       </c>
     </row>
     <row r="66" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A66" s="124"/>
-      <c r="B66" s="108"/>
-      <c r="C66" s="111"/>
-      <c r="D66" s="108"/>
+      <c r="A66" s="129"/>
+      <c r="B66" s="103"/>
+      <c r="C66" s="132"/>
+      <c r="D66" s="103"/>
       <c r="E66" s="94" t="s">
         <v>205</v>
       </c>
@@ -6192,16 +6190,16 @@
       </c>
     </row>
     <row r="67" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A67" s="115" t="s">
+      <c r="A67" s="139" t="s">
         <v>149</v>
       </c>
-      <c r="B67" s="106" t="s">
+      <c r="B67" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="109" t="s">
+      <c r="C67" s="130" t="s">
         <v>150</v>
       </c>
-      <c r="D67" s="113"/>
+      <c r="D67" s="137"/>
       <c r="E67" s="61" t="s">
         <v>151</v>
       </c>
@@ -6229,10 +6227,10 @@
       </c>
     </row>
     <row r="68" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A68" s="115"/>
-      <c r="B68" s="107"/>
-      <c r="C68" s="110"/>
-      <c r="D68" s="120"/>
+      <c r="A68" s="139"/>
+      <c r="B68" s="102"/>
+      <c r="C68" s="131"/>
+      <c r="D68" s="144"/>
       <c r="E68" s="61" t="s">
         <v>154</v>
       </c>
@@ -6260,10 +6258,10 @@
       </c>
     </row>
     <row r="69" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A69" s="115"/>
-      <c r="B69" s="107"/>
-      <c r="C69" s="110"/>
-      <c r="D69" s="120"/>
+      <c r="A69" s="139"/>
+      <c r="B69" s="102"/>
+      <c r="C69" s="131"/>
+      <c r="D69" s="144"/>
       <c r="E69" s="61" t="s">
         <v>156</v>
       </c>
@@ -6287,10 +6285,10 @@
       <c r="L69" s="38"/>
     </row>
     <row r="70" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A70" s="115"/>
-      <c r="B70" s="118"/>
-      <c r="C70" s="119"/>
-      <c r="D70" s="121"/>
+      <c r="A70" s="139"/>
+      <c r="B70" s="142"/>
+      <c r="C70" s="143"/>
+      <c r="D70" s="145"/>
       <c r="E70" s="61" t="s">
         <v>202</v>
       </c>
@@ -6316,19 +6314,19 @@
       </c>
     </row>
     <row r="71" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A71" s="117" t="s">
+      <c r="A71" s="141" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="117"/>
-      <c r="C71" s="117"/>
-      <c r="D71" s="117"/>
-      <c r="E71" s="117"/>
-      <c r="F71" s="117"/>
-      <c r="G71" s="117"/>
-      <c r="H71" s="117"/>
-      <c r="I71" s="117"/>
-      <c r="J71" s="117"/>
-      <c r="K71" s="117"/>
+      <c r="B71" s="141"/>
+      <c r="C71" s="141"/>
+      <c r="D71" s="141"/>
+      <c r="E71" s="141"/>
+      <c r="F71" s="141"/>
+      <c r="G71" s="141"/>
+      <c r="H71" s="141"/>
+      <c r="I71" s="141"/>
+      <c r="J71" s="141"/>
+      <c r="K71" s="141"/>
       <c r="L71" s="57"/>
       <c r="M71" s="25"/>
       <c r="N71" s="25"/>
@@ -6966,19 +6964,19 @@
       <c r="V90" s="25"/>
     </row>
     <row r="91" spans="1:22" ht="25.5" customHeight="1">
-      <c r="A91" s="102" t="s">
+      <c r="A91" s="140" t="s">
         <v>179</v>
       </c>
-      <c r="B91" s="102"/>
-      <c r="C91" s="102"/>
-      <c r="D91" s="102"/>
-      <c r="E91" s="102"/>
-      <c r="F91" s="102"/>
-      <c r="G91" s="102"/>
-      <c r="H91" s="102"/>
-      <c r="I91" s="102"/>
-      <c r="J91" s="102"/>
-      <c r="K91" s="102"/>
+      <c r="B91" s="140"/>
+      <c r="C91" s="140"/>
+      <c r="D91" s="140"/>
+      <c r="E91" s="140"/>
+      <c r="F91" s="140"/>
+      <c r="G91" s="140"/>
+      <c r="H91" s="140"/>
+      <c r="I91" s="140"/>
+      <c r="J91" s="140"/>
+      <c r="K91" s="140"/>
       <c r="L91" s="38"/>
       <c r="M91" s="25"/>
       <c r="N91" s="25"/>
@@ -7157,14 +7155,60 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="A47:K47"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A71:K71"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
     <mergeCell ref="L28:L30"/>
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="H28:H30"/>
@@ -7181,95 +7225,49 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="D54:D58"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A71:K71"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="A47:K47"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G20" r:id="rId1"/>
-    <hyperlink ref="G21" r:id="rId2"/>
-    <hyperlink ref="G34" r:id="rId3"/>
-    <hyperlink ref="G23" r:id="rId4"/>
-    <hyperlink ref="G12" r:id="rId5"/>
-    <hyperlink ref="G24" r:id="rId6"/>
-    <hyperlink ref="G39" r:id="rId7"/>
-    <hyperlink ref="G30" r:id="rId8"/>
-    <hyperlink ref="G33" r:id="rId9"/>
-    <hyperlink ref="G43" r:id="rId10"/>
-    <hyperlink ref="G25" r:id="rId11"/>
-    <hyperlink ref="G41" r:id="rId12"/>
-    <hyperlink ref="G44" r:id="rId13"/>
-    <hyperlink ref="G32" r:id="rId14"/>
-    <hyperlink ref="G40" r:id="rId15"/>
-    <hyperlink ref="G26:G27" r:id="rId16" display="https://github.com/antonyMontalvo/FaceSolutions/commit/8f0ec13380b96dbff2cf0f44e517515e6d8e935b"/>
-    <hyperlink ref="G63" r:id="rId17"/>
-    <hyperlink ref="G51" r:id="rId18"/>
-    <hyperlink ref="G36" r:id="rId19"/>
-    <hyperlink ref="G28:G29" r:id="rId20" display="https://github.com/antonyMontalvo/FaceSolutions/commit/b7f87017c045c76f3ed7353bf35a7680607f9adf"/>
-    <hyperlink ref="G42" r:id="rId21"/>
-    <hyperlink ref="G37" r:id="rId22"/>
-    <hyperlink ref="G50" r:id="rId23"/>
-    <hyperlink ref="G31" r:id="rId24"/>
-    <hyperlink ref="G67" r:id="rId25"/>
-    <hyperlink ref="G19" r:id="rId26"/>
-    <hyperlink ref="G35" r:id="rId27"/>
-    <hyperlink ref="G54" r:id="rId28"/>
-    <hyperlink ref="G53" r:id="rId29"/>
-    <hyperlink ref="G68" r:id="rId30"/>
-    <hyperlink ref="G64" r:id="rId31"/>
-    <hyperlink ref="G55" r:id="rId32"/>
-    <hyperlink ref="G69" r:id="rId33"/>
+    <hyperlink ref="G20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G23" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G39" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G30" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G43" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G25" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G41" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G44" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G32" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G26:G27" r:id="rId16" display="https://github.com/antonyMontalvo/FaceSolutions/commit/8f0ec13380b96dbff2cf0f44e517515e6d8e935b" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G63" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G51" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G36" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G28:G29" r:id="rId20" display="https://github.com/antonyMontalvo/FaceSolutions/commit/b7f87017c045c76f3ed7353bf35a7680607f9adf" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G42" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G37" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G50" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G31" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G67" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G19" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G35" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G54" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G53" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G68" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G64" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G55" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G69" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId34"/>
@@ -7278,7 +7276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Funcionalidad boton grabar - Modulo Administrador
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antony\Desktop\Repo\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB46D06-53DD-4AF9-B9B5-444DF031061A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C4E643-8464-4109-98AB-C1DCF495E974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="206">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -1368,6 +1368,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1377,6 +1398,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1388,141 +1523,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4004,18 +4004,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="34.875" customWidth="1"/>
-    <col min="3" max="3" width="34" style="25" customWidth="1"/>
+    <col min="3" max="3" width="33.5" style="25" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="35.875" style="25" customWidth="1"/>
     <col min="5" max="5" width="51.875" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="35.875" style="25" customWidth="1"/>
+    <col min="6" max="7" width="35.875" style="25" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="10.75" customWidth="1"/>
@@ -4028,21 +4028,21 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
-      <c r="K2" s="150"/>
-      <c r="L2" s="150"/>
-      <c r="M2" s="150"/>
-      <c r="N2" s="150"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
@@ -4056,15 +4056,15 @@
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -4084,15 +4084,15 @@
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="151"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
-      <c r="G4" s="151"/>
-      <c r="H4" s="151"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -4112,15 +4112,15 @@
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="152" t="s">
+      <c r="B5" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -4370,7 +4370,7 @@
       <c r="C13" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="112"/>
+      <c r="D13" s="143"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26" t="s">
         <v>26</v>
@@ -4406,16 +4406,16 @@
       <c r="V13" s="25"/>
     </row>
     <row r="14" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="123" t="s">
+      <c r="C14" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="113"/>
+      <c r="D14" s="144"/>
       <c r="E14" s="90" t="s">
         <v>31</v>
       </c>
@@ -4443,10 +4443,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A15" s="122"/>
-      <c r="B15" s="119"/>
-      <c r="C15" s="124"/>
-      <c r="D15" s="113"/>
+      <c r="A15" s="138"/>
+      <c r="B15" s="133"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="144"/>
       <c r="E15" s="90" t="s">
         <v>31</v>
       </c>
@@ -4483,7 +4483,7 @@
       <c r="C16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="113"/>
+      <c r="D16" s="144"/>
       <c r="E16" s="43" t="s">
         <v>34</v>
       </c>
@@ -4519,7 +4519,7 @@
       <c r="C17" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="114"/>
+      <c r="D17" s="145"/>
       <c r="E17" s="44" t="s">
         <v>36</v>
       </c>
@@ -4550,12 +4550,12 @@
       <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="105"/>
-      <c r="C18" s="106"/>
-      <c r="D18" s="106"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
-      <c r="G18" s="107"/>
+      <c r="B18" s="150"/>
+      <c r="C18" s="151"/>
+      <c r="D18" s="151"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="151"/>
+      <c r="G18" s="152"/>
       <c r="H18" s="27">
         <v>44008</v>
       </c>
@@ -4585,16 +4585,16 @@
       <c r="V18" s="25"/>
     </row>
     <row r="19" spans="1:22" s="25" customFormat="1" ht="36" customHeight="1">
-      <c r="A19" s="108" t="s">
+      <c r="A19" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="101" t="s">
+      <c r="B19" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="130" t="s">
+      <c r="C19" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="101" t="s">
+      <c r="D19" s="108" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="89" t="s">
@@ -4623,10 +4623,10 @@
       </c>
     </row>
     <row r="20" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="109"/>
-      <c r="B20" s="102"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="102"/>
+      <c r="A20" s="106"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="109"/>
       <c r="E20" s="61" t="s">
         <v>44</v>
       </c>
@@ -4653,10 +4653,10 @@
       </c>
     </row>
     <row r="21" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A21" s="110"/>
-      <c r="B21" s="103"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="103"/>
+      <c r="A21" s="107"/>
+      <c r="B21" s="110"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="110"/>
       <c r="E21" s="49" t="s">
         <v>46</v>
       </c>
@@ -4732,16 +4732,16 @@
       <c r="V22" s="25"/>
     </row>
     <row r="23" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A23" s="108" t="s">
+      <c r="A23" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="123" t="s">
+      <c r="B23" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="101" t="s">
+      <c r="D23" s="108" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="61" t="s">
@@ -4771,10 +4771,10 @@
       </c>
     </row>
     <row r="24" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A24" s="109"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="102"/>
+      <c r="A24" s="106"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="109"/>
       <c r="E24" s="89" t="s">
         <v>56</v>
       </c>
@@ -4802,10 +4802,10 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="52.5" customHeight="1">
-      <c r="A25" s="109"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="102"/>
+      <c r="A25" s="106"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="114"/>
+      <c r="D25" s="109"/>
       <c r="E25" s="84" t="s">
         <v>36</v>
       </c>
@@ -4843,61 +4843,61 @@
       <c r="V25" s="25"/>
     </row>
     <row r="26" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A26" s="125" t="s">
+      <c r="A26" s="139" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="117" t="s">
+      <c r="B26" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="117" t="s">
+      <c r="C26" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="119" t="s">
+      <c r="D26" s="133" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="117" t="s">
+      <c r="F26" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="104" t="s">
+      <c r="G26" s="149" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="116">
+      <c r="H26" s="147">
         <v>44012</v>
       </c>
-      <c r="I26" s="116">
+      <c r="I26" s="147">
         <v>44013</v>
       </c>
-      <c r="J26" s="119">
+      <c r="J26" s="133">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K26" s="118" t="s">
+      <c r="K26" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="111">
+      <c r="L26" s="142">
         <v>1</v>
       </c>
       <c r="M26" s="67"/>
       <c r="N26" s="48"/>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
-      <c r="A27" s="126"/>
-      <c r="B27" s="117"/>
-      <c r="C27" s="117"/>
-      <c r="D27" s="120"/>
+      <c r="A27" s="140"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="141"/>
       <c r="E27" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="117"/>
-      <c r="G27" s="104"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="120"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="111"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="149"/>
+      <c r="H27" s="147"/>
+      <c r="I27" s="147"/>
+      <c r="J27" s="141"/>
+      <c r="K27" s="148"/>
+      <c r="L27" s="142"/>
       <c r="M27" s="67"/>
       <c r="N27" s="48"/>
       <c r="O27" s="25"/>
@@ -4910,16 +4910,16 @@
       <c r="V27" s="25"/>
     </row>
     <row r="28" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="108" t="s">
+      <c r="A28" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="117" t="s">
+      <c r="C28" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="117" t="s">
+      <c r="D28" s="118" t="s">
         <v>66</v>
       </c>
       <c r="E28" s="90" t="s">
@@ -4928,51 +4928,51 @@
       <c r="F28" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="104" t="s">
+      <c r="G28" s="149" t="s">
         <v>68</v>
       </c>
-      <c r="H28" s="115">
+      <c r="H28" s="146">
         <v>44010</v>
       </c>
-      <c r="I28" s="116">
+      <c r="I28" s="147">
         <v>44013</v>
       </c>
-      <c r="J28" s="117">
+      <c r="J28" s="118">
         <f>I28-H28</f>
         <v>3</v>
       </c>
-      <c r="K28" s="118" t="s">
+      <c r="K28" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="111">
+      <c r="L28" s="142">
         <v>1</v>
       </c>
       <c r="N28" s="48"/>
     </row>
     <row r="29" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="109"/>
-      <c r="B29" s="117"/>
-      <c r="C29" s="117"/>
-      <c r="D29" s="117"/>
+      <c r="A29" s="106"/>
+      <c r="B29" s="118"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="118"/>
       <c r="E29" s="92" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="104"/>
-      <c r="H29" s="115"/>
-      <c r="I29" s="116"/>
-      <c r="J29" s="117"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="111"/>
+      <c r="G29" s="149"/>
+      <c r="H29" s="146"/>
+      <c r="I29" s="147"/>
+      <c r="J29" s="118"/>
+      <c r="K29" s="148"/>
+      <c r="L29" s="142"/>
       <c r="N29" s="48"/>
     </row>
     <row r="30" spans="1:22" ht="30" customHeight="1">
-      <c r="A30" s="110"/>
-      <c r="B30" s="117"/>
-      <c r="C30" s="117"/>
-      <c r="D30" s="117"/>
+      <c r="A30" s="107"/>
+      <c r="B30" s="118"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="118"/>
       <c r="E30" s="26" t="s">
         <v>70</v>
       </c>
@@ -4982,11 +4982,11 @@
       <c r="G30" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="115"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="117"/>
-      <c r="K30" s="118"/>
-      <c r="L30" s="111"/>
+      <c r="H30" s="146"/>
+      <c r="I30" s="147"/>
+      <c r="J30" s="118"/>
+      <c r="K30" s="148"/>
+      <c r="L30" s="142"/>
       <c r="M30" s="25"/>
       <c r="N30" s="48"/>
       <c r="O30" s="25"/>
@@ -4999,16 +4999,16 @@
       <c r="V30" s="25"/>
     </row>
     <row r="31" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A31" s="108" t="s">
+      <c r="A31" s="105" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="108" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="130" t="s">
+      <c r="C31" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="101" t="s">
+      <c r="D31" s="108" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="56" t="s">
@@ -5038,10 +5038,10 @@
       </c>
     </row>
     <row r="32" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A32" s="109"/>
-      <c r="B32" s="102"/>
-      <c r="C32" s="131"/>
-      <c r="D32" s="102"/>
+      <c r="A32" s="106"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="112"/>
+      <c r="D32" s="109"/>
       <c r="E32" s="44" t="s">
         <v>78</v>
       </c>
@@ -5068,10 +5068,10 @@
       </c>
     </row>
     <row r="33" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A33" s="109"/>
-      <c r="B33" s="102"/>
-      <c r="C33" s="131"/>
-      <c r="D33" s="102"/>
+      <c r="A33" s="106"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="112"/>
+      <c r="D33" s="109"/>
       <c r="E33" s="44" t="s">
         <v>80</v>
       </c>
@@ -5099,10 +5099,10 @@
       </c>
     </row>
     <row r="34" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A34" s="109"/>
-      <c r="B34" s="102"/>
-      <c r="C34" s="131"/>
-      <c r="D34" s="102"/>
+      <c r="A34" s="106"/>
+      <c r="B34" s="109"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="109"/>
       <c r="E34" s="44" t="s">
         <v>82</v>
       </c>
@@ -5130,10 +5130,10 @@
       </c>
     </row>
     <row r="35" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A35" s="109"/>
-      <c r="B35" s="102"/>
-      <c r="C35" s="131"/>
-      <c r="D35" s="102"/>
+      <c r="A35" s="106"/>
+      <c r="B35" s="109"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="109"/>
       <c r="E35" s="44" t="s">
         <v>84</v>
       </c>
@@ -5161,10 +5161,10 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="33" customHeight="1">
-      <c r="A36" s="110"/>
-      <c r="B36" s="103"/>
-      <c r="C36" s="132"/>
-      <c r="D36" s="103"/>
+      <c r="A36" s="107"/>
+      <c r="B36" s="110"/>
+      <c r="C36" s="113"/>
+      <c r="D36" s="110"/>
       <c r="E36" s="44" t="s">
         <v>86</v>
       </c>
@@ -5243,12 +5243,12 @@
       <c r="A38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="105"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="107"/>
+      <c r="B38" s="150"/>
+      <c r="C38" s="151"/>
+      <c r="D38" s="151"/>
+      <c r="E38" s="151"/>
+      <c r="F38" s="151"/>
+      <c r="G38" s="152"/>
       <c r="H38" s="27">
         <v>43837</v>
       </c>
@@ -5277,14 +5277,14 @@
       <c r="V38" s="25"/>
     </row>
     <row r="39" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A39" s="101" t="s">
+      <c r="A39" s="108" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="101" t="s">
+      <c r="B39" s="108" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101" t="s">
+      <c r="C39" s="108"/>
+      <c r="D39" s="108" t="s">
         <v>96</v>
       </c>
       <c r="E39" s="63" t="s">
@@ -5314,10 +5314,10 @@
       <c r="N39" s="48"/>
     </row>
     <row r="40" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A40" s="102"/>
-      <c r="B40" s="102"/>
-      <c r="C40" s="102"/>
-      <c r="D40" s="102"/>
+      <c r="A40" s="109"/>
+      <c r="B40" s="109"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="109"/>
       <c r="E40" s="49" t="s">
         <v>100</v>
       </c>
@@ -5345,10 +5345,10 @@
       <c r="N40" s="48"/>
     </row>
     <row r="41" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A41" s="102"/>
-      <c r="B41" s="102"/>
-      <c r="C41" s="102"/>
-      <c r="D41" s="102"/>
+      <c r="A41" s="109"/>
+      <c r="B41" s="109"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
       <c r="E41" s="49" t="s">
         <v>102</v>
       </c>
@@ -5376,10 +5376,10 @@
       <c r="N41" s="48"/>
     </row>
     <row r="42" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A42" s="102"/>
-      <c r="B42" s="102"/>
-      <c r="C42" s="102"/>
-      <c r="D42" s="102"/>
+      <c r="A42" s="109"/>
+      <c r="B42" s="109"/>
+      <c r="C42" s="109"/>
+      <c r="D42" s="109"/>
       <c r="E42" s="63" t="s">
         <v>104</v>
       </c>
@@ -5407,10 +5407,10 @@
       <c r="N42" s="48"/>
     </row>
     <row r="43" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A43" s="103"/>
-      <c r="B43" s="103"/>
-      <c r="C43" s="103"/>
-      <c r="D43" s="103"/>
+      <c r="A43" s="110"/>
+      <c r="B43" s="110"/>
+      <c r="C43" s="110"/>
+      <c r="D43" s="110"/>
       <c r="E43" s="43" t="s">
         <v>106</v>
       </c>
@@ -5487,16 +5487,16 @@
       <c r="V44" s="25"/>
     </row>
     <row r="45" spans="1:22" s="25" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A45" s="108" t="s">
+      <c r="A45" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="101" t="s">
+      <c r="B45" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="130" t="s">
+      <c r="C45" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="108" t="s">
+      <c r="D45" s="105" t="s">
         <v>27</v>
       </c>
       <c r="E45" s="43" t="s">
@@ -5526,10 +5526,10 @@
       <c r="N45" s="48"/>
     </row>
     <row r="46" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A46" s="110"/>
-      <c r="B46" s="103"/>
-      <c r="C46" s="132"/>
-      <c r="D46" s="110"/>
+      <c r="A46" s="107"/>
+      <c r="B46" s="110"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="107"/>
       <c r="E46" s="90" t="s">
         <v>117</v>
       </c>
@@ -5567,19 +5567,19 @@
       <c r="V46" s="25"/>
     </row>
     <row r="47" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A47" s="140" t="s">
+      <c r="A47" s="104" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="140"/>
-      <c r="C47" s="140"/>
-      <c r="D47" s="140"/>
-      <c r="E47" s="140"/>
-      <c r="F47" s="140"/>
-      <c r="G47" s="140"/>
-      <c r="H47" s="140"/>
-      <c r="I47" s="140"/>
-      <c r="J47" s="140"/>
-      <c r="K47" s="140"/>
+      <c r="B47" s="104"/>
+      <c r="C47" s="104"/>
+      <c r="D47" s="104"/>
+      <c r="E47" s="104"/>
+      <c r="F47" s="104"/>
+      <c r="G47" s="104"/>
+      <c r="H47" s="104"/>
+      <c r="I47" s="104"/>
+      <c r="J47" s="104"/>
+      <c r="K47" s="104"/>
       <c r="L47" s="38"/>
       <c r="M47" s="25"/>
       <c r="N47" s="25"/>
@@ -5649,16 +5649,16 @@
       </c>
     </row>
     <row r="50" spans="1:22" ht="38.25" customHeight="1">
-      <c r="A50" s="133" t="s">
+      <c r="A50" s="131" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="117" t="s">
+      <c r="B50" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="130" t="s">
+      <c r="C50" s="111" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="137"/>
+      <c r="D50" s="115"/>
       <c r="E50" s="44" t="s">
         <v>124</v>
       </c>
@@ -5696,10 +5696,10 @@
       <c r="V50" s="25"/>
     </row>
     <row r="51" spans="1:22" s="25" customFormat="1" ht="45" customHeight="1">
-      <c r="A51" s="133"/>
-      <c r="B51" s="117"/>
-      <c r="C51" s="132"/>
-      <c r="D51" s="138"/>
+      <c r="A51" s="131"/>
+      <c r="B51" s="118"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="116"/>
       <c r="E51" s="49" t="s">
         <v>126</v>
       </c>
@@ -5727,16 +5727,16 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A52" s="139" t="s">
+      <c r="A52" s="117" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="117" t="s">
+      <c r="B52" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="123" t="s">
+      <c r="C52" s="114" t="s">
         <v>123</v>
       </c>
-      <c r="D52" s="117"/>
+      <c r="D52" s="118"/>
       <c r="E52" s="88" t="s">
         <v>129</v>
       </c>
@@ -5764,10 +5764,10 @@
       </c>
     </row>
     <row r="53" spans="1:22" s="25" customFormat="1" ht="57" customHeight="1">
-      <c r="A53" s="139"/>
-      <c r="B53" s="117"/>
-      <c r="C53" s="123"/>
-      <c r="D53" s="117"/>
+      <c r="A53" s="117"/>
+      <c r="B53" s="118"/>
+      <c r="C53" s="114"/>
+      <c r="D53" s="118"/>
       <c r="E53" s="88" t="s">
         <v>130</v>
       </c>
@@ -5795,13 +5795,13 @@
       </c>
     </row>
     <row r="54" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A54" s="133" t="s">
+      <c r="A54" s="131" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="117" t="s">
+      <c r="B54" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="123" t="s">
+      <c r="C54" s="114" t="s">
         <v>133</v>
       </c>
       <c r="D54" s="135"/>
@@ -5832,9 +5832,9 @@
       </c>
     </row>
     <row r="55" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A55" s="133"/>
-      <c r="B55" s="117"/>
-      <c r="C55" s="123"/>
+      <c r="A55" s="131"/>
+      <c r="B55" s="118"/>
+      <c r="C55" s="114"/>
       <c r="D55" s="135"/>
       <c r="E55" s="96" t="s">
         <v>136</v>
@@ -5862,9 +5862,9 @@
       </c>
     </row>
     <row r="56" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A56" s="134"/>
-      <c r="B56" s="119"/>
-      <c r="C56" s="124"/>
+      <c r="A56" s="132"/>
+      <c r="B56" s="133"/>
+      <c r="C56" s="134"/>
       <c r="D56" s="136"/>
       <c r="E56" s="100" t="s">
         <v>201</v>
@@ -5890,9 +5890,9 @@
       </c>
     </row>
     <row r="57" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A57" s="134"/>
-      <c r="B57" s="119"/>
-      <c r="C57" s="124"/>
+      <c r="A57" s="132"/>
+      <c r="B57" s="133"/>
+      <c r="C57" s="134"/>
       <c r="D57" s="136"/>
       <c r="E57" s="100" t="s">
         <v>203</v>
@@ -5918,9 +5918,9 @@
       </c>
     </row>
     <row r="58" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A58" s="134"/>
-      <c r="B58" s="119"/>
-      <c r="C58" s="124"/>
+      <c r="A58" s="132"/>
+      <c r="B58" s="133"/>
+      <c r="C58" s="134"/>
       <c r="D58" s="136"/>
       <c r="E58" s="100" t="s">
         <v>204</v>
@@ -5946,16 +5946,16 @@
       </c>
     </row>
     <row r="59" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A59" s="146" t="s">
+      <c r="A59" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="147" t="s">
+      <c r="B59" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="148" t="s">
+      <c r="C59" s="126" t="s">
         <v>133</v>
       </c>
-      <c r="D59" s="149"/>
+      <c r="D59" s="127"/>
       <c r="E59" s="96" t="s">
         <v>198</v>
       </c>
@@ -5980,10 +5980,10 @@
       </c>
     </row>
     <row r="60" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A60" s="146"/>
-      <c r="B60" s="147"/>
-      <c r="C60" s="148"/>
-      <c r="D60" s="149"/>
+      <c r="A60" s="124"/>
+      <c r="B60" s="125"/>
+      <c r="C60" s="126"/>
+      <c r="D60" s="127"/>
       <c r="E60" s="96" t="s">
         <v>199</v>
       </c>
@@ -6008,10 +6008,10 @@
       </c>
     </row>
     <row r="61" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A61" s="146"/>
-      <c r="B61" s="147"/>
-      <c r="C61" s="148"/>
-      <c r="D61" s="149"/>
+      <c r="A61" s="124"/>
+      <c r="B61" s="125"/>
+      <c r="C61" s="126"/>
+      <c r="D61" s="127"/>
       <c r="E61" s="96" t="s">
         <v>200</v>
       </c>
@@ -6067,16 +6067,16 @@
       </c>
     </row>
     <row r="63" spans="1:22" s="25" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A63" s="127" t="s">
+      <c r="A63" s="128" t="s">
         <v>142</v>
       </c>
-      <c r="B63" s="101" t="s">
+      <c r="B63" s="108" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="130" t="s">
+      <c r="C63" s="111" t="s">
         <v>143</v>
       </c>
-      <c r="D63" s="101"/>
+      <c r="D63" s="108"/>
       <c r="E63" s="49" t="s">
         <v>144</v>
       </c>
@@ -6104,10 +6104,10 @@
       </c>
     </row>
     <row r="64" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A64" s="128"/>
-      <c r="B64" s="102"/>
-      <c r="C64" s="131"/>
-      <c r="D64" s="102"/>
+      <c r="A64" s="129"/>
+      <c r="B64" s="109"/>
+      <c r="C64" s="112"/>
+      <c r="D64" s="109"/>
       <c r="E64" s="84" t="s">
         <v>146</v>
       </c>
@@ -6134,10 +6134,10 @@
       </c>
     </row>
     <row r="65" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A65" s="128"/>
-      <c r="B65" s="102"/>
-      <c r="C65" s="131"/>
-      <c r="D65" s="102"/>
+      <c r="A65" s="129"/>
+      <c r="B65" s="109"/>
+      <c r="C65" s="112"/>
+      <c r="D65" s="109"/>
       <c r="E65" s="94" t="s">
         <v>148</v>
       </c>
@@ -6162,10 +6162,10 @@
       </c>
     </row>
     <row r="66" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A66" s="129"/>
-      <c r="B66" s="103"/>
-      <c r="C66" s="132"/>
-      <c r="D66" s="103"/>
+      <c r="A66" s="130"/>
+      <c r="B66" s="110"/>
+      <c r="C66" s="113"/>
+      <c r="D66" s="110"/>
       <c r="E66" s="94" t="s">
         <v>205</v>
       </c>
@@ -6190,16 +6190,16 @@
       </c>
     </row>
     <row r="67" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A67" s="139" t="s">
+      <c r="A67" s="117" t="s">
         <v>149</v>
       </c>
-      <c r="B67" s="101" t="s">
+      <c r="B67" s="108" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="130" t="s">
+      <c r="C67" s="111" t="s">
         <v>150</v>
       </c>
-      <c r="D67" s="137"/>
+      <c r="D67" s="115"/>
       <c r="E67" s="61" t="s">
         <v>151</v>
       </c>
@@ -6227,10 +6227,10 @@
       </c>
     </row>
     <row r="68" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A68" s="139"/>
-      <c r="B68" s="102"/>
-      <c r="C68" s="131"/>
-      <c r="D68" s="144"/>
+      <c r="A68" s="117"/>
+      <c r="B68" s="109"/>
+      <c r="C68" s="112"/>
+      <c r="D68" s="122"/>
       <c r="E68" s="61" t="s">
         <v>154</v>
       </c>
@@ -6258,10 +6258,10 @@
       </c>
     </row>
     <row r="69" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A69" s="139"/>
-      <c r="B69" s="102"/>
-      <c r="C69" s="131"/>
-      <c r="D69" s="144"/>
+      <c r="A69" s="117"/>
+      <c r="B69" s="109"/>
+      <c r="C69" s="112"/>
+      <c r="D69" s="122"/>
       <c r="E69" s="61" t="s">
         <v>156</v>
       </c>
@@ -6281,14 +6281,16 @@
         <f>I69-H69</f>
         <v>25</v>
       </c>
-      <c r="K69" s="58"/>
+      <c r="K69" s="60" t="s">
+        <v>139</v>
+      </c>
       <c r="L69" s="38"/>
     </row>
     <row r="70" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A70" s="139"/>
-      <c r="B70" s="142"/>
-      <c r="C70" s="143"/>
-      <c r="D70" s="145"/>
+      <c r="A70" s="117"/>
+      <c r="B70" s="120"/>
+      <c r="C70" s="121"/>
+      <c r="D70" s="123"/>
       <c r="E70" s="61" t="s">
         <v>202</v>
       </c>
@@ -6314,19 +6316,19 @@
       </c>
     </row>
     <row r="71" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A71" s="141" t="s">
+      <c r="A71" s="119" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="141"/>
-      <c r="C71" s="141"/>
-      <c r="D71" s="141"/>
-      <c r="E71" s="141"/>
-      <c r="F71" s="141"/>
-      <c r="G71" s="141"/>
-      <c r="H71" s="141"/>
-      <c r="I71" s="141"/>
-      <c r="J71" s="141"/>
-      <c r="K71" s="141"/>
+      <c r="B71" s="119"/>
+      <c r="C71" s="119"/>
+      <c r="D71" s="119"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="119"/>
+      <c r="G71" s="119"/>
+      <c r="H71" s="119"/>
+      <c r="I71" s="119"/>
+      <c r="J71" s="119"/>
+      <c r="K71" s="119"/>
       <c r="L71" s="57"/>
       <c r="M71" s="25"/>
       <c r="N71" s="25"/>
@@ -6964,19 +6966,19 @@
       <c r="V90" s="25"/>
     </row>
     <row r="91" spans="1:22" ht="25.5" customHeight="1">
-      <c r="A91" s="140" t="s">
+      <c r="A91" s="104" t="s">
         <v>179</v>
       </c>
-      <c r="B91" s="140"/>
-      <c r="C91" s="140"/>
-      <c r="D91" s="140"/>
-      <c r="E91" s="140"/>
-      <c r="F91" s="140"/>
-      <c r="G91" s="140"/>
-      <c r="H91" s="140"/>
-      <c r="I91" s="140"/>
-      <c r="J91" s="140"/>
-      <c r="K91" s="140"/>
+      <c r="B91" s="104"/>
+      <c r="C91" s="104"/>
+      <c r="D91" s="104"/>
+      <c r="E91" s="104"/>
+      <c r="F91" s="104"/>
+      <c r="G91" s="104"/>
+      <c r="H91" s="104"/>
+      <c r="I91" s="104"/>
+      <c r="J91" s="104"/>
+      <c r="K91" s="104"/>
       <c r="L91" s="38"/>
       <c r="M91" s="25"/>
       <c r="N91" s="25"/>
@@ -7155,6 +7157,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A71:K71"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D59:D61"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
@@ -7171,68 +7235,6 @@
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="C31:C36"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A71:K71"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="D54:D58"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
fix: Actualizacion de Cronograma
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antony\Desktop\Repo\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049A7D34-2BE9-44DA-B95F-F2BE16599BB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de proyecto y Gantt" sheetId="1" r:id="rId1"/>
     <sheet name="Línea base de costo" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -677,7 +676,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;S/&quot;\ #,##0.00;[Red]&quot;S/&quot;\ \-#,##0.00"/>
   </numFmts>
@@ -1110,7 +1109,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1247,9 +1246,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1368,6 +1364,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1377,6 +1394,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1388,141 +1519,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1531,7 +1527,7 @@
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Hyperlink" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4001,11 +3997,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4028,21 +4024,21 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
-      <c r="K2" s="150"/>
-      <c r="L2" s="150"/>
-      <c r="M2" s="150"/>
-      <c r="N2" s="150"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
@@ -4056,15 +4052,15 @@
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -4084,15 +4080,15 @@
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="151"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
-      <c r="G4" s="151"/>
-      <c r="H4" s="151"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -4112,15 +4108,15 @@
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="152" t="s">
+      <c r="B5" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -4329,7 +4325,7 @@
       </c>
       <c r="E12" s="49"/>
       <c r="F12" s="49"/>
-      <c r="G12" s="68" t="s">
+      <c r="G12" s="67" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="27">
@@ -4370,7 +4366,7 @@
       <c r="C13" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="112"/>
+      <c r="D13" s="142"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26" t="s">
         <v>26</v>
@@ -4406,23 +4402,23 @@
       <c r="V13" s="25"/>
     </row>
     <row r="14" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="136" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="123" t="s">
+      <c r="C14" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="113"/>
-      <c r="E14" s="90" t="s">
+      <c r="D14" s="143"/>
+      <c r="E14" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="87" t="s">
+      <c r="F14" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="87" t="s">
+      <c r="G14" s="86" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="50">
@@ -4431,11 +4427,11 @@
       <c r="I14" s="50">
         <v>44008</v>
       </c>
-      <c r="J14" s="90">
+      <c r="J14" s="89">
         <f>I14-H14</f>
         <v>2</v>
       </c>
-      <c r="K14" s="65" t="s">
+      <c r="K14" s="64" t="s">
         <v>24</v>
       </c>
       <c r="L14" s="51">
@@ -4443,17 +4439,17 @@
       </c>
     </row>
     <row r="15" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A15" s="122"/>
-      <c r="B15" s="119"/>
-      <c r="C15" s="124"/>
-      <c r="D15" s="113"/>
-      <c r="E15" s="90" t="s">
+      <c r="A15" s="137"/>
+      <c r="B15" s="132"/>
+      <c r="C15" s="133"/>
+      <c r="D15" s="143"/>
+      <c r="E15" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="87" t="s">
+      <c r="F15" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="90" t="s">
+      <c r="G15" s="89" t="s">
         <v>27</v>
       </c>
       <c r="H15" s="50">
@@ -4462,11 +4458,11 @@
       <c r="I15" s="50">
         <v>44008</v>
       </c>
-      <c r="J15" s="90">
+      <c r="J15" s="89">
         <f>I15-H15</f>
         <v>1</v>
       </c>
-      <c r="K15" s="65" t="s">
+      <c r="K15" s="64" t="s">
         <v>24</v>
       </c>
       <c r="L15" s="51">
@@ -4483,7 +4479,7 @@
       <c r="C16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="113"/>
+      <c r="D16" s="143"/>
       <c r="E16" s="43" t="s">
         <v>34</v>
       </c>
@@ -4502,7 +4498,7 @@
       <c r="J16" s="26">
         <v>1</v>
       </c>
-      <c r="K16" s="62" t="s">
+      <c r="K16" s="61" t="s">
         <v>24</v>
       </c>
       <c r="L16" s="38">
@@ -4519,7 +4515,7 @@
       <c r="C17" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="114"/>
+      <c r="D17" s="144"/>
       <c r="E17" s="44" t="s">
         <v>36</v>
       </c>
@@ -4539,7 +4535,7 @@
         <f>I17-H17</f>
         <v>6</v>
       </c>
-      <c r="K17" s="62" t="s">
+      <c r="K17" s="61" t="s">
         <v>24</v>
       </c>
       <c r="L17" s="38">
@@ -4550,12 +4546,12 @@
       <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="105"/>
-      <c r="C18" s="106"/>
-      <c r="D18" s="106"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
-      <c r="G18" s="107"/>
+      <c r="B18" s="149"/>
+      <c r="C18" s="150"/>
+      <c r="D18" s="150"/>
+      <c r="E18" s="150"/>
+      <c r="F18" s="150"/>
+      <c r="G18" s="151"/>
       <c r="H18" s="27">
         <v>44008</v>
       </c>
@@ -4585,25 +4581,25 @@
       <c r="V18" s="25"/>
     </row>
     <row r="19" spans="1:22" s="25" customFormat="1" ht="36" customHeight="1">
-      <c r="A19" s="108" t="s">
+      <c r="A19" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="101" t="s">
+      <c r="B19" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="130" t="s">
+      <c r="C19" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="101" t="s">
+      <c r="D19" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="89" t="s">
+      <c r="E19" s="88" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="81" t="s">
+      <c r="G19" s="80" t="s">
         <v>43</v>
       </c>
       <c r="H19" s="45">
@@ -4623,17 +4619,17 @@
       </c>
     </row>
     <row r="20" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="109"/>
-      <c r="B20" s="102"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="61" t="s">
+      <c r="A20" s="105"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="111"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="87" t="s">
+      <c r="F20" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="65" t="s">
         <v>45</v>
       </c>
       <c r="H20" s="45">
@@ -4653,17 +4649,17 @@
       </c>
     </row>
     <row r="21" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A21" s="110"/>
-      <c r="B21" s="103"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="103"/>
+      <c r="A21" s="106"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="109"/>
       <c r="E21" s="49" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="68" t="s">
+      <c r="G21" s="67" t="s">
         <v>48</v>
       </c>
       <c r="H21" s="45">
@@ -4732,25 +4728,25 @@
       <c r="V22" s="25"/>
     </row>
     <row r="23" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A23" s="108" t="s">
+      <c r="A23" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="123" t="s">
+      <c r="B23" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="101" t="s">
+      <c r="D23" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="60" t="s">
         <v>54</v>
       </c>
       <c r="F23" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="68" t="s">
+      <c r="G23" s="67" t="s">
         <v>55</v>
       </c>
       <c r="H23" s="27">
@@ -4771,17 +4767,17 @@
       </c>
     </row>
     <row r="24" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A24" s="109"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="102"/>
-      <c r="E24" s="89" t="s">
+      <c r="A24" s="105"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="113"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="88" t="s">
         <v>56</v>
       </c>
       <c r="F24" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="67" t="s">
         <v>57</v>
       </c>
       <c r="H24" s="27">
@@ -4802,17 +4798,17 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="52.5" customHeight="1">
-      <c r="A25" s="109"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="102"/>
-      <c r="E25" s="84" t="s">
+      <c r="A25" s="105"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="84" t="s">
+      <c r="F25" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="73" t="s">
+      <c r="G25" s="72" t="s">
         <v>58</v>
       </c>
       <c r="H25" s="52">
@@ -4821,7 +4817,7 @@
       <c r="I25" s="52">
         <v>44013</v>
       </c>
-      <c r="J25" s="91">
+      <c r="J25" s="90">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -4843,7 +4839,7 @@
       <c r="V25" s="25"/>
     </row>
     <row r="26" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A26" s="125" t="s">
+      <c r="A26" s="138" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="117" t="s">
@@ -4852,53 +4848,53 @@
       <c r="C26" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="119" t="s">
+      <c r="D26" s="132" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="90" t="s">
+      <c r="E26" s="89" t="s">
         <v>62</v>
       </c>
       <c r="F26" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="104" t="s">
+      <c r="G26" s="148" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="116">
+      <c r="H26" s="146">
         <v>44012</v>
       </c>
-      <c r="I26" s="116">
+      <c r="I26" s="146">
         <v>44013</v>
       </c>
-      <c r="J26" s="119">
+      <c r="J26" s="132">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K26" s="118" t="s">
+      <c r="K26" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="111">
+      <c r="L26" s="141">
         <v>1</v>
       </c>
-      <c r="M26" s="67"/>
+      <c r="M26" s="66"/>
       <c r="N26" s="48"/>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
-      <c r="A27" s="126"/>
+      <c r="A27" s="139"/>
       <c r="B27" s="117"/>
       <c r="C27" s="117"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="92" t="s">
+      <c r="D27" s="140"/>
+      <c r="E27" s="91" t="s">
         <v>64</v>
       </c>
       <c r="F27" s="117"/>
-      <c r="G27" s="104"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="120"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="111"/>
-      <c r="M27" s="67"/>
+      <c r="G27" s="148"/>
+      <c r="H27" s="146"/>
+      <c r="I27" s="146"/>
+      <c r="J27" s="140"/>
+      <c r="K27" s="147"/>
+      <c r="L27" s="141"/>
+      <c r="M27" s="66"/>
       <c r="N27" s="48"/>
       <c r="O27" s="25"/>
       <c r="P27" s="25"/>
@@ -4910,7 +4906,7 @@
       <c r="V27" s="25"/>
     </row>
     <row r="28" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="108" t="s">
+      <c r="A28" s="104" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="117" t="s">
@@ -4922,54 +4918,54 @@
       <c r="D28" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="90" t="s">
+      <c r="E28" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="92" t="s">
+      <c r="F28" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="104" t="s">
+      <c r="G28" s="148" t="s">
         <v>68</v>
       </c>
-      <c r="H28" s="115">
+      <c r="H28" s="145">
         <v>44010</v>
       </c>
-      <c r="I28" s="116">
+      <c r="I28" s="146">
         <v>44013</v>
       </c>
       <c r="J28" s="117">
         <f>I28-H28</f>
         <v>3</v>
       </c>
-      <c r="K28" s="118" t="s">
+      <c r="K28" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="111">
+      <c r="L28" s="141">
         <v>1</v>
       </c>
       <c r="N28" s="48"/>
     </row>
     <row r="29" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="109"/>
+      <c r="A29" s="105"/>
       <c r="B29" s="117"/>
       <c r="C29" s="117"/>
       <c r="D29" s="117"/>
-      <c r="E29" s="92" t="s">
+      <c r="E29" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="71" t="s">
+      <c r="F29" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="104"/>
-      <c r="H29" s="115"/>
-      <c r="I29" s="116"/>
+      <c r="G29" s="148"/>
+      <c r="H29" s="145"/>
+      <c r="I29" s="146"/>
       <c r="J29" s="117"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="111"/>
+      <c r="K29" s="147"/>
+      <c r="L29" s="141"/>
       <c r="N29" s="48"/>
     </row>
     <row r="30" spans="1:22" ht="30" customHeight="1">
-      <c r="A30" s="110"/>
+      <c r="A30" s="106"/>
       <c r="B30" s="117"/>
       <c r="C30" s="117"/>
       <c r="D30" s="117"/>
@@ -4979,14 +4975,14 @@
       <c r="F30" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="G30" s="72" t="s">
+      <c r="G30" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="115"/>
-      <c r="I30" s="116"/>
+      <c r="H30" s="145"/>
+      <c r="I30" s="146"/>
       <c r="J30" s="117"/>
-      <c r="K30" s="118"/>
-      <c r="L30" s="111"/>
+      <c r="K30" s="147"/>
+      <c r="L30" s="141"/>
       <c r="M30" s="25"/>
       <c r="N30" s="48"/>
       <c r="O30" s="25"/>
@@ -4999,16 +4995,16 @@
       <c r="V30" s="25"/>
     </row>
     <row r="31" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A31" s="108" t="s">
+      <c r="A31" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="130" t="s">
+      <c r="C31" s="110" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="101" t="s">
+      <c r="D31" s="107" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="56" t="s">
@@ -5017,7 +5013,7 @@
       <c r="F31" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="69" t="s">
+      <c r="G31" s="68" t="s">
         <v>77</v>
       </c>
       <c r="H31" s="45">
@@ -5038,23 +5034,23 @@
       </c>
     </row>
     <row r="32" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A32" s="109"/>
-      <c r="B32" s="102"/>
-      <c r="C32" s="131"/>
-      <c r="D32" s="102"/>
+      <c r="A32" s="105"/>
+      <c r="B32" s="108"/>
+      <c r="C32" s="111"/>
+      <c r="D32" s="108"/>
       <c r="E32" s="44" t="s">
         <v>78</v>
       </c>
       <c r="F32" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="69" t="s">
+      <c r="G32" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="H32" s="76">
+      <c r="H32" s="75">
         <v>44019</v>
       </c>
-      <c r="I32" s="76">
+      <c r="I32" s="75">
         <v>44022</v>
       </c>
       <c r="J32" s="44">
@@ -5068,17 +5064,17 @@
       </c>
     </row>
     <row r="33" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A33" s="109"/>
-      <c r="B33" s="102"/>
-      <c r="C33" s="131"/>
-      <c r="D33" s="102"/>
+      <c r="A33" s="105"/>
+      <c r="B33" s="108"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="108"/>
       <c r="E33" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="87" t="s">
+      <c r="F33" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="66" t="s">
+      <c r="G33" s="65" t="s">
         <v>81</v>
       </c>
       <c r="H33" s="45">
@@ -5099,17 +5095,17 @@
       </c>
     </row>
     <row r="34" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A34" s="109"/>
-      <c r="B34" s="102"/>
-      <c r="C34" s="131"/>
-      <c r="D34" s="102"/>
+      <c r="A34" s="105"/>
+      <c r="B34" s="108"/>
+      <c r="C34" s="111"/>
+      <c r="D34" s="108"/>
       <c r="E34" s="44" t="s">
         <v>82</v>
       </c>
       <c r="F34" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="G34" s="69" t="s">
+      <c r="G34" s="68" t="s">
         <v>83</v>
       </c>
       <c r="H34" s="45">
@@ -5130,17 +5126,17 @@
       </c>
     </row>
     <row r="35" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A35" s="109"/>
-      <c r="B35" s="102"/>
-      <c r="C35" s="131"/>
-      <c r="D35" s="102"/>
+      <c r="A35" s="105"/>
+      <c r="B35" s="108"/>
+      <c r="C35" s="111"/>
+      <c r="D35" s="108"/>
       <c r="E35" s="44" t="s">
         <v>84</v>
       </c>
       <c r="F35" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="G35" s="81" t="s">
+      <c r="G35" s="80" t="s">
         <v>85</v>
       </c>
       <c r="H35" s="45">
@@ -5161,17 +5157,17 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="33" customHeight="1">
-      <c r="A36" s="110"/>
-      <c r="B36" s="103"/>
-      <c r="C36" s="132"/>
-      <c r="D36" s="103"/>
+      <c r="A36" s="106"/>
+      <c r="B36" s="109"/>
+      <c r="C36" s="112"/>
+      <c r="D36" s="109"/>
       <c r="E36" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="F36" s="92" t="s">
+      <c r="F36" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="75" t="s">
+      <c r="G36" s="74" t="s">
         <v>87</v>
       </c>
       <c r="H36" s="45">
@@ -5220,7 +5216,7 @@
       <c r="F37" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="69" t="s">
+      <c r="G37" s="68" t="s">
         <v>91</v>
       </c>
       <c r="H37" s="27" t="s">
@@ -5243,12 +5239,12 @@
       <c r="A38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="105"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="107"/>
+      <c r="B38" s="149"/>
+      <c r="C38" s="150"/>
+      <c r="D38" s="150"/>
+      <c r="E38" s="150"/>
+      <c r="F38" s="150"/>
+      <c r="G38" s="151"/>
       <c r="H38" s="27">
         <v>43837</v>
       </c>
@@ -5277,23 +5273,23 @@
       <c r="V38" s="25"/>
     </row>
     <row r="39" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A39" s="101" t="s">
+      <c r="A39" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="101" t="s">
+      <c r="B39" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101" t="s">
+      <c r="C39" s="107"/>
+      <c r="D39" s="107" t="s">
         <v>96</v>
       </c>
-      <c r="E39" s="63" t="s">
+      <c r="E39" s="62" t="s">
         <v>97</v>
       </c>
       <c r="F39" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="69" t="s">
+      <c r="G39" s="68" t="s">
         <v>99</v>
       </c>
       <c r="H39" s="27">
@@ -5314,17 +5310,17 @@
       <c r="N39" s="48"/>
     </row>
     <row r="40" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A40" s="102"/>
-      <c r="B40" s="102"/>
-      <c r="C40" s="102"/>
-      <c r="D40" s="102"/>
+      <c r="A40" s="108"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="108"/>
+      <c r="D40" s="108"/>
       <c r="E40" s="49" t="s">
         <v>100</v>
       </c>
       <c r="F40" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G40" s="69" t="s">
+      <c r="G40" s="68" t="s">
         <v>101</v>
       </c>
       <c r="H40" s="27">
@@ -5345,17 +5341,17 @@
       <c r="N40" s="48"/>
     </row>
     <row r="41" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A41" s="102"/>
-      <c r="B41" s="102"/>
-      <c r="C41" s="102"/>
-      <c r="D41" s="102"/>
+      <c r="A41" s="108"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="108"/>
+      <c r="D41" s="108"/>
       <c r="E41" s="49" t="s">
         <v>102</v>
       </c>
       <c r="F41" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="68" t="s">
+      <c r="G41" s="67" t="s">
         <v>103</v>
       </c>
       <c r="H41" s="27">
@@ -5376,17 +5372,17 @@
       <c r="N41" s="48"/>
     </row>
     <row r="42" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A42" s="102"/>
-      <c r="B42" s="102"/>
-      <c r="C42" s="102"/>
-      <c r="D42" s="102"/>
-      <c r="E42" s="63" t="s">
+      <c r="A42" s="108"/>
+      <c r="B42" s="108"/>
+      <c r="C42" s="108"/>
+      <c r="D42" s="108"/>
+      <c r="E42" s="62" t="s">
         <v>104</v>
       </c>
       <c r="F42" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="G42" s="68" t="s">
+      <c r="G42" s="67" t="s">
         <v>105</v>
       </c>
       <c r="H42" s="27">
@@ -5407,17 +5403,17 @@
       <c r="N42" s="48"/>
     </row>
     <row r="43" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A43" s="103"/>
-      <c r="B43" s="103"/>
-      <c r="C43" s="103"/>
-      <c r="D43" s="103"/>
+      <c r="A43" s="109"/>
+      <c r="B43" s="109"/>
+      <c r="C43" s="109"/>
+      <c r="D43" s="109"/>
       <c r="E43" s="43" t="s">
         <v>106</v>
       </c>
       <c r="F43" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="G43" s="69" t="s">
+      <c r="G43" s="68" t="s">
         <v>107</v>
       </c>
       <c r="H43" s="27">
@@ -5456,7 +5452,7 @@
       <c r="F44" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="G44" s="74" t="s">
+      <c r="G44" s="73" t="s">
         <v>112</v>
       </c>
       <c r="H44" s="27">
@@ -5487,25 +5483,25 @@
       <c r="V44" s="25"/>
     </row>
     <row r="45" spans="1:22" s="25" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A45" s="108" t="s">
+      <c r="A45" s="104" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="101" t="s">
+      <c r="B45" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="130" t="s">
+      <c r="C45" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="108" t="s">
+      <c r="D45" s="104" t="s">
         <v>27</v>
       </c>
       <c r="E45" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="F45" s="88" t="s">
+      <c r="F45" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="G45" s="88" t="s">
+      <c r="G45" s="87" t="s">
         <v>27</v>
       </c>
       <c r="H45" s="45">
@@ -5526,17 +5522,17 @@
       <c r="N45" s="48"/>
     </row>
     <row r="46" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A46" s="110"/>
-      <c r="B46" s="103"/>
-      <c r="C46" s="132"/>
-      <c r="D46" s="110"/>
-      <c r="E46" s="90" t="s">
+      <c r="A46" s="106"/>
+      <c r="B46" s="109"/>
+      <c r="C46" s="112"/>
+      <c r="D46" s="106"/>
+      <c r="E46" s="89" t="s">
         <v>117</v>
       </c>
-      <c r="F46" s="88" t="s">
+      <c r="F46" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="G46" s="88" t="s">
+      <c r="G46" s="87" t="s">
         <v>27</v>
       </c>
       <c r="H46" s="45">
@@ -5567,19 +5563,19 @@
       <c r="V46" s="25"/>
     </row>
     <row r="47" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A47" s="140" t="s">
+      <c r="A47" s="103" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="140"/>
-      <c r="C47" s="140"/>
-      <c r="D47" s="140"/>
-      <c r="E47" s="140"/>
-      <c r="F47" s="140"/>
-      <c r="G47" s="140"/>
-      <c r="H47" s="140"/>
-      <c r="I47" s="140"/>
-      <c r="J47" s="140"/>
-      <c r="K47" s="140"/>
+      <c r="B47" s="103"/>
+      <c r="C47" s="103"/>
+      <c r="D47" s="103"/>
+      <c r="E47" s="103"/>
+      <c r="F47" s="103"/>
+      <c r="G47" s="103"/>
+      <c r="H47" s="103"/>
+      <c r="I47" s="103"/>
+      <c r="J47" s="103"/>
+      <c r="K47" s="103"/>
       <c r="L47" s="38"/>
       <c r="M47" s="25"/>
       <c r="N47" s="25"/>
@@ -5615,7 +5611,7 @@
       <c r="K48" s="28"/>
       <c r="L48" s="39">
         <f>AVERAGE(L49,L62)</f>
-        <v>0.73416666666666663</v>
+        <v>0.93166666666666664</v>
       </c>
     </row>
     <row r="49" spans="1:22" s="25" customFormat="1" ht="27" customHeight="1">
@@ -5645,27 +5641,27 @@
       </c>
       <c r="L49" s="40">
         <f>AVERAGE(L50:L61)</f>
-        <v>0.83333333333333337</v>
+        <v>0.93333333333333346</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="38.25" customHeight="1">
-      <c r="A50" s="133" t="s">
+      <c r="A50" s="130" t="s">
         <v>122</v>
       </c>
       <c r="B50" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="130" t="s">
+      <c r="C50" s="110" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="137"/>
+      <c r="D50" s="114"/>
       <c r="E50" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="F50" s="92" t="s">
+      <c r="F50" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="G50" s="75" t="s">
+      <c r="G50" s="74" t="s">
         <v>125</v>
       </c>
       <c r="H50" s="27">
@@ -5696,17 +5692,17 @@
       <c r="V50" s="25"/>
     </row>
     <row r="51" spans="1:22" s="25" customFormat="1" ht="45" customHeight="1">
-      <c r="A51" s="133"/>
+      <c r="A51" s="130"/>
       <c r="B51" s="117"/>
-      <c r="C51" s="132"/>
-      <c r="D51" s="138"/>
+      <c r="C51" s="112"/>
+      <c r="D51" s="115"/>
       <c r="E51" s="49" t="s">
         <v>126</v>
       </c>
       <c r="F51" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="G51" s="85" t="s">
+      <c r="G51" s="84" t="s">
         <v>127</v>
       </c>
       <c r="H51" s="27">
@@ -5727,23 +5723,23 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A52" s="139" t="s">
+      <c r="A52" s="116" t="s">
         <v>128</v>
       </c>
       <c r="B52" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="123" t="s">
+      <c r="C52" s="113" t="s">
         <v>123</v>
       </c>
       <c r="D52" s="117"/>
-      <c r="E52" s="88" t="s">
+      <c r="E52" s="87" t="s">
         <v>129</v>
       </c>
-      <c r="F52" s="92" t="s">
+      <c r="F52" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="G52" s="86" t="s">
+      <c r="G52" s="85" t="s">
         <v>27</v>
       </c>
       <c r="H52" s="50">
@@ -5752,66 +5748,66 @@
       <c r="I52" s="50">
         <v>44043</v>
       </c>
-      <c r="J52" s="90">
+      <c r="J52" s="89">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="K52" s="64" t="s">
+      <c r="K52" s="63" t="s">
         <v>121</v>
       </c>
       <c r="L52" s="51">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="53" spans="1:22" s="25" customFormat="1" ht="57" customHeight="1">
-      <c r="A53" s="139"/>
+      <c r="A53" s="116"/>
       <c r="B53" s="117"/>
-      <c r="C53" s="123"/>
+      <c r="C53" s="113"/>
       <c r="D53" s="117"/>
-      <c r="E53" s="88" t="s">
+      <c r="E53" s="87" t="s">
         <v>130</v>
       </c>
-      <c r="F53" s="87" t="s">
+      <c r="F53" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="G53" s="85" t="s">
+      <c r="G53" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="H53" s="77">
+      <c r="H53" s="76">
         <v>44036</v>
       </c>
-      <c r="I53" s="77">
+      <c r="I53" s="76">
         <v>44043</v>
       </c>
-      <c r="J53" s="78">
+      <c r="J53" s="77">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K53" s="79" t="s">
+      <c r="K53" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="L53" s="80">
+      <c r="L53" s="79">
         <v>0.7</v>
       </c>
     </row>
     <row r="54" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A54" s="133" t="s">
+      <c r="A54" s="130" t="s">
         <v>132</v>
       </c>
       <c r="B54" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="123" t="s">
+      <c r="C54" s="113" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="135"/>
-      <c r="E54" s="88" t="s">
+      <c r="D54" s="134"/>
+      <c r="E54" s="87" t="s">
         <v>134</v>
       </c>
-      <c r="F54" s="87" t="s">
+      <c r="F54" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="G54" s="82" t="s">
+      <c r="G54" s="81" t="s">
         <v>135</v>
       </c>
       <c r="H54" s="50">
@@ -5820,29 +5816,29 @@
       <c r="I54" s="50">
         <v>44043</v>
       </c>
-      <c r="J54" s="90">
+      <c r="J54" s="89">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K54" s="64" t="s">
+      <c r="K54" s="63" t="s">
         <v>121</v>
       </c>
       <c r="L54" s="51">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="55" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A55" s="133"/>
+      <c r="A55" s="130"/>
       <c r="B55" s="117"/>
-      <c r="C55" s="123"/>
-      <c r="D55" s="135"/>
-      <c r="E55" s="96" t="s">
+      <c r="C55" s="113"/>
+      <c r="D55" s="134"/>
+      <c r="E55" s="95" t="s">
         <v>136</v>
       </c>
-      <c r="F55" s="96" t="s">
+      <c r="F55" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="G55" s="74" t="s">
+      <c r="G55" s="73" t="s">
         <v>137</v>
       </c>
       <c r="H55" s="50">
@@ -5851,128 +5847,128 @@
       <c r="I55" s="50">
         <v>44043</v>
       </c>
-      <c r="J55" s="96">
+      <c r="J55" s="95">
         <v>7</v>
       </c>
-      <c r="K55" s="64" t="s">
-        <v>121</v>
+      <c r="K55" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L55" s="51">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A56" s="134"/>
-      <c r="B56" s="119"/>
-      <c r="C56" s="124"/>
-      <c r="D56" s="136"/>
-      <c r="E56" s="100" t="s">
+      <c r="A56" s="131"/>
+      <c r="B56" s="132"/>
+      <c r="C56" s="133"/>
+      <c r="D56" s="135"/>
+      <c r="E56" s="99" t="s">
         <v>201</v>
       </c>
-      <c r="F56" s="95" t="s">
+      <c r="F56" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="G56" s="74"/>
+      <c r="G56" s="73"/>
       <c r="H56" s="50">
         <v>44043</v>
       </c>
       <c r="I56" s="27">
         <v>44057</v>
       </c>
-      <c r="J56" s="96">
+      <c r="J56" s="95">
         <v>14</v>
       </c>
-      <c r="K56" s="64" t="s">
-        <v>121</v>
+      <c r="K56" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L56" s="51">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A57" s="134"/>
-      <c r="B57" s="119"/>
-      <c r="C57" s="124"/>
-      <c r="D57" s="136"/>
-      <c r="E57" s="100" t="s">
+      <c r="A57" s="131"/>
+      <c r="B57" s="132"/>
+      <c r="C57" s="133"/>
+      <c r="D57" s="135"/>
+      <c r="E57" s="99" t="s">
         <v>203</v>
       </c>
-      <c r="F57" s="95" t="s">
+      <c r="F57" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="G57" s="74"/>
+      <c r="G57" s="73"/>
       <c r="H57" s="50">
         <v>44043</v>
       </c>
       <c r="I57" s="27">
         <v>44057</v>
       </c>
-      <c r="J57" s="96">
+      <c r="J57" s="95">
         <v>14</v>
       </c>
-      <c r="K57" s="64" t="s">
-        <v>121</v>
+      <c r="K57" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L57" s="51">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A58" s="134"/>
-      <c r="B58" s="119"/>
-      <c r="C58" s="124"/>
-      <c r="D58" s="136"/>
-      <c r="E58" s="100" t="s">
+      <c r="A58" s="131"/>
+      <c r="B58" s="132"/>
+      <c r="C58" s="133"/>
+      <c r="D58" s="135"/>
+      <c r="E58" s="99" t="s">
         <v>204</v>
       </c>
-      <c r="F58" s="96" t="s">
+      <c r="F58" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="74"/>
+      <c r="G58" s="73"/>
       <c r="H58" s="50">
         <v>44043</v>
       </c>
       <c r="I58" s="27">
         <v>44057</v>
       </c>
-      <c r="J58" s="96">
+      <c r="J58" s="95">
         <v>14</v>
       </c>
-      <c r="K58" s="64" t="s">
-        <v>121</v>
+      <c r="K58" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L58" s="51">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A59" s="146" t="s">
+      <c r="A59" s="123" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="147" t="s">
+      <c r="B59" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="148" t="s">
+      <c r="C59" s="125" t="s">
         <v>133</v>
       </c>
-      <c r="D59" s="149"/>
-      <c r="E59" s="96" t="s">
+      <c r="D59" s="126"/>
+      <c r="E59" s="95" t="s">
         <v>198</v>
       </c>
-      <c r="F59" s="96" t="s">
+      <c r="F59" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="99"/>
+      <c r="G59" s="98"/>
       <c r="H59" s="50">
         <v>44043</v>
       </c>
       <c r="I59" s="27">
         <v>44057</v>
       </c>
-      <c r="J59" s="90">
+      <c r="J59" s="89">
         <v>14</v>
       </c>
-      <c r="K59" s="64" t="s">
+      <c r="K59" s="63" t="s">
         <v>121</v>
       </c>
       <c r="L59" s="38">
@@ -5980,27 +5976,27 @@
       </c>
     </row>
     <row r="60" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A60" s="146"/>
-      <c r="B60" s="147"/>
-      <c r="C60" s="148"/>
-      <c r="D60" s="149"/>
-      <c r="E60" s="96" t="s">
+      <c r="A60" s="123"/>
+      <c r="B60" s="124"/>
+      <c r="C60" s="125"/>
+      <c r="D60" s="126"/>
+      <c r="E60" s="95" t="s">
         <v>199</v>
       </c>
-      <c r="F60" s="96" t="s">
+      <c r="F60" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="99"/>
+      <c r="G60" s="98"/>
       <c r="H60" s="50">
         <v>44043</v>
       </c>
       <c r="I60" s="27">
         <v>44057</v>
       </c>
-      <c r="J60" s="96">
+      <c r="J60" s="95">
         <v>14</v>
       </c>
-      <c r="K60" s="64" t="s">
+      <c r="K60" s="63" t="s">
         <v>121</v>
       </c>
       <c r="L60" s="38">
@@ -6008,14 +6004,14 @@
       </c>
     </row>
     <row r="61" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A61" s="146"/>
-      <c r="B61" s="147"/>
-      <c r="C61" s="148"/>
-      <c r="D61" s="149"/>
-      <c r="E61" s="96" t="s">
+      <c r="A61" s="123"/>
+      <c r="B61" s="124"/>
+      <c r="C61" s="125"/>
+      <c r="D61" s="126"/>
+      <c r="E61" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="F61" s="96" t="s">
+      <c r="F61" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G61" s="26"/>
@@ -6029,7 +6025,7 @@
         <f>I61-H61</f>
         <v>5</v>
       </c>
-      <c r="K61" s="64" t="s">
+      <c r="K61" s="63" t="s">
         <v>121</v>
       </c>
       <c r="L61" s="38">
@@ -6063,27 +6059,27 @@
       </c>
       <c r="L62" s="40">
         <f>AVERAGE(L63:L70,L72:L73)</f>
-        <v>0.63500000000000001</v>
+        <v>0.92999999999999994</v>
       </c>
     </row>
     <row r="63" spans="1:22" s="25" customFormat="1" ht="42.75" customHeight="1">
       <c r="A63" s="127" t="s">
         <v>142</v>
       </c>
-      <c r="B63" s="101" t="s">
+      <c r="B63" s="107" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="130" t="s">
+      <c r="C63" s="110" t="s">
         <v>143</v>
       </c>
-      <c r="D63" s="101"/>
+      <c r="D63" s="107"/>
       <c r="E63" s="49" t="s">
         <v>144</v>
       </c>
       <c r="F63" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="G63" s="68" t="s">
+      <c r="G63" s="67" t="s">
         <v>145</v>
       </c>
       <c r="H63" s="27">
@@ -6100,21 +6096,21 @@
         <v>121</v>
       </c>
       <c r="L63" s="38">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
       <c r="A64" s="128"/>
-      <c r="B64" s="102"/>
-      <c r="C64" s="131"/>
-      <c r="D64" s="102"/>
-      <c r="E64" s="84" t="s">
+      <c r="B64" s="108"/>
+      <c r="C64" s="111"/>
+      <c r="D64" s="108"/>
+      <c r="E64" s="83" t="s">
         <v>146</v>
       </c>
-      <c r="F64" s="92" t="s">
+      <c r="F64" s="91" t="s">
         <v>147</v>
       </c>
-      <c r="G64" s="93" t="s">
+      <c r="G64" s="92" t="s">
         <v>125</v>
       </c>
       <c r="H64" s="52">
@@ -6123,63 +6119,63 @@
       <c r="I64" s="27">
         <v>44057</v>
       </c>
-      <c r="J64" s="91">
+      <c r="J64" s="90">
         <v>21</v>
       </c>
       <c r="K64" s="58" t="s">
         <v>121</v>
       </c>
       <c r="L64" s="38">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="65" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
       <c r="A65" s="128"/>
-      <c r="B65" s="102"/>
-      <c r="C65" s="131"/>
-      <c r="D65" s="102"/>
-      <c r="E65" s="94" t="s">
+      <c r="B65" s="108"/>
+      <c r="C65" s="111"/>
+      <c r="D65" s="108"/>
+      <c r="E65" s="93" t="s">
         <v>148</v>
       </c>
       <c r="F65" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="G65" s="94"/>
+      <c r="G65" s="93"/>
       <c r="H65" s="52">
         <v>44030</v>
       </c>
       <c r="I65" s="27">
         <v>44057</v>
       </c>
-      <c r="J65" s="97">
+      <c r="J65" s="96">
         <v>21</v>
       </c>
       <c r="K65" s="58" t="s">
         <v>121</v>
       </c>
       <c r="L65" s="38">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="66" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
       <c r="A66" s="129"/>
-      <c r="B66" s="103"/>
-      <c r="C66" s="132"/>
-      <c r="D66" s="103"/>
-      <c r="E66" s="94" t="s">
+      <c r="B66" s="109"/>
+      <c r="C66" s="112"/>
+      <c r="D66" s="109"/>
+      <c r="E66" s="93" t="s">
         <v>205</v>
       </c>
-      <c r="F66" s="98" t="s">
+      <c r="F66" s="97" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="84"/>
+      <c r="G66" s="83"/>
       <c r="H66" s="52">
         <v>44030</v>
       </c>
       <c r="I66" s="27">
         <v>44057</v>
       </c>
-      <c r="J66" s="91">
+      <c r="J66" s="90">
         <v>21</v>
       </c>
       <c r="K66" s="58" t="s">
@@ -6190,23 +6186,23 @@
       </c>
     </row>
     <row r="67" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A67" s="139" t="s">
+      <c r="A67" s="116" t="s">
         <v>149</v>
       </c>
-      <c r="B67" s="101" t="s">
+      <c r="B67" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="130" t="s">
+      <c r="C67" s="110" t="s">
         <v>150</v>
       </c>
-      <c r="D67" s="137"/>
-      <c r="E67" s="61" t="s">
+      <c r="D67" s="114"/>
+      <c r="E67" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="F67" s="91" t="s">
+      <c r="F67" s="90" t="s">
         <v>152</v>
       </c>
-      <c r="G67" s="70" t="s">
+      <c r="G67" s="69" t="s">
         <v>153</v>
       </c>
       <c r="H67" s="52">
@@ -6215,29 +6211,29 @@
       <c r="I67" s="27">
         <v>44057</v>
       </c>
-      <c r="J67" s="91">
+      <c r="J67" s="90">
         <f>I67-H67</f>
         <v>25</v>
       </c>
-      <c r="K67" s="58" t="s">
-        <v>121</v>
+      <c r="K67" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L67" s="38">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A68" s="139"/>
-      <c r="B68" s="102"/>
-      <c r="C68" s="131"/>
-      <c r="D68" s="144"/>
-      <c r="E68" s="61" t="s">
+      <c r="A68" s="116"/>
+      <c r="B68" s="108"/>
+      <c r="C68" s="111"/>
+      <c r="D68" s="121"/>
+      <c r="E68" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="F68" s="91" t="s">
+      <c r="F68" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="G68" s="83" t="s">
+      <c r="G68" s="82" t="s">
         <v>155</v>
       </c>
       <c r="H68" s="52">
@@ -6246,29 +6242,29 @@
       <c r="I68" s="27">
         <v>44057</v>
       </c>
-      <c r="J68" s="91">
+      <c r="J68" s="90">
         <f>I68-H68</f>
         <v>25</v>
       </c>
-      <c r="K68" s="58" t="s">
-        <v>121</v>
+      <c r="K68" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L68" s="38">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A69" s="139"/>
-      <c r="B69" s="102"/>
-      <c r="C69" s="131"/>
-      <c r="D69" s="144"/>
-      <c r="E69" s="61" t="s">
+      <c r="A69" s="116"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="111"/>
+      <c r="D69" s="121"/>
+      <c r="E69" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="F69" s="97" t="s">
+      <c r="F69" s="96" t="s">
         <v>157</v>
       </c>
-      <c r="G69" s="70" t="s">
+      <c r="G69" s="69" t="s">
         <v>158</v>
       </c>
       <c r="H69" s="52">
@@ -6277,60 +6273,60 @@
       <c r="I69" s="27">
         <v>44057</v>
       </c>
-      <c r="J69" s="97">
+      <c r="J69" s="96">
         <f>I69-H69</f>
         <v>25</v>
       </c>
-      <c r="K69" s="60" t="s">
+      <c r="K69" s="58" t="s">
         <v>121</v>
       </c>
       <c r="L69" s="38">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="70" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A70" s="139"/>
-      <c r="B70" s="142"/>
-      <c r="C70" s="143"/>
-      <c r="D70" s="145"/>
-      <c r="E70" s="61" t="s">
+      <c r="A70" s="116"/>
+      <c r="B70" s="119"/>
+      <c r="C70" s="120"/>
+      <c r="D70" s="122"/>
+      <c r="E70" s="60" t="s">
         <v>202</v>
       </c>
-      <c r="F70" s="91" t="s">
+      <c r="F70" s="90" t="s">
         <v>157</v>
       </c>
-      <c r="G70" s="70"/>
+      <c r="G70" s="69"/>
       <c r="H70" s="52">
         <v>44032</v>
       </c>
       <c r="I70" s="27">
         <v>44057</v>
       </c>
-      <c r="J70" s="91">
+      <c r="J70" s="90">
         <f>I70-H70</f>
         <v>25</v>
       </c>
-      <c r="K70" s="58" t="s">
-        <v>121</v>
+      <c r="K70" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L70" s="38">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A71" s="141" t="s">
+      <c r="A71" s="118" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="141"/>
-      <c r="C71" s="141"/>
-      <c r="D71" s="141"/>
-      <c r="E71" s="141"/>
-      <c r="F71" s="141"/>
-      <c r="G71" s="141"/>
-      <c r="H71" s="141"/>
-      <c r="I71" s="141"/>
-      <c r="J71" s="141"/>
-      <c r="K71" s="141"/>
+      <c r="B71" s="118"/>
+      <c r="C71" s="118"/>
+      <c r="D71" s="118"/>
+      <c r="E71" s="118"/>
+      <c r="F71" s="118"/>
+      <c r="G71" s="118"/>
+      <c r="H71" s="118"/>
+      <c r="I71" s="118"/>
+      <c r="J71" s="118"/>
+      <c r="K71" s="118"/>
       <c r="L71" s="57"/>
       <c r="M71" s="25"/>
       <c r="N71" s="25"/>
@@ -6347,29 +6343,29 @@
       <c r="A72" s="59" t="s">
         <v>160</v>
       </c>
-      <c r="B72" s="92" t="s">
+      <c r="B72" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="C72" s="92"/>
-      <c r="D72" s="92"/>
-      <c r="E72" s="92"/>
-      <c r="F72" s="92"/>
-      <c r="G72" s="92"/>
+      <c r="C72" s="91"/>
+      <c r="D72" s="91"/>
+      <c r="E72" s="91"/>
+      <c r="F72" s="91"/>
+      <c r="G72" s="91"/>
       <c r="H72" s="55">
         <v>44043</v>
       </c>
       <c r="I72" s="27">
         <v>44057</v>
       </c>
-      <c r="J72" s="92">
+      <c r="J72" s="91">
         <f t="shared" ref="J72:J90" si="2">I72-H72</f>
         <v>14</v>
       </c>
-      <c r="K72" s="60" t="s">
-        <v>139</v>
+      <c r="K72" s="58" t="s">
+        <v>121</v>
       </c>
       <c r="L72" s="38">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M72" s="25"/>
       <c r="N72" s="25"/>
@@ -6404,11 +6400,11 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="K73" s="28" t="s">
-        <v>139</v>
+      <c r="K73" s="58" t="s">
+        <v>121</v>
       </c>
       <c r="L73" s="38">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M73" s="25"/>
       <c r="N73" s="25"/>
@@ -6968,19 +6964,19 @@
       <c r="V90" s="25"/>
     </row>
     <row r="91" spans="1:22" ht="25.5" customHeight="1">
-      <c r="A91" s="140" t="s">
+      <c r="A91" s="103" t="s">
         <v>179</v>
       </c>
-      <c r="B91" s="140"/>
-      <c r="C91" s="140"/>
-      <c r="D91" s="140"/>
-      <c r="E91" s="140"/>
-      <c r="F91" s="140"/>
-      <c r="G91" s="140"/>
-      <c r="H91" s="140"/>
-      <c r="I91" s="140"/>
-      <c r="J91" s="140"/>
-      <c r="K91" s="140"/>
+      <c r="B91" s="103"/>
+      <c r="C91" s="103"/>
+      <c r="D91" s="103"/>
+      <c r="E91" s="103"/>
+      <c r="F91" s="103"/>
+      <c r="G91" s="103"/>
+      <c r="H91" s="103"/>
+      <c r="I91" s="103"/>
+      <c r="J91" s="103"/>
+      <c r="K91" s="103"/>
       <c r="L91" s="38"/>
       <c r="M91" s="25"/>
       <c r="N91" s="25"/>
@@ -7159,6 +7155,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A71:K71"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D59:D61"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
@@ -7175,103 +7233,41 @@
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="C31:C36"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A71:K71"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="D54:D58"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G23" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G39" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G30" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G43" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G25" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G41" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G44" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G32" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G26:G27" r:id="rId16" display="https://github.com/antonyMontalvo/FaceSolutions/commit/8f0ec13380b96dbff2cf0f44e517515e6d8e935b" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G63" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G51" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G36" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G28:G29" r:id="rId20" display="https://github.com/antonyMontalvo/FaceSolutions/commit/b7f87017c045c76f3ed7353bf35a7680607f9adf" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G42" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G37" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G50" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G31" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G67" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G19" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G35" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G54" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G53" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="G68" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="G64" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="G55" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G69" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G20" r:id="rId1"/>
+    <hyperlink ref="G21" r:id="rId2"/>
+    <hyperlink ref="G34" r:id="rId3"/>
+    <hyperlink ref="G23" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5"/>
+    <hyperlink ref="G24" r:id="rId6"/>
+    <hyperlink ref="G39" r:id="rId7"/>
+    <hyperlink ref="G30" r:id="rId8"/>
+    <hyperlink ref="G33" r:id="rId9"/>
+    <hyperlink ref="G43" r:id="rId10"/>
+    <hyperlink ref="G25" r:id="rId11"/>
+    <hyperlink ref="G41" r:id="rId12"/>
+    <hyperlink ref="G44" r:id="rId13"/>
+    <hyperlink ref="G32" r:id="rId14"/>
+    <hyperlink ref="G40" r:id="rId15"/>
+    <hyperlink ref="G26:G27" r:id="rId16" display="https://github.com/antonyMontalvo/FaceSolutions/commit/8f0ec13380b96dbff2cf0f44e517515e6d8e935b"/>
+    <hyperlink ref="G63" r:id="rId17"/>
+    <hyperlink ref="G51" r:id="rId18"/>
+    <hyperlink ref="G36" r:id="rId19"/>
+    <hyperlink ref="G28:G29" r:id="rId20" display="https://github.com/antonyMontalvo/FaceSolutions/commit/b7f87017c045c76f3ed7353bf35a7680607f9adf"/>
+    <hyperlink ref="G42" r:id="rId21"/>
+    <hyperlink ref="G37" r:id="rId22"/>
+    <hyperlink ref="G50" r:id="rId23"/>
+    <hyperlink ref="G31" r:id="rId24"/>
+    <hyperlink ref="G67" r:id="rId25"/>
+    <hyperlink ref="G19" r:id="rId26"/>
+    <hyperlink ref="G35" r:id="rId27"/>
+    <hyperlink ref="G54" r:id="rId28"/>
+    <hyperlink ref="G53" r:id="rId29"/>
+    <hyperlink ref="G68" r:id="rId30"/>
+    <hyperlink ref="G64" r:id="rId31"/>
+    <hyperlink ref="G55" r:id="rId32"/>
+    <hyperlink ref="G69" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId34"/>
@@ -7280,7 +7276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Implementacion de envio de correo dinamico
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antony\Desktop\Repo\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C83EA8E-8CBC-48A6-963B-70E1667F20C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de proyecto y Gantt" sheetId="1" r:id="rId1"/>
     <sheet name="Línea base de costo" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -676,7 +677,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;S/&quot;\ #,##0.00;[Red]&quot;S/&quot;\ \-#,##0.00"/>
   </numFmts>
@@ -1364,6 +1365,153 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1372,153 +1520,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1527,7 +1528,7 @@
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6"/>
+    <cellStyle name="Hyperlink" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3997,11 +3998,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4024,21 +4025,21 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="149"/>
+      <c r="L2" s="149"/>
+      <c r="M2" s="149"/>
+      <c r="N2" s="149"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
@@ -4052,15 +4053,15 @@
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -4080,15 +4081,15 @@
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
+      <c r="C4" s="150"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="150"/>
+      <c r="H4" s="150"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -4108,15 +4109,15 @@
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
+      <c r="C5" s="151"/>
+      <c r="D5" s="151"/>
+      <c r="E5" s="151"/>
+      <c r="F5" s="151"/>
+      <c r="G5" s="151"/>
+      <c r="H5" s="151"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -4217,7 +4218,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="5">
-        <v>0.68</v>
+        <v>0.72</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4366,7 +4367,7 @@
       <c r="C13" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="142"/>
+      <c r="D13" s="111"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26" t="s">
         <v>26</v>
@@ -4402,16 +4403,16 @@
       <c r="V13" s="25"/>
     </row>
     <row r="14" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A14" s="136" t="s">
+      <c r="A14" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="113" t="s">
+      <c r="C14" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="143"/>
+      <c r="D14" s="112"/>
       <c r="E14" s="89" t="s">
         <v>31</v>
       </c>
@@ -4439,10 +4440,10 @@
       </c>
     </row>
     <row r="15" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A15" s="137"/>
-      <c r="B15" s="132"/>
-      <c r="C15" s="133"/>
-      <c r="D15" s="143"/>
+      <c r="A15" s="121"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="112"/>
       <c r="E15" s="89" t="s">
         <v>31</v>
       </c>
@@ -4479,7 +4480,7 @@
       <c r="C16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="143"/>
+      <c r="D16" s="112"/>
       <c r="E16" s="43" t="s">
         <v>34</v>
       </c>
@@ -4515,7 +4516,7 @@
       <c r="C17" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="144"/>
+      <c r="D17" s="113"/>
       <c r="E17" s="44" t="s">
         <v>36</v>
       </c>
@@ -4546,12 +4547,12 @@
       <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="149"/>
-      <c r="C18" s="150"/>
-      <c r="D18" s="150"/>
-      <c r="E18" s="150"/>
-      <c r="F18" s="150"/>
-      <c r="G18" s="151"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="106"/>
       <c r="H18" s="27">
         <v>44008</v>
       </c>
@@ -4581,16 +4582,16 @@
       <c r="V18" s="25"/>
     </row>
     <row r="19" spans="1:22" s="25" customFormat="1" ht="36" customHeight="1">
-      <c r="A19" s="104" t="s">
+      <c r="A19" s="107" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="110" t="s">
+      <c r="C19" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="107" t="s">
+      <c r="D19" s="100" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="88" t="s">
@@ -4619,10 +4620,10 @@
       </c>
     </row>
     <row r="20" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="105"/>
-      <c r="B20" s="108"/>
-      <c r="C20" s="111"/>
-      <c r="D20" s="108"/>
+      <c r="A20" s="108"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="130"/>
+      <c r="D20" s="101"/>
       <c r="E20" s="60" t="s">
         <v>44</v>
       </c>
@@ -4649,10 +4650,10 @@
       </c>
     </row>
     <row r="21" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A21" s="106"/>
-      <c r="B21" s="109"/>
-      <c r="C21" s="112"/>
-      <c r="D21" s="109"/>
+      <c r="A21" s="109"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="131"/>
+      <c r="D21" s="102"/>
       <c r="E21" s="49" t="s">
         <v>46</v>
       </c>
@@ -4728,16 +4729,16 @@
       <c r="V22" s="25"/>
     </row>
     <row r="23" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A23" s="104" t="s">
+      <c r="A23" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="113" t="s">
+      <c r="B23" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="113" t="s">
+      <c r="C23" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="107" t="s">
+      <c r="D23" s="100" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="60" t="s">
@@ -4767,10 +4768,10 @@
       </c>
     </row>
     <row r="24" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A24" s="105"/>
-      <c r="B24" s="113"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="108"/>
+      <c r="A24" s="108"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="101"/>
       <c r="E24" s="88" t="s">
         <v>56</v>
       </c>
@@ -4798,10 +4799,10 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="52.5" customHeight="1">
-      <c r="A25" s="105"/>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="108"/>
+      <c r="A25" s="108"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="122"/>
+      <c r="D25" s="101"/>
       <c r="E25" s="83" t="s">
         <v>36</v>
       </c>
@@ -4839,61 +4840,61 @@
       <c r="V25" s="25"/>
     </row>
     <row r="26" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A26" s="138" t="s">
+      <c r="A26" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="117" t="s">
+      <c r="B26" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="117" t="s">
+      <c r="C26" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="132" t="s">
+      <c r="D26" s="118" t="s">
         <v>61</v>
       </c>
       <c r="E26" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="117" t="s">
+      <c r="F26" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="148" t="s">
+      <c r="G26" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="146">
+      <c r="H26" s="115">
         <v>44012</v>
       </c>
-      <c r="I26" s="146">
+      <c r="I26" s="115">
         <v>44013</v>
       </c>
-      <c r="J26" s="132">
+      <c r="J26" s="118">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K26" s="147" t="s">
+      <c r="K26" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="141">
+      <c r="L26" s="110">
         <v>1</v>
       </c>
       <c r="M26" s="66"/>
       <c r="N26" s="48"/>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
-      <c r="A27" s="139"/>
-      <c r="B27" s="117"/>
-      <c r="C27" s="117"/>
-      <c r="D27" s="140"/>
+      <c r="A27" s="125"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="119"/>
       <c r="E27" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="117"/>
-      <c r="G27" s="148"/>
-      <c r="H27" s="146"/>
-      <c r="I27" s="146"/>
-      <c r="J27" s="140"/>
-      <c r="K27" s="147"/>
-      <c r="L27" s="141"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="119"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="110"/>
       <c r="M27" s="66"/>
       <c r="N27" s="48"/>
       <c r="O27" s="25"/>
@@ -4906,16 +4907,16 @@
       <c r="V27" s="25"/>
     </row>
     <row r="28" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="104" t="s">
+      <c r="A28" s="107" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="117" t="s">
+      <c r="C28" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="117" t="s">
+      <c r="D28" s="116" t="s">
         <v>66</v>
       </c>
       <c r="E28" s="89" t="s">
@@ -4924,51 +4925,51 @@
       <c r="F28" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="148" t="s">
+      <c r="G28" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="H28" s="145">
+      <c r="H28" s="114">
         <v>44010</v>
       </c>
-      <c r="I28" s="146">
+      <c r="I28" s="115">
         <v>44013</v>
       </c>
-      <c r="J28" s="117">
+      <c r="J28" s="116">
         <f>I28-H28</f>
         <v>3</v>
       </c>
-      <c r="K28" s="147" t="s">
+      <c r="K28" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="141">
+      <c r="L28" s="110">
         <v>1</v>
       </c>
       <c r="N28" s="48"/>
     </row>
     <row r="29" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="105"/>
-      <c r="B29" s="117"/>
-      <c r="C29" s="117"/>
-      <c r="D29" s="117"/>
+      <c r="A29" s="108"/>
+      <c r="B29" s="116"/>
+      <c r="C29" s="116"/>
+      <c r="D29" s="116"/>
       <c r="E29" s="91" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="148"/>
-      <c r="H29" s="145"/>
-      <c r="I29" s="146"/>
-      <c r="J29" s="117"/>
-      <c r="K29" s="147"/>
-      <c r="L29" s="141"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="114"/>
+      <c r="I29" s="115"/>
+      <c r="J29" s="116"/>
+      <c r="K29" s="117"/>
+      <c r="L29" s="110"/>
       <c r="N29" s="48"/>
     </row>
     <row r="30" spans="1:22" ht="30" customHeight="1">
-      <c r="A30" s="106"/>
-      <c r="B30" s="117"/>
-      <c r="C30" s="117"/>
-      <c r="D30" s="117"/>
+      <c r="A30" s="109"/>
+      <c r="B30" s="116"/>
+      <c r="C30" s="116"/>
+      <c r="D30" s="116"/>
       <c r="E30" s="26" t="s">
         <v>70</v>
       </c>
@@ -4978,11 +4979,11 @@
       <c r="G30" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="145"/>
-      <c r="I30" s="146"/>
-      <c r="J30" s="117"/>
-      <c r="K30" s="147"/>
-      <c r="L30" s="141"/>
+      <c r="H30" s="114"/>
+      <c r="I30" s="115"/>
+      <c r="J30" s="116"/>
+      <c r="K30" s="117"/>
+      <c r="L30" s="110"/>
       <c r="M30" s="25"/>
       <c r="N30" s="48"/>
       <c r="O30" s="25"/>
@@ -4995,16 +4996,16 @@
       <c r="V30" s="25"/>
     </row>
     <row r="31" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A31" s="104" t="s">
+      <c r="A31" s="107" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="107" t="s">
+      <c r="B31" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="110" t="s">
+      <c r="C31" s="129" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="107" t="s">
+      <c r="D31" s="100" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="56" t="s">
@@ -5034,10 +5035,10 @@
       </c>
     </row>
     <row r="32" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A32" s="105"/>
-      <c r="B32" s="108"/>
-      <c r="C32" s="111"/>
-      <c r="D32" s="108"/>
+      <c r="A32" s="108"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="130"/>
+      <c r="D32" s="101"/>
       <c r="E32" s="44" t="s">
         <v>78</v>
       </c>
@@ -5064,10 +5065,10 @@
       </c>
     </row>
     <row r="33" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A33" s="105"/>
-      <c r="B33" s="108"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="108"/>
+      <c r="A33" s="108"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="130"/>
+      <c r="D33" s="101"/>
       <c r="E33" s="44" t="s">
         <v>80</v>
       </c>
@@ -5095,10 +5096,10 @@
       </c>
     </row>
     <row r="34" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A34" s="105"/>
-      <c r="B34" s="108"/>
-      <c r="C34" s="111"/>
-      <c r="D34" s="108"/>
+      <c r="A34" s="108"/>
+      <c r="B34" s="101"/>
+      <c r="C34" s="130"/>
+      <c r="D34" s="101"/>
       <c r="E34" s="44" t="s">
         <v>82</v>
       </c>
@@ -5126,10 +5127,10 @@
       </c>
     </row>
     <row r="35" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A35" s="105"/>
-      <c r="B35" s="108"/>
-      <c r="C35" s="111"/>
-      <c r="D35" s="108"/>
+      <c r="A35" s="108"/>
+      <c r="B35" s="101"/>
+      <c r="C35" s="130"/>
+      <c r="D35" s="101"/>
       <c r="E35" s="44" t="s">
         <v>84</v>
       </c>
@@ -5157,10 +5158,10 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="33" customHeight="1">
-      <c r="A36" s="106"/>
-      <c r="B36" s="109"/>
-      <c r="C36" s="112"/>
-      <c r="D36" s="109"/>
+      <c r="A36" s="109"/>
+      <c r="B36" s="102"/>
+      <c r="C36" s="131"/>
+      <c r="D36" s="102"/>
       <c r="E36" s="44" t="s">
         <v>86</v>
       </c>
@@ -5239,12 +5240,12 @@
       <c r="A38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="149"/>
-      <c r="C38" s="150"/>
-      <c r="D38" s="150"/>
-      <c r="E38" s="150"/>
-      <c r="F38" s="150"/>
-      <c r="G38" s="151"/>
+      <c r="B38" s="104"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="105"/>
+      <c r="E38" s="105"/>
+      <c r="F38" s="105"/>
+      <c r="G38" s="106"/>
       <c r="H38" s="27">
         <v>43837</v>
       </c>
@@ -5273,14 +5274,14 @@
       <c r="V38" s="25"/>
     </row>
     <row r="39" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A39" s="107" t="s">
+      <c r="A39" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="107" t="s">
+      <c r="B39" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="107"/>
-      <c r="D39" s="107" t="s">
+      <c r="C39" s="100"/>
+      <c r="D39" s="100" t="s">
         <v>96</v>
       </c>
       <c r="E39" s="62" t="s">
@@ -5310,10 +5311,10 @@
       <c r="N39" s="48"/>
     </row>
     <row r="40" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A40" s="108"/>
-      <c r="B40" s="108"/>
-      <c r="C40" s="108"/>
-      <c r="D40" s="108"/>
+      <c r="A40" s="101"/>
+      <c r="B40" s="101"/>
+      <c r="C40" s="101"/>
+      <c r="D40" s="101"/>
       <c r="E40" s="49" t="s">
         <v>100</v>
       </c>
@@ -5341,10 +5342,10 @@
       <c r="N40" s="48"/>
     </row>
     <row r="41" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A41" s="108"/>
-      <c r="B41" s="108"/>
-      <c r="C41" s="108"/>
-      <c r="D41" s="108"/>
+      <c r="A41" s="101"/>
+      <c r="B41" s="101"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="101"/>
       <c r="E41" s="49" t="s">
         <v>102</v>
       </c>
@@ -5372,10 +5373,10 @@
       <c r="N41" s="48"/>
     </row>
     <row r="42" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A42" s="108"/>
-      <c r="B42" s="108"/>
-      <c r="C42" s="108"/>
-      <c r="D42" s="108"/>
+      <c r="A42" s="101"/>
+      <c r="B42" s="101"/>
+      <c r="C42" s="101"/>
+      <c r="D42" s="101"/>
       <c r="E42" s="62" t="s">
         <v>104</v>
       </c>
@@ -5403,10 +5404,10 @@
       <c r="N42" s="48"/>
     </row>
     <row r="43" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A43" s="109"/>
-      <c r="B43" s="109"/>
-      <c r="C43" s="109"/>
-      <c r="D43" s="109"/>
+      <c r="A43" s="102"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="102"/>
+      <c r="D43" s="102"/>
       <c r="E43" s="43" t="s">
         <v>106</v>
       </c>
@@ -5483,16 +5484,16 @@
       <c r="V44" s="25"/>
     </row>
     <row r="45" spans="1:22" s="25" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A45" s="104" t="s">
+      <c r="A45" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="107" t="s">
+      <c r="B45" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="110" t="s">
+      <c r="C45" s="129" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="104" t="s">
+      <c r="D45" s="107" t="s">
         <v>27</v>
       </c>
       <c r="E45" s="43" t="s">
@@ -5522,10 +5523,10 @@
       <c r="N45" s="48"/>
     </row>
     <row r="46" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A46" s="106"/>
-      <c r="B46" s="109"/>
-      <c r="C46" s="112"/>
-      <c r="D46" s="106"/>
+      <c r="A46" s="109"/>
+      <c r="B46" s="102"/>
+      <c r="C46" s="131"/>
+      <c r="D46" s="109"/>
       <c r="E46" s="89" t="s">
         <v>117</v>
       </c>
@@ -5563,19 +5564,19 @@
       <c r="V46" s="25"/>
     </row>
     <row r="47" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A47" s="103" t="s">
+      <c r="A47" s="139" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="103"/>
-      <c r="C47" s="103"/>
-      <c r="D47" s="103"/>
-      <c r="E47" s="103"/>
-      <c r="F47" s="103"/>
-      <c r="G47" s="103"/>
-      <c r="H47" s="103"/>
-      <c r="I47" s="103"/>
-      <c r="J47" s="103"/>
-      <c r="K47" s="103"/>
+      <c r="B47" s="139"/>
+      <c r="C47" s="139"/>
+      <c r="D47" s="139"/>
+      <c r="E47" s="139"/>
+      <c r="F47" s="139"/>
+      <c r="G47" s="139"/>
+      <c r="H47" s="139"/>
+      <c r="I47" s="139"/>
+      <c r="J47" s="139"/>
+      <c r="K47" s="139"/>
       <c r="L47" s="38"/>
       <c r="M47" s="25"/>
       <c r="N47" s="25"/>
@@ -5645,16 +5646,16 @@
       </c>
     </row>
     <row r="50" spans="1:22" ht="38.25" customHeight="1">
-      <c r="A50" s="130" t="s">
+      <c r="A50" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="117" t="s">
+      <c r="B50" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="110" t="s">
+      <c r="C50" s="129" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="114"/>
+      <c r="D50" s="136"/>
       <c r="E50" s="44" t="s">
         <v>124</v>
       </c>
@@ -5692,10 +5693,10 @@
       <c r="V50" s="25"/>
     </row>
     <row r="51" spans="1:22" s="25" customFormat="1" ht="45" customHeight="1">
-      <c r="A51" s="130"/>
-      <c r="B51" s="117"/>
-      <c r="C51" s="112"/>
-      <c r="D51" s="115"/>
+      <c r="A51" s="132"/>
+      <c r="B51" s="116"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="137"/>
       <c r="E51" s="49" t="s">
         <v>126</v>
       </c>
@@ -5723,16 +5724,16 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A52" s="116" t="s">
+      <c r="A52" s="138" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="117" t="s">
+      <c r="B52" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="113" t="s">
+      <c r="C52" s="122" t="s">
         <v>123</v>
       </c>
-      <c r="D52" s="117"/>
+      <c r="D52" s="116"/>
       <c r="E52" s="87" t="s">
         <v>129</v>
       </c>
@@ -5760,10 +5761,10 @@
       </c>
     </row>
     <row r="53" spans="1:22" s="25" customFormat="1" ht="57" customHeight="1">
-      <c r="A53" s="116"/>
-      <c r="B53" s="117"/>
-      <c r="C53" s="113"/>
-      <c r="D53" s="117"/>
+      <c r="A53" s="138"/>
+      <c r="B53" s="116"/>
+      <c r="C53" s="122"/>
+      <c r="D53" s="116"/>
       <c r="E53" s="87" t="s">
         <v>130</v>
       </c>
@@ -5791,13 +5792,13 @@
       </c>
     </row>
     <row r="54" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A54" s="130" t="s">
+      <c r="A54" s="132" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="117" t="s">
+      <c r="B54" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="113" t="s">
+      <c r="C54" s="122" t="s">
         <v>133</v>
       </c>
       <c r="D54" s="134"/>
@@ -5828,9 +5829,9 @@
       </c>
     </row>
     <row r="55" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A55" s="130"/>
-      <c r="B55" s="117"/>
-      <c r="C55" s="113"/>
+      <c r="A55" s="132"/>
+      <c r="B55" s="116"/>
+      <c r="C55" s="122"/>
       <c r="D55" s="134"/>
       <c r="E55" s="95" t="s">
         <v>136</v>
@@ -5858,9 +5859,9 @@
       </c>
     </row>
     <row r="56" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A56" s="131"/>
-      <c r="B56" s="132"/>
-      <c r="C56" s="133"/>
+      <c r="A56" s="133"/>
+      <c r="B56" s="118"/>
+      <c r="C56" s="123"/>
       <c r="D56" s="135"/>
       <c r="E56" s="99" t="s">
         <v>201</v>
@@ -5886,9 +5887,9 @@
       </c>
     </row>
     <row r="57" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A57" s="131"/>
-      <c r="B57" s="132"/>
-      <c r="C57" s="133"/>
+      <c r="A57" s="133"/>
+      <c r="B57" s="118"/>
+      <c r="C57" s="123"/>
       <c r="D57" s="135"/>
       <c r="E57" s="99" t="s">
         <v>203</v>
@@ -5914,9 +5915,9 @@
       </c>
     </row>
     <row r="58" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A58" s="131"/>
-      <c r="B58" s="132"/>
-      <c r="C58" s="133"/>
+      <c r="A58" s="133"/>
+      <c r="B58" s="118"/>
+      <c r="C58" s="123"/>
       <c r="D58" s="135"/>
       <c r="E58" s="99" t="s">
         <v>204</v>
@@ -5942,16 +5943,16 @@
       </c>
     </row>
     <row r="59" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A59" s="123" t="s">
+      <c r="A59" s="145" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="124" t="s">
+      <c r="B59" s="146" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="125" t="s">
+      <c r="C59" s="147" t="s">
         <v>133</v>
       </c>
-      <c r="D59" s="126"/>
+      <c r="D59" s="148"/>
       <c r="E59" s="95" t="s">
         <v>198</v>
       </c>
@@ -5976,10 +5977,10 @@
       </c>
     </row>
     <row r="60" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A60" s="123"/>
-      <c r="B60" s="124"/>
-      <c r="C60" s="125"/>
-      <c r="D60" s="126"/>
+      <c r="A60" s="145"/>
+      <c r="B60" s="146"/>
+      <c r="C60" s="147"/>
+      <c r="D60" s="148"/>
       <c r="E60" s="95" t="s">
         <v>199</v>
       </c>
@@ -6004,10 +6005,10 @@
       </c>
     </row>
     <row r="61" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A61" s="123"/>
-      <c r="B61" s="124"/>
-      <c r="C61" s="125"/>
-      <c r="D61" s="126"/>
+      <c r="A61" s="145"/>
+      <c r="B61" s="146"/>
+      <c r="C61" s="147"/>
+      <c r="D61" s="148"/>
       <c r="E61" s="95" t="s">
         <v>200</v>
       </c>
@@ -6063,16 +6064,16 @@
       </c>
     </row>
     <row r="63" spans="1:22" s="25" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A63" s="127" t="s">
+      <c r="A63" s="126" t="s">
         <v>142</v>
       </c>
-      <c r="B63" s="107" t="s">
+      <c r="B63" s="100" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="110" t="s">
+      <c r="C63" s="129" t="s">
         <v>143</v>
       </c>
-      <c r="D63" s="107"/>
+      <c r="D63" s="100"/>
       <c r="E63" s="49" t="s">
         <v>144</v>
       </c>
@@ -6100,10 +6101,10 @@
       </c>
     </row>
     <row r="64" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A64" s="128"/>
-      <c r="B64" s="108"/>
-      <c r="C64" s="111"/>
-      <c r="D64" s="108"/>
+      <c r="A64" s="127"/>
+      <c r="B64" s="101"/>
+      <c r="C64" s="130"/>
+      <c r="D64" s="101"/>
       <c r="E64" s="83" t="s">
         <v>146</v>
       </c>
@@ -6130,10 +6131,10 @@
       </c>
     </row>
     <row r="65" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A65" s="128"/>
-      <c r="B65" s="108"/>
-      <c r="C65" s="111"/>
-      <c r="D65" s="108"/>
+      <c r="A65" s="127"/>
+      <c r="B65" s="101"/>
+      <c r="C65" s="130"/>
+      <c r="D65" s="101"/>
       <c r="E65" s="93" t="s">
         <v>148</v>
       </c>
@@ -6158,10 +6159,10 @@
       </c>
     </row>
     <row r="66" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A66" s="129"/>
-      <c r="B66" s="109"/>
-      <c r="C66" s="112"/>
-      <c r="D66" s="109"/>
+      <c r="A66" s="128"/>
+      <c r="B66" s="102"/>
+      <c r="C66" s="131"/>
+      <c r="D66" s="102"/>
       <c r="E66" s="93" t="s">
         <v>205</v>
       </c>
@@ -6186,16 +6187,16 @@
       </c>
     </row>
     <row r="67" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A67" s="116" t="s">
+      <c r="A67" s="138" t="s">
         <v>149</v>
       </c>
-      <c r="B67" s="107" t="s">
+      <c r="B67" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="110" t="s">
+      <c r="C67" s="129" t="s">
         <v>150</v>
       </c>
-      <c r="D67" s="114"/>
+      <c r="D67" s="136"/>
       <c r="E67" s="60" t="s">
         <v>151</v>
       </c>
@@ -6223,10 +6224,10 @@
       </c>
     </row>
     <row r="68" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A68" s="116"/>
-      <c r="B68" s="108"/>
-      <c r="C68" s="111"/>
-      <c r="D68" s="121"/>
+      <c r="A68" s="138"/>
+      <c r="B68" s="101"/>
+      <c r="C68" s="130"/>
+      <c r="D68" s="143"/>
       <c r="E68" s="60" t="s">
         <v>154</v>
       </c>
@@ -6254,10 +6255,10 @@
       </c>
     </row>
     <row r="69" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A69" s="116"/>
-      <c r="B69" s="108"/>
-      <c r="C69" s="111"/>
-      <c r="D69" s="121"/>
+      <c r="A69" s="138"/>
+      <c r="B69" s="101"/>
+      <c r="C69" s="130"/>
+      <c r="D69" s="143"/>
       <c r="E69" s="60" t="s">
         <v>156</v>
       </c>
@@ -6285,10 +6286,10 @@
       </c>
     </row>
     <row r="70" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A70" s="116"/>
-      <c r="B70" s="119"/>
-      <c r="C70" s="120"/>
-      <c r="D70" s="122"/>
+      <c r="A70" s="138"/>
+      <c r="B70" s="141"/>
+      <c r="C70" s="142"/>
+      <c r="D70" s="144"/>
       <c r="E70" s="60" t="s">
         <v>202</v>
       </c>
@@ -6314,19 +6315,19 @@
       </c>
     </row>
     <row r="71" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A71" s="118" t="s">
+      <c r="A71" s="140" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="118"/>
-      <c r="C71" s="118"/>
-      <c r="D71" s="118"/>
-      <c r="E71" s="118"/>
-      <c r="F71" s="118"/>
-      <c r="G71" s="118"/>
-      <c r="H71" s="118"/>
-      <c r="I71" s="118"/>
-      <c r="J71" s="118"/>
-      <c r="K71" s="118"/>
+      <c r="B71" s="140"/>
+      <c r="C71" s="140"/>
+      <c r="D71" s="140"/>
+      <c r="E71" s="140"/>
+      <c r="F71" s="140"/>
+      <c r="G71" s="140"/>
+      <c r="H71" s="140"/>
+      <c r="I71" s="140"/>
+      <c r="J71" s="140"/>
+      <c r="K71" s="140"/>
       <c r="L71" s="57"/>
       <c r="M71" s="25"/>
       <c r="N71" s="25"/>
@@ -6441,8 +6442,7 @@
         <v>139</v>
       </c>
       <c r="L74" s="39">
-        <f>AVERAGE(L78,L82,L85)</f>
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="M74" s="25"/>
       <c r="N74" s="25"/>
@@ -6481,7 +6481,7 @@
         <v>139</v>
       </c>
       <c r="L75" s="38">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="76" spans="1:22" s="25" customFormat="1" ht="24.75" customHeight="1">
@@ -6510,7 +6510,7 @@
         <v>139</v>
       </c>
       <c r="L76" s="38">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="77" spans="1:22" s="25" customFormat="1" ht="20.25" customHeight="1">
@@ -6539,7 +6539,7 @@
         <v>139</v>
       </c>
       <c r="L77" s="38">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="78" spans="1:22" s="25" customFormat="1" ht="24.75" customHeight="1">
@@ -6569,7 +6569,7 @@
       </c>
       <c r="L78" s="40">
         <f>AVERAGE(L79:L81)</f>
-        <v>0</v>
+        <v>1.6666666666666666E-2</v>
       </c>
     </row>
     <row r="79" spans="1:22" s="25" customFormat="1" ht="21.75" customHeight="1">
@@ -6598,7 +6598,7 @@
         <v>139</v>
       </c>
       <c r="L79" s="38">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="80" spans="1:22" s="25" customFormat="1" ht="18.75" customHeight="1">
@@ -6964,19 +6964,19 @@
       <c r="V90" s="25"/>
     </row>
     <row r="91" spans="1:22" ht="25.5" customHeight="1">
-      <c r="A91" s="103" t="s">
+      <c r="A91" s="139" t="s">
         <v>179</v>
       </c>
-      <c r="B91" s="103"/>
-      <c r="C91" s="103"/>
-      <c r="D91" s="103"/>
-      <c r="E91" s="103"/>
-      <c r="F91" s="103"/>
-      <c r="G91" s="103"/>
-      <c r="H91" s="103"/>
-      <c r="I91" s="103"/>
-      <c r="J91" s="103"/>
-      <c r="K91" s="103"/>
+      <c r="B91" s="139"/>
+      <c r="C91" s="139"/>
+      <c r="D91" s="139"/>
+      <c r="E91" s="139"/>
+      <c r="F91" s="139"/>
+      <c r="G91" s="139"/>
+      <c r="H91" s="139"/>
+      <c r="I91" s="139"/>
+      <c r="J91" s="139"/>
+      <c r="K91" s="139"/>
       <c r="L91" s="38"/>
       <c r="M91" s="25"/>
       <c r="N91" s="25"/>
@@ -7155,14 +7155,60 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="A47:K47"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A71:K71"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
     <mergeCell ref="L28:L30"/>
     <mergeCell ref="D13:D17"/>
     <mergeCell ref="H28:H30"/>
@@ -7179,95 +7225,49 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="D54:D58"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A71:K71"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="A47:K47"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G20" r:id="rId1"/>
-    <hyperlink ref="G21" r:id="rId2"/>
-    <hyperlink ref="G34" r:id="rId3"/>
-    <hyperlink ref="G23" r:id="rId4"/>
-    <hyperlink ref="G12" r:id="rId5"/>
-    <hyperlink ref="G24" r:id="rId6"/>
-    <hyperlink ref="G39" r:id="rId7"/>
-    <hyperlink ref="G30" r:id="rId8"/>
-    <hyperlink ref="G33" r:id="rId9"/>
-    <hyperlink ref="G43" r:id="rId10"/>
-    <hyperlink ref="G25" r:id="rId11"/>
-    <hyperlink ref="G41" r:id="rId12"/>
-    <hyperlink ref="G44" r:id="rId13"/>
-    <hyperlink ref="G32" r:id="rId14"/>
-    <hyperlink ref="G40" r:id="rId15"/>
-    <hyperlink ref="G26:G27" r:id="rId16" display="https://github.com/antonyMontalvo/FaceSolutions/commit/8f0ec13380b96dbff2cf0f44e517515e6d8e935b"/>
-    <hyperlink ref="G63" r:id="rId17"/>
-    <hyperlink ref="G51" r:id="rId18"/>
-    <hyperlink ref="G36" r:id="rId19"/>
-    <hyperlink ref="G28:G29" r:id="rId20" display="https://github.com/antonyMontalvo/FaceSolutions/commit/b7f87017c045c76f3ed7353bf35a7680607f9adf"/>
-    <hyperlink ref="G42" r:id="rId21"/>
-    <hyperlink ref="G37" r:id="rId22"/>
-    <hyperlink ref="G50" r:id="rId23"/>
-    <hyperlink ref="G31" r:id="rId24"/>
-    <hyperlink ref="G67" r:id="rId25"/>
-    <hyperlink ref="G19" r:id="rId26"/>
-    <hyperlink ref="G35" r:id="rId27"/>
-    <hyperlink ref="G54" r:id="rId28"/>
-    <hyperlink ref="G53" r:id="rId29"/>
-    <hyperlink ref="G68" r:id="rId30"/>
-    <hyperlink ref="G64" r:id="rId31"/>
-    <hyperlink ref="G55" r:id="rId32"/>
-    <hyperlink ref="G69" r:id="rId33"/>
+    <hyperlink ref="G20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G23" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G39" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G30" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G43" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G25" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G41" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G44" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G32" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G40" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G26:G27" r:id="rId16" display="https://github.com/antonyMontalvo/FaceSolutions/commit/8f0ec13380b96dbff2cf0f44e517515e6d8e935b" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G63" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G51" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G36" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G28:G29" r:id="rId20" display="https://github.com/antonyMontalvo/FaceSolutions/commit/b7f87017c045c76f3ed7353bf35a7680607f9adf" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G42" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G37" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G50" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G31" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G67" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G19" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G35" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G54" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G53" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G68" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G64" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G55" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G69" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId34"/>
@@ -7276,7 +7276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Correcion de panel de filtros
</commit_message>
<xml_diff>
--- a/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
+++ b/desarrollo/FRSIAAATR/Gestión/FRSIAAATR_C.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antony\Desktop\Repo\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antony\Desktop\Repositorio\FaceSolutions\desarrollo\FRSIAAATR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C83EA8E-8CBC-48A6-963B-70E1667F20C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3172231-2256-42FD-BBFA-CC6C6184E94B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de proyecto y Gantt" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="204">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -384,9 +384,6 @@
   </si>
   <si>
     <t>Desarrollo del backend</t>
-  </si>
-  <si>
-    <t>En proceso</t>
   </si>
   <si>
     <t>Implementar algoritmo de reconocimiento facial.</t>
@@ -451,9 +448,6 @@
     <t>Generación de la constancia de ingreso digital</t>
   </si>
   <si>
-    <t>Sin empezar</t>
-  </si>
-  <si>
     <t>Desarrollo del frontend</t>
   </si>
   <si>
@@ -681,7 +675,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;S/&quot;\ #,##0.00;[Red]&quot;S/&quot;\ \-#,##0.00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -779,14 +773,6 @@
       <b/>
       <sz val="16"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1107,10 +1093,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1199,9 +1185,6 @@
     <xf numFmtId="9" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1241,16 +1224,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1259,37 +1239,34 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1301,23 +1278,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1341,7 +1315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1359,12 +1333,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1374,7 +1369,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1385,141 +1494,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4001,8 +3975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4025,21 +3999,21 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="149" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
+      <c r="B2" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
@@ -4053,15 +4027,15 @@
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -4081,15 +4055,15 @@
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="150" t="s">
+      <c r="B4" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="150"/>
-      <c r="D4" s="150"/>
-      <c r="E4" s="150"/>
-      <c r="F4" s="150"/>
-      <c r="G4" s="150"/>
-      <c r="H4" s="150"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -4109,15 +4083,15 @@
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="151" t="s">
+      <c r="B5" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="151"/>
-      <c r="D5" s="151"/>
-      <c r="E5" s="151"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="151"/>
-      <c r="H5" s="151"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -4320,13 +4294,13 @@
       <c r="B12" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="49" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="67" t="s">
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="64" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="27">
@@ -4364,10 +4338,10 @@
       <c r="B13" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="111"/>
+      <c r="D13" s="138"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26" t="s">
         <v>26</v>
@@ -4403,70 +4377,70 @@
       <c r="V13" s="25"/>
     </row>
     <row r="14" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A14" s="120" t="s">
+      <c r="A14" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="116" t="s">
+      <c r="B14" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="112"/>
-      <c r="E14" s="89" t="s">
+      <c r="D14" s="139"/>
+      <c r="E14" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="86" t="s">
+      <c r="F14" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="86" t="s">
+      <c r="G14" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="50">
+      <c r="H14" s="49">
         <v>44006</v>
       </c>
-      <c r="I14" s="50">
+      <c r="I14" s="49">
         <v>44008</v>
       </c>
-      <c r="J14" s="89">
+      <c r="J14" s="85">
         <f>I14-H14</f>
         <v>2</v>
       </c>
-      <c r="K14" s="64" t="s">
+      <c r="K14" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="51">
+      <c r="L14" s="50">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:22" s="25" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A15" s="121"/>
-      <c r="B15" s="118"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="89" t="s">
+      <c r="A15" s="133"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="129"/>
+      <c r="D15" s="139"/>
+      <c r="E15" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="86" t="s">
+      <c r="F15" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="89" t="s">
+      <c r="G15" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="50">
+      <c r="H15" s="49">
         <v>44007</v>
       </c>
-      <c r="I15" s="50">
+      <c r="I15" s="49">
         <v>44008</v>
       </c>
-      <c r="J15" s="89">
+      <c r="J15" s="85">
         <f>I15-H15</f>
         <v>1</v>
       </c>
-      <c r="K15" s="64" t="s">
+      <c r="K15" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="51">
+      <c r="L15" s="50">
         <v>1</v>
       </c>
     </row>
@@ -4477,14 +4451,14 @@
       <c r="B16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="112"/>
-      <c r="E16" s="43" t="s">
+      <c r="D16" s="139"/>
+      <c r="E16" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="43" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="26" t="s">
@@ -4499,7 +4473,7 @@
       <c r="J16" s="26">
         <v>1</v>
       </c>
-      <c r="K16" s="61" t="s">
+      <c r="K16" s="59" t="s">
         <v>24</v>
       </c>
       <c r="L16" s="38">
@@ -4513,11 +4487,11 @@
       <c r="B17" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="113"/>
-      <c r="E17" s="44" t="s">
+      <c r="D17" s="140"/>
+      <c r="E17" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F17" s="26" t="s">
@@ -4536,7 +4510,7 @@
         <f>I17-H17</f>
         <v>6</v>
       </c>
-      <c r="K17" s="61" t="s">
+      <c r="K17" s="59" t="s">
         <v>24</v>
       </c>
       <c r="L17" s="38">
@@ -4547,12 +4521,12 @@
       <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="104"/>
-      <c r="C18" s="105"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="106"/>
+      <c r="B18" s="145"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="146"/>
+      <c r="F18" s="146"/>
+      <c r="G18" s="147"/>
       <c r="H18" s="27">
         <v>44008</v>
       </c>
@@ -4582,31 +4556,31 @@
       <c r="V18" s="25"/>
     </row>
     <row r="19" spans="1:22" s="25" customFormat="1" ht="36" customHeight="1">
-      <c r="A19" s="107" t="s">
+      <c r="A19" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="129" t="s">
+      <c r="C19" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="100" t="s">
+      <c r="D19" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="88" t="s">
+      <c r="E19" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="80" t="s">
+      <c r="G19" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="45">
+      <c r="H19" s="44">
         <v>44008</v>
       </c>
-      <c r="I19" s="45">
+      <c r="I19" s="44">
         <v>44013</v>
       </c>
       <c r="J19" s="26">
@@ -4620,23 +4594,23 @@
       </c>
     </row>
     <row r="20" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="108"/>
-      <c r="B20" s="101"/>
-      <c r="C20" s="130"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="60" t="s">
+      <c r="A20" s="101"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="86" t="s">
+      <c r="F20" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="65" t="s">
+      <c r="G20" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="45">
+      <c r="H20" s="44">
         <v>44008</v>
       </c>
-      <c r="I20" s="45">
+      <c r="I20" s="44">
         <v>44013</v>
       </c>
       <c r="J20" s="26">
@@ -4650,55 +4624,55 @@
       </c>
     </row>
     <row r="21" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A21" s="109"/>
-      <c r="B21" s="102"/>
-      <c r="C21" s="131"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="49" t="s">
+      <c r="A21" s="102"/>
+      <c r="B21" s="105"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="67" t="s">
+      <c r="G21" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="45">
+      <c r="H21" s="44">
         <v>44008</v>
       </c>
-      <c r="I21" s="45">
+      <c r="I21" s="44">
         <v>44013</v>
       </c>
-      <c r="J21" s="44">
+      <c r="J21" s="43">
         <f t="shared" ref="J21:J26" si="0">I21-H21</f>
         <v>5</v>
       </c>
-      <c r="K21" s="46" t="s">
+      <c r="K21" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="L21" s="47">
-        <v>1</v>
-      </c>
-      <c r="N21" s="48"/>
+      <c r="L21" s="46">
+        <v>1</v>
+      </c>
+      <c r="N21" s="47"/>
     </row>
     <row r="22" spans="1:22" ht="29.25" customHeight="1">
       <c r="A22" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="43" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="26"/>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="44" t="s">
+      <c r="F22" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="44" t="s">
+      <c r="G22" s="43" t="s">
         <v>27</v>
       </c>
       <c r="H22" s="27">
@@ -4729,25 +4703,25 @@
       <c r="V22" s="25"/>
     </row>
     <row r="23" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A23" s="107" t="s">
+      <c r="A23" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="122" t="s">
+      <c r="B23" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="122" t="s">
+      <c r="C23" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="100" t="s">
+      <c r="D23" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="44" t="s">
+      <c r="F23" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="67" t="s">
+      <c r="G23" s="64" t="s">
         <v>55</v>
       </c>
       <c r="H23" s="27">
@@ -4768,17 +4742,17 @@
       </c>
     </row>
     <row r="24" spans="1:22" s="25" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A24" s="108"/>
-      <c r="B24" s="122"/>
-      <c r="C24" s="122"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="88" t="s">
+      <c r="A24" s="101"/>
+      <c r="B24" s="109"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="67" t="s">
+      <c r="G24" s="64" t="s">
         <v>57</v>
       </c>
       <c r="H24" s="27">
@@ -4799,33 +4773,33 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="52.5" customHeight="1">
-      <c r="A25" s="108"/>
-      <c r="B25" s="122"/>
-      <c r="C25" s="122"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="83" t="s">
+      <c r="A25" s="101"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="104"/>
+      <c r="E25" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="83" t="s">
+      <c r="F25" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="72" t="s">
+      <c r="G25" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="H25" s="52">
+      <c r="H25" s="51">
         <v>44008</v>
       </c>
-      <c r="I25" s="52">
+      <c r="I25" s="51">
         <v>44013</v>
       </c>
-      <c r="J25" s="90">
+      <c r="J25" s="86">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="K25" s="53" t="s">
+      <c r="K25" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="54">
+      <c r="L25" s="53">
         <v>1</v>
       </c>
       <c r="M25" s="25"/>
@@ -4840,63 +4814,63 @@
       <c r="V25" s="25"/>
     </row>
     <row r="26" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A26" s="124" t="s">
+      <c r="A26" s="134" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="116" t="s">
+      <c r="B26" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="116" t="s">
+      <c r="C26" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="118" t="s">
+      <c r="D26" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="89" t="s">
+      <c r="E26" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="116" t="s">
+      <c r="F26" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="103" t="s">
+      <c r="G26" s="144" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="115">
+      <c r="H26" s="142">
         <v>44012</v>
       </c>
-      <c r="I26" s="115">
+      <c r="I26" s="142">
         <v>44013</v>
       </c>
-      <c r="J26" s="118">
+      <c r="J26" s="128">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K26" s="117" t="s">
+      <c r="K26" s="143" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="110">
-        <v>1</v>
-      </c>
-      <c r="M26" s="66"/>
-      <c r="N26" s="48"/>
+      <c r="L26" s="137">
+        <v>1</v>
+      </c>
+      <c r="M26" s="63"/>
+      <c r="N26" s="47"/>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
-      <c r="A27" s="125"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="119"/>
-      <c r="E27" s="91" t="s">
+      <c r="A27" s="135"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="116"/>
-      <c r="G27" s="103"/>
-      <c r="H27" s="115"/>
-      <c r="I27" s="115"/>
-      <c r="J27" s="119"/>
-      <c r="K27" s="117"/>
-      <c r="L27" s="110"/>
-      <c r="M27" s="66"/>
-      <c r="N27" s="48"/>
+      <c r="F27" s="113"/>
+      <c r="G27" s="144"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="136"/>
+      <c r="K27" s="143"/>
+      <c r="L27" s="137"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="47"/>
       <c r="O27" s="25"/>
       <c r="P27" s="25"/>
       <c r="Q27" s="25"/>
@@ -4907,85 +4881,85 @@
       <c r="V27" s="25"/>
     </row>
     <row r="28" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A28" s="107" t="s">
+      <c r="A28" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="116" t="s">
+      <c r="B28" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="116" t="s">
+      <c r="C28" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="116" t="s">
+      <c r="D28" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="89" t="s">
+      <c r="E28" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="91" t="s">
+      <c r="F28" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="103" t="s">
+      <c r="G28" s="144" t="s">
         <v>68</v>
       </c>
-      <c r="H28" s="114">
+      <c r="H28" s="141">
         <v>44010</v>
       </c>
-      <c r="I28" s="115">
+      <c r="I28" s="142">
         <v>44013</v>
       </c>
-      <c r="J28" s="116">
+      <c r="J28" s="113">
         <f>I28-H28</f>
         <v>3</v>
       </c>
-      <c r="K28" s="117" t="s">
+      <c r="K28" s="143" t="s">
         <v>24</v>
       </c>
-      <c r="L28" s="110">
-        <v>1</v>
-      </c>
-      <c r="N28" s="48"/>
+      <c r="L28" s="137">
+        <v>1</v>
+      </c>
+      <c r="N28" s="47"/>
     </row>
     <row r="29" spans="1:22" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A29" s="108"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="116"/>
-      <c r="D29" s="116"/>
-      <c r="E29" s="91" t="s">
+      <c r="A29" s="101"/>
+      <c r="B29" s="113"/>
+      <c r="C29" s="113"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="70" t="s">
+      <c r="F29" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="103"/>
-      <c r="H29" s="114"/>
-      <c r="I29" s="115"/>
-      <c r="J29" s="116"/>
-      <c r="K29" s="117"/>
-      <c r="L29" s="110"/>
-      <c r="N29" s="48"/>
+      <c r="G29" s="144"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="142"/>
+      <c r="J29" s="113"/>
+      <c r="K29" s="143"/>
+      <c r="L29" s="137"/>
+      <c r="N29" s="47"/>
     </row>
     <row r="30" spans="1:22" ht="30" customHeight="1">
-      <c r="A30" s="109"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
+      <c r="A30" s="102"/>
+      <c r="B30" s="113"/>
+      <c r="C30" s="113"/>
+      <c r="D30" s="113"/>
       <c r="E30" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="44" t="s">
+      <c r="F30" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="G30" s="71" t="s">
+      <c r="G30" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="H30" s="114"/>
-      <c r="I30" s="115"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="117"/>
-      <c r="L30" s="110"/>
+      <c r="H30" s="141"/>
+      <c r="I30" s="142"/>
+      <c r="J30" s="113"/>
+      <c r="K30" s="143"/>
+      <c r="L30" s="137"/>
       <c r="M30" s="25"/>
-      <c r="N30" s="48"/>
+      <c r="N30" s="47"/>
       <c r="O30" s="25"/>
       <c r="P30" s="25"/>
       <c r="Q30" s="25"/>
@@ -4996,38 +4970,38 @@
       <c r="V30" s="25"/>
     </row>
     <row r="31" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A31" s="107" t="s">
+      <c r="A31" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="103" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="129" t="s">
+      <c r="C31" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="100" t="s">
+      <c r="D31" s="103" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="55" t="s">
         <v>76</v>
       </c>
       <c r="F31" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="68" t="s">
+      <c r="G31" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="H31" s="45">
+      <c r="H31" s="44">
         <v>44019</v>
       </c>
-      <c r="I31" s="45">
+      <c r="I31" s="44">
         <v>44022</v>
       </c>
-      <c r="J31" s="44">
+      <c r="J31" s="43">
         <f>I31-H31</f>
         <v>3</v>
       </c>
-      <c r="K31" s="46" t="s">
+      <c r="K31" s="45" t="s">
         <v>24</v>
       </c>
       <c r="L31" s="38">
@@ -5035,29 +5009,29 @@
       </c>
     </row>
     <row r="32" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A32" s="108"/>
-      <c r="B32" s="101"/>
-      <c r="C32" s="130"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="44" t="s">
+      <c r="A32" s="101"/>
+      <c r="B32" s="104"/>
+      <c r="C32" s="107"/>
+      <c r="D32" s="104"/>
+      <c r="E32" s="43" t="s">
         <v>78</v>
       </c>
       <c r="F32" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="68" t="s">
+      <c r="G32" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="H32" s="75">
+      <c r="H32" s="72">
         <v>44019</v>
       </c>
-      <c r="I32" s="75">
+      <c r="I32" s="72">
         <v>44022</v>
       </c>
-      <c r="J32" s="44">
+      <c r="J32" s="43">
         <v>3</v>
       </c>
-      <c r="K32" s="46" t="s">
+      <c r="K32" s="45" t="s">
         <v>24</v>
       </c>
       <c r="L32" s="38">
@@ -5065,30 +5039,30 @@
       </c>
     </row>
     <row r="33" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A33" s="108"/>
-      <c r="B33" s="101"/>
-      <c r="C33" s="130"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="44" t="s">
+      <c r="A33" s="101"/>
+      <c r="B33" s="104"/>
+      <c r="C33" s="107"/>
+      <c r="D33" s="104"/>
+      <c r="E33" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="86" t="s">
+      <c r="F33" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="65" t="s">
+      <c r="G33" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="H33" s="45">
+      <c r="H33" s="44">
         <v>44019</v>
       </c>
-      <c r="I33" s="45">
+      <c r="I33" s="44">
         <v>44022</v>
       </c>
-      <c r="J33" s="44">
+      <c r="J33" s="43">
         <f>I33-H33</f>
         <v>3</v>
       </c>
-      <c r="K33" s="46" t="s">
+      <c r="K33" s="45" t="s">
         <v>24</v>
       </c>
       <c r="L33" s="38">
@@ -5096,30 +5070,30 @@
       </c>
     </row>
     <row r="34" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A34" s="108"/>
-      <c r="B34" s="101"/>
-      <c r="C34" s="130"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="44" t="s">
+      <c r="A34" s="101"/>
+      <c r="B34" s="104"/>
+      <c r="C34" s="107"/>
+      <c r="D34" s="104"/>
+      <c r="E34" s="43" t="s">
         <v>82</v>
       </c>
       <c r="F34" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="G34" s="68" t="s">
+      <c r="G34" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="45">
+      <c r="H34" s="44">
         <v>44019</v>
       </c>
-      <c r="I34" s="45">
+      <c r="I34" s="44">
         <v>44022</v>
       </c>
-      <c r="J34" s="44">
+      <c r="J34" s="43">
         <f>I34-H34</f>
         <v>3</v>
       </c>
-      <c r="K34" s="46" t="s">
+      <c r="K34" s="45" t="s">
         <v>24</v>
       </c>
       <c r="L34" s="38">
@@ -5127,30 +5101,30 @@
       </c>
     </row>
     <row r="35" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A35" s="108"/>
-      <c r="B35" s="101"/>
-      <c r="C35" s="130"/>
-      <c r="D35" s="101"/>
-      <c r="E35" s="44" t="s">
+      <c r="A35" s="101"/>
+      <c r="B35" s="104"/>
+      <c r="C35" s="107"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="44" t="s">
+      <c r="F35" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="G35" s="80" t="s">
+      <c r="G35" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="H35" s="45">
+      <c r="H35" s="44">
         <v>44019</v>
       </c>
-      <c r="I35" s="45">
+      <c r="I35" s="44">
         <v>44022</v>
       </c>
-      <c r="J35" s="44">
+      <c r="J35" s="43">
         <f>I35-H35</f>
         <v>3</v>
       </c>
-      <c r="K35" s="46" t="s">
+      <c r="K35" s="45" t="s">
         <v>24</v>
       </c>
       <c r="L35" s="38">
@@ -5158,33 +5132,33 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="33" customHeight="1">
-      <c r="A36" s="109"/>
-      <c r="B36" s="102"/>
-      <c r="C36" s="131"/>
-      <c r="D36" s="102"/>
-      <c r="E36" s="44" t="s">
+      <c r="A36" s="102"/>
+      <c r="B36" s="105"/>
+      <c r="C36" s="108"/>
+      <c r="D36" s="105"/>
+      <c r="E36" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F36" s="91" t="s">
+      <c r="F36" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="74" t="s">
+      <c r="G36" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="H36" s="45">
+      <c r="H36" s="44">
         <v>44019</v>
       </c>
-      <c r="I36" s="45">
+      <c r="I36" s="44">
         <v>44022</v>
       </c>
-      <c r="J36" s="44">
+      <c r="J36" s="43">
         <f>I36-H36</f>
         <v>3</v>
       </c>
-      <c r="K36" s="46" t="s">
+      <c r="K36" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="L36" s="47">
+      <c r="L36" s="46">
         <v>1</v>
       </c>
       <c r="M36" s="25"/>
@@ -5202,22 +5176,22 @@
       <c r="A37" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="44" t="s">
+      <c r="C37" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="44" t="s">
+      <c r="D37" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="44" t="s">
+      <c r="E37" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="F37" s="44" t="s">
+      <c r="F37" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="68" t="s">
+      <c r="G37" s="65" t="s">
         <v>91</v>
       </c>
       <c r="H37" s="27" t="s">
@@ -5240,12 +5214,12 @@
       <c r="A38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="104"/>
-      <c r="C38" s="105"/>
-      <c r="D38" s="105"/>
-      <c r="E38" s="105"/>
-      <c r="F38" s="105"/>
-      <c r="G38" s="106"/>
+      <c r="B38" s="145"/>
+      <c r="C38" s="146"/>
+      <c r="D38" s="146"/>
+      <c r="E38" s="146"/>
+      <c r="F38" s="146"/>
+      <c r="G38" s="147"/>
       <c r="H38" s="27">
         <v>43837</v>
       </c>
@@ -5263,7 +5237,7 @@
         <v>1</v>
       </c>
       <c r="M38" s="25"/>
-      <c r="N38" s="48"/>
+      <c r="N38" s="47"/>
       <c r="O38" s="25"/>
       <c r="P38" s="25"/>
       <c r="Q38" s="25"/>
@@ -5274,23 +5248,23 @@
       <c r="V38" s="25"/>
     </row>
     <row r="39" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A39" s="100" t="s">
+      <c r="A39" s="103" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="100" t="s">
+      <c r="B39" s="103" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="100"/>
-      <c r="D39" s="100" t="s">
+      <c r="C39" s="103"/>
+      <c r="D39" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="E39" s="62" t="s">
+      <c r="E39" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="F39" s="44" t="s">
+      <c r="F39" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="68" t="s">
+      <c r="G39" s="65" t="s">
         <v>99</v>
       </c>
       <c r="H39" s="27">
@@ -5308,20 +5282,20 @@
       <c r="L39" s="38">
         <v>1</v>
       </c>
-      <c r="N39" s="48"/>
+      <c r="N39" s="47"/>
     </row>
     <row r="40" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
-      <c r="C40" s="101"/>
-      <c r="D40" s="101"/>
-      <c r="E40" s="49" t="s">
+      <c r="A40" s="104"/>
+      <c r="B40" s="104"/>
+      <c r="C40" s="104"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="48" t="s">
         <v>100</v>
       </c>
       <c r="F40" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G40" s="68" t="s">
+      <c r="G40" s="65" t="s">
         <v>101</v>
       </c>
       <c r="H40" s="27">
@@ -5339,20 +5313,20 @@
       <c r="L40" s="38">
         <v>1</v>
       </c>
-      <c r="N40" s="48"/>
+      <c r="N40" s="47"/>
     </row>
     <row r="41" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A41" s="101"/>
-      <c r="B41" s="101"/>
-      <c r="C41" s="101"/>
-      <c r="D41" s="101"/>
-      <c r="E41" s="49" t="s">
+      <c r="A41" s="104"/>
+      <c r="B41" s="104"/>
+      <c r="C41" s="104"/>
+      <c r="D41" s="104"/>
+      <c r="E41" s="48" t="s">
         <v>102</v>
       </c>
       <c r="F41" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="67" t="s">
+      <c r="G41" s="64" t="s">
         <v>103</v>
       </c>
       <c r="H41" s="27">
@@ -5370,20 +5344,20 @@
       <c r="L41" s="38">
         <v>1</v>
       </c>
-      <c r="N41" s="48"/>
+      <c r="N41" s="47"/>
     </row>
     <row r="42" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A42" s="101"/>
-      <c r="B42" s="101"/>
-      <c r="C42" s="101"/>
-      <c r="D42" s="101"/>
-      <c r="E42" s="62" t="s">
+      <c r="A42" s="104"/>
+      <c r="B42" s="104"/>
+      <c r="C42" s="104"/>
+      <c r="D42" s="104"/>
+      <c r="E42" s="60" t="s">
         <v>104</v>
       </c>
       <c r="F42" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="G42" s="67" t="s">
+      <c r="G42" s="64" t="s">
         <v>105</v>
       </c>
       <c r="H42" s="27">
@@ -5401,20 +5375,20 @@
       <c r="L42" s="38">
         <v>1</v>
       </c>
-      <c r="N42" s="48"/>
+      <c r="N42" s="47"/>
     </row>
     <row r="43" spans="1:22" s="25" customFormat="1" ht="30.6" customHeight="1">
-      <c r="A43" s="102"/>
-      <c r="B43" s="102"/>
-      <c r="C43" s="102"/>
-      <c r="D43" s="102"/>
-      <c r="E43" s="43" t="s">
+      <c r="A43" s="105"/>
+      <c r="B43" s="105"/>
+      <c r="C43" s="105"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="42" t="s">
         <v>106</v>
       </c>
       <c r="F43" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="G43" s="68" t="s">
+      <c r="G43" s="65" t="s">
         <v>107</v>
       </c>
       <c r="H43" s="27">
@@ -5432,28 +5406,28 @@
       <c r="L43" s="38">
         <v>1</v>
       </c>
-      <c r="N43" s="48"/>
+      <c r="N43" s="47"/>
     </row>
     <row r="44" spans="1:22" ht="49.5" customHeight="1">
       <c r="A44" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="44" t="s">
+      <c r="C44" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="E44" s="49" t="s">
+      <c r="E44" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F44" s="44" t="s">
+      <c r="F44" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="G44" s="73" t="s">
+      <c r="G44" s="70" t="s">
         <v>112</v>
       </c>
       <c r="H44" s="27">
@@ -5473,7 +5447,7 @@
         <v>1</v>
       </c>
       <c r="M44" s="25"/>
-      <c r="N44" s="48"/>
+      <c r="N44" s="47"/>
       <c r="O44" s="25"/>
       <c r="P44" s="25"/>
       <c r="Q44" s="25"/>
@@ -5484,31 +5458,31 @@
       <c r="V44" s="25"/>
     </row>
     <row r="45" spans="1:22" s="25" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A45" s="107" t="s">
+      <c r="A45" s="100" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="100" t="s">
+      <c r="B45" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="129" t="s">
+      <c r="C45" s="106" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="107" t="s">
+      <c r="D45" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="43" t="s">
+      <c r="E45" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="F45" s="87" t="s">
+      <c r="F45" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="G45" s="87" t="s">
+      <c r="G45" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="H45" s="45">
+      <c r="H45" s="44">
         <v>44024</v>
       </c>
-      <c r="I45" s="45">
+      <c r="I45" s="44">
         <v>44024</v>
       </c>
       <c r="J45" s="26">
@@ -5520,36 +5494,36 @@
       <c r="L45" s="38">
         <v>1</v>
       </c>
-      <c r="N45" s="48"/>
+      <c r="N45" s="47"/>
     </row>
     <row r="46" spans="1:22" ht="46.5" customHeight="1">
-      <c r="A46" s="109"/>
-      <c r="B46" s="102"/>
-      <c r="C46" s="131"/>
-      <c r="D46" s="109"/>
-      <c r="E46" s="89" t="s">
+      <c r="A46" s="102"/>
+      <c r="B46" s="105"/>
+      <c r="C46" s="108"/>
+      <c r="D46" s="102"/>
+      <c r="E46" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="F46" s="87" t="s">
+      <c r="F46" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="G46" s="87" t="s">
+      <c r="G46" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="H46" s="45">
+      <c r="H46" s="44">
         <v>44027</v>
       </c>
-      <c r="I46" s="45">
+      <c r="I46" s="44">
         <v>44029</v>
       </c>
-      <c r="J46" s="44">
+      <c r="J46" s="43">
         <f>I46-H46</f>
         <v>2</v>
       </c>
-      <c r="K46" s="46" t="s">
+      <c r="K46" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="L46" s="47">
+      <c r="L46" s="46">
         <v>1</v>
       </c>
       <c r="M46" s="25"/>
@@ -5564,19 +5538,19 @@
       <c r="V46" s="25"/>
     </row>
     <row r="47" spans="1:22" ht="30.75" customHeight="1">
-      <c r="A47" s="139" t="s">
+      <c r="A47" s="99" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="139"/>
-      <c r="C47" s="139"/>
-      <c r="D47" s="139"/>
-      <c r="E47" s="139"/>
-      <c r="F47" s="139"/>
-      <c r="G47" s="139"/>
-      <c r="H47" s="139"/>
-      <c r="I47" s="139"/>
-      <c r="J47" s="139"/>
-      <c r="K47" s="139"/>
+      <c r="B47" s="99"/>
+      <c r="C47" s="99"/>
+      <c r="D47" s="99"/>
+      <c r="E47" s="99"/>
+      <c r="F47" s="99"/>
+      <c r="G47" s="99"/>
+      <c r="H47" s="99"/>
+      <c r="I47" s="99"/>
+      <c r="J47" s="99"/>
+      <c r="K47" s="99"/>
       <c r="L47" s="38"/>
       <c r="M47" s="25"/>
       <c r="N47" s="25"/>
@@ -5612,7 +5586,7 @@
       <c r="K48" s="28"/>
       <c r="L48" s="39">
         <f>AVERAGE(L49,L62)</f>
-        <v>0.93166666666666664</v>
+        <v>0.94166666666666665</v>
       </c>
     </row>
     <row r="49" spans="1:22" s="25" customFormat="1" ht="27" customHeight="1">
@@ -5637,8 +5611,8 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="K49" s="42" t="s">
-        <v>121</v>
+      <c r="K49" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L49" s="40">
         <f>AVERAGE(L50:L61)</f>
@@ -5646,24 +5620,24 @@
       </c>
     </row>
     <row r="50" spans="1:22" ht="38.25" customHeight="1">
-      <c r="A50" s="132" t="s">
+      <c r="A50" s="126" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" s="113" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="106" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="116" t="s">
+      <c r="D50" s="110"/>
+      <c r="E50" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="F50" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="129" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" s="136"/>
-      <c r="E50" s="44" t="s">
+      <c r="G50" s="71" t="s">
         <v>124</v>
-      </c>
-      <c r="F50" s="91" t="s">
-        <v>60</v>
-      </c>
-      <c r="G50" s="74" t="s">
-        <v>125</v>
       </c>
       <c r="H50" s="27">
         <v>44029</v>
@@ -5693,18 +5667,18 @@
       <c r="V50" s="25"/>
     </row>
     <row r="51" spans="1:22" s="25" customFormat="1" ht="45" customHeight="1">
-      <c r="A51" s="132"/>
-      <c r="B51" s="116"/>
-      <c r="C51" s="131"/>
-      <c r="D51" s="137"/>
-      <c r="E51" s="49" t="s">
+      <c r="A51" s="126"/>
+      <c r="B51" s="113"/>
+      <c r="C51" s="108"/>
+      <c r="D51" s="111"/>
+      <c r="E51" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="F51" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51" s="80" t="s">
         <v>126</v>
-      </c>
-      <c r="F51" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="G51" s="84" t="s">
-        <v>127</v>
       </c>
       <c r="H51" s="27">
         <v>44029</v>
@@ -5724,295 +5698,295 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A52" s="138" t="s">
+      <c r="A52" s="112" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="113" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="D52" s="113"/>
+      <c r="E52" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="116" t="s">
+      <c r="F52" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="122" t="s">
-        <v>123</v>
-      </c>
-      <c r="D52" s="116"/>
-      <c r="E52" s="87" t="s">
-        <v>129</v>
-      </c>
-      <c r="F52" s="91" t="s">
-        <v>60</v>
-      </c>
-      <c r="G52" s="85" t="s">
+      <c r="G52" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="H52" s="50">
+      <c r="H52" s="49">
         <v>44029</v>
       </c>
-      <c r="I52" s="50">
+      <c r="I52" s="49">
         <v>44043</v>
       </c>
-      <c r="J52" s="89">
+      <c r="J52" s="85">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="K52" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="L52" s="51">
+      <c r="K52" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L52" s="50">
         <v>0.9</v>
       </c>
     </row>
     <row r="53" spans="1:22" s="25" customFormat="1" ht="57" customHeight="1">
-      <c r="A53" s="138"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="122"/>
-      <c r="D53" s="116"/>
-      <c r="E53" s="87" t="s">
+      <c r="A53" s="112"/>
+      <c r="B53" s="113"/>
+      <c r="C53" s="109"/>
+      <c r="D53" s="113"/>
+      <c r="E53" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="F53" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="G53" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="F53" s="86" t="s">
-        <v>109</v>
-      </c>
-      <c r="G53" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="H53" s="76">
+      <c r="H53" s="73">
         <v>44036</v>
       </c>
-      <c r="I53" s="76">
+      <c r="I53" s="73">
         <v>44043</v>
       </c>
-      <c r="J53" s="77">
+      <c r="J53" s="74">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K53" s="78" t="s">
-        <v>121</v>
-      </c>
-      <c r="L53" s="79">
+      <c r="K53" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L53" s="75">
         <v>0.7</v>
       </c>
     </row>
     <row r="54" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A54" s="132" t="s">
+      <c r="A54" s="126" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="113" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="116" t="s">
-        <v>60</v>
-      </c>
-      <c r="C54" s="122" t="s">
+      <c r="D54" s="130"/>
+      <c r="E54" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="134"/>
-      <c r="E54" s="87" t="s">
+      <c r="F54" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="F54" s="86" t="s">
-        <v>21</v>
-      </c>
-      <c r="G54" s="81" t="s">
-        <v>135</v>
-      </c>
-      <c r="H54" s="50">
+      <c r="H54" s="49">
         <v>44036</v>
       </c>
-      <c r="I54" s="50">
+      <c r="I54" s="49">
         <v>44043</v>
       </c>
-      <c r="J54" s="89">
+      <c r="J54" s="85">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="K54" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="L54" s="51">
+      <c r="K54" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L54" s="50">
         <v>0.9</v>
       </c>
     </row>
     <row r="55" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A55" s="132"/>
-      <c r="B55" s="116"/>
-      <c r="C55" s="122"/>
-      <c r="D55" s="134"/>
-      <c r="E55" s="95" t="s">
+      <c r="A55" s="126"/>
+      <c r="B55" s="113"/>
+      <c r="C55" s="109"/>
+      <c r="D55" s="130"/>
+      <c r="E55" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="F55" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="G55" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="F55" s="95" t="s">
-        <v>5</v>
-      </c>
-      <c r="G55" s="73" t="s">
-        <v>137</v>
-      </c>
-      <c r="H55" s="50">
+      <c r="H55" s="49">
         <v>44036</v>
       </c>
-      <c r="I55" s="50">
+      <c r="I55" s="49">
         <v>44043</v>
       </c>
-      <c r="J55" s="95">
+      <c r="J55" s="91">
         <v>7</v>
       </c>
       <c r="K55" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="L55" s="51">
+      <c r="L55" s="50">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A56" s="133"/>
-      <c r="B56" s="118"/>
-      <c r="C56" s="123"/>
-      <c r="D56" s="135"/>
-      <c r="E56" s="99" t="s">
-        <v>201</v>
-      </c>
-      <c r="F56" s="94" t="s">
+      <c r="A56" s="127"/>
+      <c r="B56" s="128"/>
+      <c r="C56" s="129"/>
+      <c r="D56" s="131"/>
+      <c r="E56" s="95" t="s">
+        <v>199</v>
+      </c>
+      <c r="F56" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="G56" s="73"/>
-      <c r="H56" s="50">
+      <c r="G56" s="70"/>
+      <c r="H56" s="49">
         <v>44043</v>
       </c>
       <c r="I56" s="27">
         <v>44057</v>
       </c>
-      <c r="J56" s="95">
+      <c r="J56" s="91">
         <v>14</v>
       </c>
       <c r="K56" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="L56" s="51">
+      <c r="L56" s="50">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:22" s="25" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A57" s="133"/>
-      <c r="B57" s="118"/>
-      <c r="C57" s="123"/>
-      <c r="D57" s="135"/>
-      <c r="E57" s="99" t="s">
-        <v>203</v>
-      </c>
-      <c r="F57" s="94" t="s">
+      <c r="A57" s="127"/>
+      <c r="B57" s="128"/>
+      <c r="C57" s="129"/>
+      <c r="D57" s="131"/>
+      <c r="E57" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="F57" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="G57" s="73"/>
-      <c r="H57" s="50">
+      <c r="G57" s="70"/>
+      <c r="H57" s="49">
         <v>44043</v>
       </c>
       <c r="I57" s="27">
         <v>44057</v>
       </c>
-      <c r="J57" s="95">
+      <c r="J57" s="91">
         <v>14</v>
       </c>
       <c r="K57" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="L57" s="51">
+      <c r="L57" s="50">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A58" s="133"/>
-      <c r="B58" s="118"/>
-      <c r="C58" s="123"/>
-      <c r="D58" s="135"/>
-      <c r="E58" s="99" t="s">
-        <v>204</v>
-      </c>
-      <c r="F58" s="95" t="s">
+      <c r="A58" s="127"/>
+      <c r="B58" s="128"/>
+      <c r="C58" s="129"/>
+      <c r="D58" s="131"/>
+      <c r="E58" s="95" t="s">
+        <v>202</v>
+      </c>
+      <c r="F58" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="73"/>
-      <c r="H58" s="50">
+      <c r="G58" s="70"/>
+      <c r="H58" s="49">
         <v>44043</v>
       </c>
       <c r="I58" s="27">
         <v>44057</v>
       </c>
-      <c r="J58" s="95">
+      <c r="J58" s="91">
         <v>14</v>
       </c>
       <c r="K58" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="L58" s="51">
+      <c r="L58" s="50">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A59" s="145" t="s">
-        <v>138</v>
-      </c>
-      <c r="B59" s="146" t="s">
+      <c r="A59" s="119" t="s">
+        <v>137</v>
+      </c>
+      <c r="B59" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="147" t="s">
-        <v>133</v>
-      </c>
-      <c r="D59" s="148"/>
-      <c r="E59" s="95" t="s">
-        <v>198</v>
-      </c>
-      <c r="F59" s="95" t="s">
+      <c r="C59" s="121" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" s="122"/>
+      <c r="E59" s="91" t="s">
+        <v>196</v>
+      </c>
+      <c r="F59" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="98"/>
-      <c r="H59" s="50">
+      <c r="G59" s="94"/>
+      <c r="H59" s="49">
         <v>44043</v>
       </c>
       <c r="I59" s="27">
         <v>44057</v>
       </c>
-      <c r="J59" s="89">
+      <c r="J59" s="85">
         <v>14</v>
       </c>
-      <c r="K59" s="63" t="s">
-        <v>121</v>
+      <c r="K59" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L59" s="38">
         <v>0.9</v>
       </c>
     </row>
     <row r="60" spans="1:22" s="25" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A60" s="145"/>
-      <c r="B60" s="146"/>
-      <c r="C60" s="147"/>
-      <c r="D60" s="148"/>
-      <c r="E60" s="95" t="s">
-        <v>199</v>
-      </c>
-      <c r="F60" s="95" t="s">
+      <c r="A60" s="119"/>
+      <c r="B60" s="120"/>
+      <c r="C60" s="121"/>
+      <c r="D60" s="122"/>
+      <c r="E60" s="91" t="s">
+        <v>197</v>
+      </c>
+      <c r="F60" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="98"/>
-      <c r="H60" s="50">
+      <c r="G60" s="94"/>
+      <c r="H60" s="49">
         <v>44043</v>
       </c>
       <c r="I60" s="27">
         <v>44057</v>
       </c>
-      <c r="J60" s="95">
+      <c r="J60" s="91">
         <v>14</v>
       </c>
-      <c r="K60" s="63" t="s">
-        <v>121</v>
+      <c r="K60" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L60" s="38">
         <v>0.9</v>
       </c>
     </row>
     <row r="61" spans="1:22" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A61" s="145"/>
-      <c r="B61" s="146"/>
-      <c r="C61" s="147"/>
-      <c r="D61" s="148"/>
-      <c r="E61" s="95" t="s">
-        <v>200</v>
-      </c>
-      <c r="F61" s="95" t="s">
+      <c r="A61" s="119"/>
+      <c r="B61" s="120"/>
+      <c r="C61" s="121"/>
+      <c r="D61" s="122"/>
+      <c r="E61" s="91" t="s">
+        <v>198</v>
+      </c>
+      <c r="F61" s="91" t="s">
         <v>5</v>
       </c>
       <c r="G61" s="26"/>
@@ -6026,8 +6000,8 @@
         <f>I61-H61</f>
         <v>5</v>
       </c>
-      <c r="K61" s="63" t="s">
-        <v>121</v>
+      <c r="K61" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L61" s="38">
         <v>0.9</v>
@@ -6035,10 +6009,10 @@
     </row>
     <row r="62" spans="1:22" s="25" customFormat="1" ht="33.75" customHeight="1">
       <c r="A62" s="34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C62" s="26"/>
       <c r="D62" s="26"/>
@@ -6055,33 +6029,33 @@
         <f>I62-H62</f>
         <v>28</v>
       </c>
-      <c r="K62" s="42" t="s">
-        <v>121</v>
+      <c r="K62" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L62" s="40">
         <f>AVERAGE(L63:L70,L72:L73)</f>
-        <v>0.92999999999999994</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="63" spans="1:22" s="25" customFormat="1" ht="42.75" customHeight="1">
-      <c r="A63" s="126" t="s">
+      <c r="A63" s="123" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" s="103" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="106" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" s="103"/>
+      <c r="E63" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="B63" s="100" t="s">
-        <v>141</v>
-      </c>
-      <c r="C63" s="129" t="s">
+      <c r="F63" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G63" s="64" t="s">
         <v>143</v>
-      </c>
-      <c r="D63" s="100"/>
-      <c r="E63" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="F63" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="G63" s="67" t="s">
-        <v>145</v>
       </c>
       <c r="H63" s="27">
         <v>44029</v>
@@ -6093,126 +6067,126 @@
         <f>I63-H63</f>
         <v>28</v>
       </c>
-      <c r="K63" s="42" t="s">
-        <v>121</v>
+      <c r="K63" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L63" s="38">
         <v>0.9</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A64" s="127"/>
-      <c r="B64" s="101"/>
-      <c r="C64" s="130"/>
-      <c r="D64" s="101"/>
-      <c r="E64" s="83" t="s">
-        <v>146</v>
-      </c>
-      <c r="F64" s="91" t="s">
-        <v>147</v>
-      </c>
-      <c r="G64" s="92" t="s">
-        <v>125</v>
-      </c>
-      <c r="H64" s="52">
+      <c r="A64" s="124"/>
+      <c r="B64" s="104"/>
+      <c r="C64" s="107"/>
+      <c r="D64" s="104"/>
+      <c r="E64" s="79" t="s">
+        <v>144</v>
+      </c>
+      <c r="F64" s="87" t="s">
+        <v>145</v>
+      </c>
+      <c r="G64" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="H64" s="51">
         <v>44030</v>
       </c>
       <c r="I64" s="27">
         <v>44057</v>
       </c>
-      <c r="J64" s="90">
+      <c r="J64" s="86">
         <v>21</v>
       </c>
-      <c r="K64" s="58" t="s">
-        <v>121</v>
+      <c r="K64" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L64" s="38">
         <v>0.95</v>
       </c>
     </row>
     <row r="65" spans="1:22" s="25" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A65" s="127"/>
-      <c r="B65" s="101"/>
-      <c r="C65" s="130"/>
-      <c r="D65" s="101"/>
-      <c r="E65" s="93" t="s">
-        <v>148</v>
-      </c>
-      <c r="F65" s="44" t="s">
+      <c r="A65" s="124"/>
+      <c r="B65" s="104"/>
+      <c r="C65" s="107"/>
+      <c r="D65" s="104"/>
+      <c r="E65" s="89" t="s">
+        <v>146</v>
+      </c>
+      <c r="F65" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="G65" s="93"/>
-      <c r="H65" s="52">
+      <c r="G65" s="89"/>
+      <c r="H65" s="51">
         <v>44030</v>
       </c>
       <c r="I65" s="27">
         <v>44057</v>
       </c>
-      <c r="J65" s="96">
+      <c r="J65" s="92">
         <v>21</v>
       </c>
-      <c r="K65" s="58" t="s">
-        <v>121</v>
+      <c r="K65" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L65" s="38">
         <v>0.95</v>
       </c>
     </row>
     <row r="66" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A66" s="128"/>
-      <c r="B66" s="102"/>
-      <c r="C66" s="131"/>
-      <c r="D66" s="102"/>
-      <c r="E66" s="93" t="s">
-        <v>205</v>
-      </c>
-      <c r="F66" s="97" t="s">
-        <v>147</v>
-      </c>
-      <c r="G66" s="83"/>
-      <c r="H66" s="52">
+      <c r="A66" s="125"/>
+      <c r="B66" s="105"/>
+      <c r="C66" s="108"/>
+      <c r="D66" s="105"/>
+      <c r="E66" s="89" t="s">
+        <v>203</v>
+      </c>
+      <c r="F66" s="93" t="s">
+        <v>145</v>
+      </c>
+      <c r="G66" s="79"/>
+      <c r="H66" s="51">
         <v>44030</v>
       </c>
       <c r="I66" s="27">
         <v>44057</v>
       </c>
-      <c r="J66" s="90">
+      <c r="J66" s="86">
         <v>21</v>
       </c>
-      <c r="K66" s="58" t="s">
-        <v>121</v>
+      <c r="K66" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L66" s="38">
         <v>0.9</v>
       </c>
     </row>
     <row r="67" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A67" s="138" t="s">
+      <c r="A67" s="112" t="s">
+        <v>147</v>
+      </c>
+      <c r="B67" s="103" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="106" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" s="110"/>
+      <c r="E67" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="B67" s="100" t="s">
-        <v>73</v>
-      </c>
-      <c r="C67" s="129" t="s">
+      <c r="F67" s="86" t="s">
         <v>150</v>
       </c>
-      <c r="D67" s="136"/>
-      <c r="E67" s="60" t="s">
+      <c r="G67" s="66" t="s">
         <v>151</v>
       </c>
-      <c r="F67" s="90" t="s">
-        <v>152</v>
-      </c>
-      <c r="G67" s="69" t="s">
-        <v>153</v>
-      </c>
-      <c r="H67" s="52">
+      <c r="H67" s="51">
         <v>44032</v>
       </c>
       <c r="I67" s="27">
         <v>44057</v>
       </c>
-      <c r="J67" s="90">
+      <c r="J67" s="86">
         <f>I67-H67</f>
         <v>25</v>
       </c>
@@ -6224,26 +6198,26 @@
       </c>
     </row>
     <row r="68" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A68" s="138"/>
-      <c r="B68" s="101"/>
-      <c r="C68" s="130"/>
-      <c r="D68" s="143"/>
-      <c r="E68" s="60" t="s">
-        <v>154</v>
-      </c>
-      <c r="F68" s="90" t="s">
+      <c r="A68" s="112"/>
+      <c r="B68" s="104"/>
+      <c r="C68" s="107"/>
+      <c r="D68" s="117"/>
+      <c r="E68" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="F68" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="G68" s="82" t="s">
-        <v>155</v>
-      </c>
-      <c r="H68" s="52">
+      <c r="G68" s="78" t="s">
+        <v>153</v>
+      </c>
+      <c r="H68" s="51">
         <v>44032</v>
       </c>
       <c r="I68" s="27">
         <v>44057</v>
       </c>
-      <c r="J68" s="90">
+      <c r="J68" s="86">
         <f>I68-H68</f>
         <v>25</v>
       </c>
@@ -6255,55 +6229,55 @@
       </c>
     </row>
     <row r="69" spans="1:22" s="25" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A69" s="138"/>
-      <c r="B69" s="101"/>
-      <c r="C69" s="130"/>
-      <c r="D69" s="143"/>
-      <c r="E69" s="60" t="s">
+      <c r="A69" s="112"/>
+      <c r="B69" s="104"/>
+      <c r="C69" s="107"/>
+      <c r="D69" s="117"/>
+      <c r="E69" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="F69" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="G69" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="F69" s="96" t="s">
-        <v>157</v>
-      </c>
-      <c r="G69" s="69" t="s">
-        <v>158</v>
-      </c>
-      <c r="H69" s="52">
+      <c r="H69" s="51">
         <v>44032</v>
       </c>
       <c r="I69" s="27">
         <v>44057</v>
       </c>
-      <c r="J69" s="96">
+      <c r="J69" s="92">
         <f>I69-H69</f>
         <v>25</v>
       </c>
-      <c r="K69" s="58" t="s">
-        <v>121</v>
+      <c r="K69" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L69" s="38">
         <v>0.8</v>
       </c>
     </row>
     <row r="70" spans="1:22" s="25" customFormat="1" ht="45.2" customHeight="1">
-      <c r="A70" s="138"/>
-      <c r="B70" s="141"/>
-      <c r="C70" s="142"/>
-      <c r="D70" s="144"/>
-      <c r="E70" s="60" t="s">
-        <v>202</v>
-      </c>
-      <c r="F70" s="90" t="s">
-        <v>157</v>
-      </c>
-      <c r="G70" s="69"/>
-      <c r="H70" s="52">
+      <c r="A70" s="112"/>
+      <c r="B70" s="115"/>
+      <c r="C70" s="116"/>
+      <c r="D70" s="118"/>
+      <c r="E70" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="F70" s="86" t="s">
+        <v>155</v>
+      </c>
+      <c r="G70" s="66"/>
+      <c r="H70" s="51">
         <v>44032</v>
       </c>
       <c r="I70" s="27">
         <v>44057</v>
       </c>
-      <c r="J70" s="90">
+      <c r="J70" s="86">
         <f>I70-H70</f>
         <v>25</v>
       </c>
@@ -6315,20 +6289,20 @@
       </c>
     </row>
     <row r="71" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A71" s="140" t="s">
-        <v>159</v>
-      </c>
-      <c r="B71" s="140"/>
-      <c r="C71" s="140"/>
-      <c r="D71" s="140"/>
-      <c r="E71" s="140"/>
-      <c r="F71" s="140"/>
-      <c r="G71" s="140"/>
-      <c r="H71" s="140"/>
-      <c r="I71" s="140"/>
-      <c r="J71" s="140"/>
-      <c r="K71" s="140"/>
-      <c r="L71" s="57"/>
+      <c r="A71" s="114" t="s">
+        <v>157</v>
+      </c>
+      <c r="B71" s="114"/>
+      <c r="C71" s="114"/>
+      <c r="D71" s="114"/>
+      <c r="E71" s="114"/>
+      <c r="F71" s="114"/>
+      <c r="G71" s="114"/>
+      <c r="H71" s="114"/>
+      <c r="I71" s="114"/>
+      <c r="J71" s="114"/>
+      <c r="K71" s="114"/>
+      <c r="L71" s="56"/>
       <c r="M71" s="25"/>
       <c r="N71" s="25"/>
       <c r="O71" s="25"/>
@@ -6341,32 +6315,32 @@
       <c r="V71" s="25"/>
     </row>
     <row r="72" spans="1:22" ht="44.25" customHeight="1">
-      <c r="A72" s="59" t="s">
-        <v>160</v>
-      </c>
-      <c r="B72" s="91" t="s">
+      <c r="A72" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="B72" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="C72" s="91"/>
-      <c r="D72" s="91"/>
-      <c r="E72" s="91"/>
-      <c r="F72" s="91"/>
-      <c r="G72" s="91"/>
-      <c r="H72" s="55">
+      <c r="C72" s="87"/>
+      <c r="D72" s="87"/>
+      <c r="E72" s="87"/>
+      <c r="F72" s="87"/>
+      <c r="G72" s="87"/>
+      <c r="H72" s="54">
         <v>44043</v>
       </c>
       <c r="I72" s="27">
         <v>44057</v>
       </c>
-      <c r="J72" s="91">
+      <c r="J72" s="87">
         <f t="shared" ref="J72:J90" si="2">I72-H72</f>
         <v>14</v>
       </c>
-      <c r="K72" s="58" t="s">
-        <v>121</v>
+      <c r="K72" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L72" s="38">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M72" s="25"/>
       <c r="N72" s="25"/>
@@ -6381,7 +6355,7 @@
     </row>
     <row r="73" spans="1:22" ht="25.5" customHeight="1">
       <c r="A73" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B73" s="26" t="s">
         <v>29</v>
@@ -6401,11 +6375,11 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="K73" s="58" t="s">
-        <v>121</v>
+      <c r="K73" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L73" s="38">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M73" s="25"/>
       <c r="N73" s="25"/>
@@ -6420,7 +6394,7 @@
     </row>
     <row r="74" spans="1:22" ht="32.25" customHeight="1">
       <c r="A74" s="20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B74" s="26"/>
       <c r="C74" s="26"/>
@@ -6438,11 +6412,11 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="K74" s="28" t="s">
-        <v>139</v>
+      <c r="K74" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L74" s="39">
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="M74" s="25"/>
       <c r="N74" s="25"/>
@@ -6457,7 +6431,7 @@
     </row>
     <row r="75" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
       <c r="A75" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B75" s="26" t="s">
         <v>29</v>
@@ -6477,16 +6451,16 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K75" s="28" t="s">
-        <v>139</v>
+      <c r="K75" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L75" s="38">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:22" s="25" customFormat="1" ht="24.75" customHeight="1">
       <c r="A76" s="21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B76" s="26" t="s">
         <v>29</v>
@@ -6506,16 +6480,16 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K76" s="28" t="s">
-        <v>139</v>
+      <c r="K76" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L76" s="38">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:22" s="25" customFormat="1" ht="20.25" customHeight="1">
       <c r="A77" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B77" s="26" t="s">
         <v>29</v>
@@ -6535,16 +6509,16 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="K77" s="28" t="s">
-        <v>139</v>
+      <c r="K77" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L77" s="38">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:22" s="25" customFormat="1" ht="24.75" customHeight="1">
       <c r="A78" s="35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B78" s="26" t="s">
         <v>29</v>
@@ -6564,17 +6538,16 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="K78" s="28" t="s">
-        <v>139</v>
+      <c r="K78" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L78" s="40">
-        <f>AVERAGE(L79:L81)</f>
-        <v>1.6666666666666666E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:22" s="25" customFormat="1" ht="21.75" customHeight="1">
       <c r="A79" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B79" s="26" t="s">
         <v>29</v>
@@ -6594,16 +6567,16 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K79" s="28" t="s">
-        <v>139</v>
+      <c r="K79" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L79" s="38">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:22" s="25" customFormat="1" ht="18.75" customHeight="1">
       <c r="A80" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B80" s="26" t="s">
         <v>29</v>
@@ -6623,16 +6596,16 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="K80" s="28" t="s">
-        <v>139</v>
+      <c r="K80" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L80" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:22" s="25" customFormat="1" ht="21.75" customHeight="1">
       <c r="A81" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B81" s="26" t="s">
         <v>29</v>
@@ -6652,16 +6625,16 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="K81" s="28" t="s">
-        <v>139</v>
+      <c r="K81" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L81" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:22" ht="24" customHeight="1">
       <c r="A82" s="35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B82" s="26" t="s">
         <v>21</v>
@@ -6681,12 +6654,12 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="K82" s="28" t="s">
-        <v>139</v>
+      <c r="K82" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L82" s="40">
         <f>AVERAGE(L83:L84)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M82" s="25"/>
       <c r="N82" s="25"/>
@@ -6701,7 +6674,7 @@
     </row>
     <row r="83" spans="1:22" s="25" customFormat="1" ht="18.75" customHeight="1">
       <c r="A83" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B83" s="26" t="s">
         <v>21</v>
@@ -6721,16 +6694,16 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K83" s="28" t="s">
-        <v>139</v>
+      <c r="K83" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L83" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:22" s="25" customFormat="1" ht="20.25" customHeight="1">
       <c r="A84" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B84" s="26" t="s">
         <v>21</v>
@@ -6750,16 +6723,16 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K84" s="28" t="s">
-        <v>139</v>
+      <c r="K84" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L84" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:22" ht="22.5" customHeight="1">
       <c r="A85" s="35" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B85" s="26" t="s">
         <v>73</v>
@@ -6779,12 +6752,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K85" s="28" t="s">
-        <v>139</v>
+      <c r="K85" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L85" s="40">
         <f>AVERAGE(L86:L87)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M85" s="25"/>
       <c r="N85" s="25"/>
@@ -6799,7 +6772,7 @@
     </row>
     <row r="86" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
       <c r="A86" s="22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B86" s="26" t="s">
         <v>73</v>
@@ -6819,16 +6792,16 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K86" s="28" t="s">
-        <v>139</v>
+      <c r="K86" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L86" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
       <c r="A87" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B87" s="26" t="s">
         <v>73</v>
@@ -6848,16 +6821,16 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K87" s="28" t="s">
-        <v>139</v>
+      <c r="K87" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L87" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:22" ht="25.5" customHeight="1">
       <c r="A88" s="32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B88" s="26" t="s">
         <v>5</v>
@@ -6877,12 +6850,11 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="K88" s="28" t="s">
-        <v>139</v>
+      <c r="K88" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L88" s="39">
-        <f>AVERAGE(L89:L90)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M88" s="25"/>
       <c r="N88" s="25"/>
@@ -6897,7 +6869,7 @@
     </row>
     <row r="89" spans="1:22" s="25" customFormat="1" ht="25.5" customHeight="1">
       <c r="A89" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B89" s="26" t="s">
         <v>5</v>
@@ -6917,16 +6889,16 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="K89" s="28" t="s">
-        <v>139</v>
+      <c r="K89" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L89" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:22" ht="25.5" customHeight="1">
       <c r="A90" s="29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B90" s="26" t="s">
         <v>5</v>
@@ -6946,11 +6918,11 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K90" s="28" t="s">
-        <v>139</v>
+      <c r="K90" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="L90" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M90" s="25"/>
       <c r="N90" s="25"/>
@@ -6964,19 +6936,19 @@
       <c r="V90" s="25"/>
     </row>
     <row r="91" spans="1:22" ht="25.5" customHeight="1">
-      <c r="A91" s="139" t="s">
-        <v>179</v>
-      </c>
-      <c r="B91" s="139"/>
-      <c r="C91" s="139"/>
-      <c r="D91" s="139"/>
-      <c r="E91" s="139"/>
-      <c r="F91" s="139"/>
-      <c r="G91" s="139"/>
-      <c r="H91" s="139"/>
-      <c r="I91" s="139"/>
-      <c r="J91" s="139"/>
-      <c r="K91" s="139"/>
+      <c r="A91" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="B91" s="99"/>
+      <c r="C91" s="99"/>
+      <c r="D91" s="99"/>
+      <c r="E91" s="99"/>
+      <c r="F91" s="99"/>
+      <c r="G91" s="99"/>
+      <c r="H91" s="99"/>
+      <c r="I91" s="99"/>
+      <c r="J91" s="99"/>
+      <c r="K91" s="99"/>
       <c r="L91" s="38"/>
       <c r="M91" s="25"/>
       <c r="N91" s="25"/>
@@ -7071,7 +7043,7 @@
       <c r="K96" s="31"/>
       <c r="L96" s="31"/>
       <c r="N96" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="S96" s="31"/>
       <c r="T96" s="31"/>
@@ -7155,6 +7127,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A91:K91"/>
+    <mergeCell ref="A71:K71"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D59:D61"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
@@ -7171,68 +7205,6 @@
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="C31:C36"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A91:K91"/>
-    <mergeCell ref="A71:K71"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="D54:D58"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -7295,7 +7267,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -7305,27 +7277,27 @@
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="A3" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.15" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
@@ -7345,7 +7317,7 @@
     </row>
     <row r="5" spans="1:6" ht="43.15" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
@@ -7365,7 +7337,7 @@
     </row>
     <row r="6" spans="1:6" ht="43.15" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B6" s="8">
         <v>0.3</v>
@@ -7385,7 +7357,7 @@
     </row>
     <row r="7" spans="1:6" ht="43.15" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B7" s="8">
         <v>0.15</v>
@@ -7405,7 +7377,7 @@
     </row>
     <row r="8" spans="1:6" ht="43.15" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B8" s="8">
         <v>0.15</v>
@@ -7425,7 +7397,7 @@
     </row>
     <row r="9" spans="1:6" ht="43.15" customHeight="1">
       <c r="A9" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B9" s="8">
         <v>0.15</v>
@@ -7445,7 +7417,7 @@
     </row>
     <row r="10" spans="1:6" ht="43.15" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B10" s="8">
         <v>0.15</v>
@@ -7465,7 +7437,7 @@
     </row>
     <row r="11" spans="1:6" ht="43.15" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B11" s="8">
         <v>0.15</v>
@@ -7485,7 +7457,7 @@
     </row>
     <row r="12" spans="1:6" ht="43.15" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B12" s="8">
         <v>1</v>
@@ -7505,7 +7477,7 @@
     </row>
     <row r="13" spans="1:6" ht="43.15" customHeight="1">
       <c r="A13" s="16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="19">

</xml_diff>